<commit_message>
Uploaded 04-May-2021 15:59:15 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="97">
   <si>
     <t>RuleSet</t>
   </si>
@@ -881,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -961,7 +961,9 @@
       <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="G4" s="8"/>
       <c r="K4" s="3"/>
     </row>

</xml_diff>

<commit_message>
Uploaded 04-May-2021 16:02:22 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="97">
   <si>
     <t>RuleSet</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>factor</t>
-  </si>
-  <si>
-    <t>getValue().equals("$param")</t>
   </si>
   <si>
     <t>OPTICAL CARE</t>
@@ -186,9 +183,6 @@
     <t>100 Days</t>
   </si>
   <si>
-    <t>getBenefit_group().getCoveredDays().equals("$param")</t>
-  </si>
-  <si>
     <t>12 Hours</t>
   </si>
   <si>
@@ -270,9 +264,6 @@
     <t>7 Sessions per year</t>
   </si>
   <si>
-    <t>getName().equals("$param")</t>
-  </si>
-  <si>
     <t>Facials</t>
   </si>
   <si>
@@ -322,6 +313,15 @@
       </rPr>
       <t>AssumptionUsedByGroupName</t>
     </r>
+  </si>
+  <si>
+    <t>$benefit.getBenefit_group().getCoveredDays().equals("$param")</t>
+  </si>
+  <si>
+    <t>$benefit.getName().equals("$param")</t>
+  </si>
+  <si>
+    <t>$benefit.getValue().equals("$param")</t>
   </si>
 </sst>
 </file>
@@ -881,7 +881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -915,7 +915,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -955,15 +955,9 @@
       <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="K4" s="3"/>
     </row>
@@ -974,13 +968,13 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>8</v>
@@ -997,10 +991,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>10</v>
@@ -1015,12 +1009,12 @@
         <v>17</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
       <c r="F7" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="20">
         <v>0.5</v>
@@ -1032,12 +1026,12 @@
         <v>17</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="20">
         <v>0.6</v>
@@ -1049,12 +1043,12 @@
         <v>17</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="20">
         <v>0.65</v>
@@ -1066,12 +1060,12 @@
         <v>17</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
       <c r="F10" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" s="20">
         <v>0.7</v>
@@ -1083,12 +1077,12 @@
         <v>17</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="20">
         <v>0.72</v>
@@ -1100,12 +1094,12 @@
         <v>17</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
       <c r="F12" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="20">
         <v>0.75</v>
@@ -1117,12 +1111,12 @@
         <v>17</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="20">
         <v>0.86</v>
@@ -1134,12 +1128,12 @@
         <v>17</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
       <c r="F14" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" s="20">
         <v>0.89</v>
@@ -1151,12 +1145,12 @@
         <v>17</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" s="20">
         <v>0.89900000000000002</v>
@@ -1168,12 +1162,12 @@
         <v>17</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="20">
         <v>0.9</v>
@@ -1185,12 +1179,12 @@
         <v>17</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
       <c r="F17" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" s="20">
         <v>0.91</v>
@@ -1202,12 +1196,12 @@
         <v>17</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G18" s="20">
         <v>0.99099999999999999</v>
@@ -1219,12 +1213,12 @@
         <v>17</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
       <c r="F19" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G19" s="20">
         <v>0.995</v>
@@ -1236,12 +1230,12 @@
         <v>17</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="20">
         <v>0.996</v>
@@ -1253,12 +1247,12 @@
         <v>17</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
       <c r="F21" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="20">
         <v>0.997</v>
@@ -1270,12 +1264,12 @@
         <v>17</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
       <c r="F22" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22" s="20">
         <v>0.998</v>
@@ -1287,12 +1281,12 @@
         <v>17</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G23" s="20">
         <v>0.999</v>
@@ -1304,12 +1298,12 @@
         <v>17</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24" s="20">
         <v>1</v>
@@ -1321,12 +1315,12 @@
         <v>17</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G25" s="20">
         <v>0.4</v>
@@ -1338,12 +1332,12 @@
         <v>17</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
       <c r="F26" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G26" s="20">
         <v>0.5</v>
@@ -1355,12 +1349,12 @@
         <v>17</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
       <c r="F27" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G27" s="20">
         <v>0.55000000000000004</v>
@@ -1372,12 +1366,12 @@
         <v>17</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
       <c r="F28" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G28" s="20">
         <v>0.6</v>
@@ -1389,12 +1383,12 @@
         <v>17</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G29" s="20">
         <v>0.62</v>
@@ -1406,12 +1400,12 @@
         <v>17</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
       <c r="F30" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G30" s="20">
         <v>0.65</v>
@@ -1423,12 +1417,12 @@
         <v>17</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="21"/>
       <c r="F31" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G31" s="20">
         <v>0.7</v>
@@ -1440,12 +1434,12 @@
         <v>17</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
       <c r="F32" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G32" s="20">
         <v>0.88</v>
@@ -1457,12 +1451,12 @@
         <v>17</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
       <c r="F33" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G33" s="20">
         <v>0.9</v>
@@ -1474,12 +1468,12 @@
         <v>17</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
       <c r="F34" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G34" s="20">
         <v>0.995</v>
@@ -1491,12 +1485,12 @@
         <v>17</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="21"/>
       <c r="F35" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G35" s="20">
         <v>0.99550000000000005</v>
@@ -1508,12 +1502,12 @@
         <v>17</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="21"/>
       <c r="F36" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G36" s="20">
         <v>0.996</v>
@@ -1525,12 +1519,12 @@
         <v>17</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
       <c r="F37" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G37" s="20">
         <v>0.99650000000000005</v>
@@ -1542,12 +1536,12 @@
         <v>17</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="21"/>
       <c r="F38" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G38" s="20">
         <v>0.997</v>
@@ -1559,12 +1553,12 @@
         <v>17</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="21"/>
       <c r="F39" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G39" s="20">
         <v>0.99750000000000005</v>
@@ -1576,12 +1570,12 @@
         <v>17</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
       <c r="F40" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G40" s="20">
         <v>0.998</v>
@@ -1593,12 +1587,12 @@
         <v>17</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="21"/>
       <c r="F41" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G41" s="20">
         <v>0.999</v>
@@ -1610,12 +1604,12 @@
         <v>17</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="21"/>
       <c r="F42" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G42" s="20">
         <v>1</v>
@@ -1627,12 +1621,12 @@
         <v>17</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="21"/>
       <c r="F43" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G43" s="20">
         <v>0.1</v>
@@ -1644,12 +1638,12 @@
         <v>17</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="21"/>
       <c r="F44" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G44" s="20">
         <v>0.25</v>
@@ -1661,12 +1655,12 @@
         <v>17</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D45" s="21"/>
       <c r="E45" s="21"/>
       <c r="F45" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G45" s="20">
         <v>0.3</v>
@@ -1678,12 +1672,12 @@
         <v>17</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D46" s="21"/>
       <c r="E46" s="21"/>
       <c r="F46" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G46" s="20">
         <v>0.4</v>
@@ -1695,12 +1689,12 @@
         <v>17</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D47" s="21"/>
       <c r="E47" s="21"/>
       <c r="F47" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G47" s="20">
         <v>0.45</v>
@@ -1712,12 +1706,12 @@
         <v>17</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="21"/>
       <c r="F48" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G48" s="20">
         <v>0.5</v>
@@ -1729,12 +1723,12 @@
         <v>17</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D49" s="21"/>
       <c r="E49" s="21"/>
       <c r="F49" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G49" s="20">
         <v>0.61</v>
@@ -1746,12 +1740,12 @@
         <v>17</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21"/>
       <c r="F50" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G50" s="20">
         <v>0.65</v>
@@ -1763,12 +1757,12 @@
         <v>17</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D51" s="21"/>
       <c r="E51" s="21"/>
       <c r="F51" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G51" s="20">
         <v>0.7</v>
@@ -1780,12 +1774,12 @@
         <v>17</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D52" s="21"/>
       <c r="E52" s="21"/>
       <c r="F52" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G52" s="20">
         <v>0.8</v>
@@ -1797,12 +1791,12 @@
         <v>17</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="21"/>
       <c r="F53" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G53" s="20">
         <v>0.87</v>
@@ -1814,12 +1808,12 @@
         <v>17</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="21"/>
       <c r="F54" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G54" s="20">
         <v>0.88</v>
@@ -1831,12 +1825,12 @@
         <v>17</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="21"/>
       <c r="F55" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G55" s="20">
         <v>0.9</v>
@@ -1848,12 +1842,12 @@
         <v>17</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="21"/>
       <c r="F56" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G56" s="20">
         <v>0.996</v>
@@ -1865,12 +1859,12 @@
         <v>17</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="21"/>
       <c r="F57" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G57" s="20">
         <v>0.997</v>
@@ -1882,12 +1876,12 @@
         <v>17</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="21"/>
       <c r="F58" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G58" s="20">
         <v>0.998</v>
@@ -1899,12 +1893,12 @@
         <v>17</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="21"/>
       <c r="F59" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G59" s="20">
         <v>0.999</v>
@@ -1916,12 +1910,12 @@
         <v>17</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="21"/>
       <c r="F60" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G60" s="20">
         <v>1</v>
@@ -1933,12 +1927,12 @@
         <v>17</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G61" s="20">
         <v>0.48</v>
@@ -1950,12 +1944,12 @@
         <v>17</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="21"/>
       <c r="F62" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G62" s="20">
         <v>0.55000000000000004</v>
@@ -1967,12 +1961,12 @@
         <v>17</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D63" s="21"/>
       <c r="E63" s="21"/>
       <c r="F63" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G63" s="20">
         <v>0.65</v>
@@ -1984,12 +1978,12 @@
         <v>17</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="21"/>
       <c r="F64" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G64" s="20">
         <v>0.77</v>
@@ -2001,12 +1995,12 @@
         <v>17</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D65" s="21"/>
       <c r="E65" s="21"/>
       <c r="F65" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G65" s="20">
         <v>0.79</v>
@@ -2018,12 +2012,12 @@
         <v>17</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="21"/>
       <c r="F66" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G66" s="20">
         <v>0.8</v>
@@ -2035,12 +2029,12 @@
         <v>17</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="21"/>
       <c r="F67" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G67" s="20">
         <v>0.88</v>
@@ -2052,12 +2046,12 @@
         <v>17</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D68" s="21"/>
       <c r="E68" s="21"/>
       <c r="F68" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G68" s="20">
         <v>0.99</v>
@@ -2069,12 +2063,12 @@
         <v>17</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D69" s="21"/>
       <c r="E69" s="21"/>
       <c r="F69" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G69" s="20">
         <v>0.99099999999999999</v>
@@ -2086,12 +2080,12 @@
         <v>17</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="21"/>
       <c r="F70" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G70" s="20">
         <v>0.99199999999999999</v>
@@ -2103,12 +2097,12 @@
         <v>17</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D71" s="21"/>
       <c r="E71" s="21"/>
       <c r="F71" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G71" s="20">
         <v>0.99299999999999999</v>
@@ -2120,12 +2114,12 @@
         <v>17</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="21"/>
       <c r="F72" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G72" s="20">
         <v>0.99399999999999999</v>
@@ -2137,12 +2131,12 @@
         <v>17</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D73" s="21"/>
       <c r="E73" s="21"/>
       <c r="F73" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G73" s="20">
         <v>0.995</v>
@@ -2154,12 +2148,12 @@
         <v>17</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D74" s="21"/>
       <c r="E74" s="21"/>
       <c r="F74" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G74" s="20">
         <v>0.996</v>
@@ -2171,12 +2165,12 @@
         <v>17</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D75" s="21"/>
       <c r="E75" s="21"/>
       <c r="F75" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G75" s="20">
         <v>0.997</v>
@@ -2188,12 +2182,12 @@
         <v>17</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D76" s="21"/>
       <c r="E76" s="21"/>
       <c r="F76" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G76" s="20">
         <v>0.998</v>
@@ -2205,12 +2199,12 @@
         <v>17</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="21"/>
       <c r="F77" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G77" s="20">
         <v>0.999</v>
@@ -2222,12 +2216,12 @@
         <v>17</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="21"/>
       <c r="F78" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G78" s="20">
         <v>1</v>
@@ -2239,12 +2233,12 @@
         <v>17</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="21"/>
       <c r="F79" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G79" s="20">
         <v>0.79</v>
@@ -2256,12 +2250,12 @@
         <v>17</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="21"/>
       <c r="F80" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G80" s="20">
         <v>0.82</v>
@@ -2273,12 +2267,12 @@
         <v>17</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="21"/>
       <c r="F81" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G81" s="20">
         <v>0.85</v>
@@ -2290,12 +2284,12 @@
         <v>17</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
       <c r="F82" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G82" s="20">
         <v>0.9</v>
@@ -2307,12 +2301,12 @@
         <v>17</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
       <c r="F83" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G83" s="20">
         <v>0.98499999999999999</v>
@@ -2324,12 +2318,12 @@
         <v>17</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21"/>
       <c r="F84" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G84" s="20">
         <v>0.98799999999999999</v>
@@ -2341,12 +2335,12 @@
         <v>17</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
       <c r="F85" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G85" s="20">
         <v>0.98899999999999999</v>
@@ -2358,12 +2352,12 @@
         <v>17</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21"/>
       <c r="F86" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G86" s="20">
         <v>0.99</v>
@@ -2375,12 +2369,12 @@
         <v>17</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="21"/>
       <c r="F87" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G87" s="20">
         <v>0.99099999999999999</v>
@@ -2392,12 +2386,12 @@
         <v>17</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
       <c r="F88" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G88" s="20">
         <v>0.99199999999999999</v>
@@ -2409,12 +2403,12 @@
         <v>17</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21"/>
       <c r="F89" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G89" s="20">
         <v>0.99299999999999999</v>
@@ -2426,12 +2420,12 @@
         <v>17</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D90" s="21"/>
       <c r="E90" s="21"/>
       <c r="F90" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G90" s="20">
         <v>0.99399999999999999</v>
@@ -2443,12 +2437,12 @@
         <v>17</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
       <c r="F91" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G91" s="20">
         <v>0.995</v>
@@ -2460,12 +2454,12 @@
         <v>17</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
       <c r="F92" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G92" s="20">
         <v>0.996</v>
@@ -2477,12 +2471,12 @@
         <v>17</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
       <c r="F93" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G93" s="20">
         <v>0.997</v>
@@ -2494,12 +2488,12 @@
         <v>17</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
       <c r="F94" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G94" s="20">
         <v>0.998</v>
@@ -2511,12 +2505,12 @@
         <v>17</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D95" s="21"/>
       <c r="E95" s="21"/>
       <c r="F95" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G95" s="20">
         <v>0.999</v>
@@ -2528,12 +2522,12 @@
         <v>17</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
       <c r="F96" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G96" s="20">
         <v>1</v>
@@ -2545,10 +2539,10 @@
         <v>17</v>
       </c>
       <c r="C97" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D97" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="D97" s="19" t="s">
-        <v>37</v>
       </c>
       <c r="E97" s="19"/>
       <c r="F97" s="19"/>
@@ -2562,10 +2556,10 @@
         <v>17</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D98" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E98" s="19"/>
       <c r="F98" s="19"/>
@@ -2579,10 +2573,10 @@
         <v>17</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D99" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E99" s="19"/>
       <c r="F99" s="19"/>
@@ -2596,10 +2590,10 @@
         <v>17</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D100" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E100" s="19"/>
       <c r="F100" s="19"/>
@@ -2613,10 +2607,10 @@
         <v>17</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D101" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E101" s="19"/>
       <c r="F101" s="19"/>
@@ -2630,10 +2624,10 @@
         <v>17</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D102" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E102" s="19"/>
       <c r="F102" s="19"/>
@@ -2647,10 +2641,10 @@
         <v>17</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E103" s="19"/>
       <c r="F103" s="19"/>
@@ -2664,10 +2658,10 @@
         <v>17</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D104" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E104" s="19"/>
       <c r="F104" s="19"/>
@@ -2681,10 +2675,10 @@
         <v>17</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E105" s="19"/>
       <c r="F105" s="19"/>
@@ -2698,10 +2692,10 @@
         <v>17</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E106" s="19"/>
       <c r="F106" s="19"/>
@@ -2715,10 +2709,10 @@
         <v>17</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D107" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E107" s="19"/>
       <c r="F107" s="19"/>
@@ -2732,10 +2726,10 @@
         <v>17</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D108" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E108" s="19"/>
       <c r="F108" s="19"/>
@@ -2749,10 +2743,10 @@
         <v>17</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D109" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E109" s="19"/>
       <c r="F109" s="19"/>
@@ -2766,10 +2760,10 @@
         <v>17</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D110" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E110" s="19"/>
       <c r="F110" s="19"/>
@@ -2783,10 +2777,10 @@
         <v>17</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D111" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E111" s="19"/>
       <c r="F111" s="19"/>
@@ -2800,10 +2794,10 @@
         <v>17</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D112" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E112" s="19"/>
       <c r="F112" s="19"/>
@@ -2817,10 +2811,10 @@
         <v>17</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D113" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E113" s="19"/>
       <c r="F113" s="19"/>
@@ -2834,10 +2828,10 @@
         <v>17</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E114" s="19"/>
       <c r="F114" s="19"/>
@@ -2851,10 +2845,10 @@
         <v>17</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E115" s="19"/>
       <c r="F115" s="19"/>
@@ -2868,12 +2862,12 @@
         <v>17</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D116" s="15"/>
       <c r="E116" s="21"/>
       <c r="F116" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G116" s="20">
         <v>0.5</v>
@@ -2885,12 +2879,12 @@
         <v>17</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D117" s="15"/>
       <c r="E117" s="21"/>
       <c r="F117" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G117" s="20">
         <v>1</v>
@@ -2902,12 +2896,12 @@
         <v>17</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D118" s="15"/>
       <c r="E118" s="21"/>
       <c r="F118" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G118" s="20">
         <v>1.3</v>
@@ -2919,12 +2913,12 @@
         <v>17</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D119" s="15"/>
       <c r="E119" s="21"/>
       <c r="F119" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G119" s="20">
         <v>2</v>
@@ -2936,12 +2930,12 @@
         <v>17</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D120" s="15"/>
       <c r="E120" s="21"/>
       <c r="F120" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G120" s="20">
         <v>2.1</v>
@@ -2953,12 +2947,12 @@
         <v>17</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D121" s="15"/>
       <c r="E121" s="21"/>
       <c r="F121" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G121" s="20">
         <v>3</v>
@@ -2970,12 +2964,12 @@
         <v>17</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D122" s="15"/>
       <c r="E122" s="21"/>
       <c r="F122" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G122" s="20">
         <v>3</v>
@@ -2987,12 +2981,12 @@
         <v>17</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D123" s="15"/>
       <c r="E123" s="21"/>
       <c r="F123" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G123" s="20">
         <v>4</v>
@@ -3004,12 +2998,12 @@
         <v>17</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D124" s="15"/>
       <c r="E124" s="21"/>
       <c r="F124" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G124" s="20">
         <v>6</v>
@@ -3021,12 +3015,12 @@
         <v>17</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D125" s="15"/>
       <c r="E125" s="21"/>
       <c r="F125" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G125" s="20">
         <v>10</v>
@@ -3038,12 +3032,12 @@
         <v>17</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D126" s="15"/>
       <c r="E126" s="21"/>
       <c r="F126" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G126" s="20">
         <v>15</v>
@@ -3055,12 +3049,12 @@
         <v>17</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D127" s="15"/>
       <c r="E127" s="21"/>
       <c r="F127" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G127" s="20">
         <v>21</v>
@@ -3072,12 +3066,12 @@
         <v>17</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D128" s="15"/>
       <c r="E128" s="21"/>
       <c r="F128" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G128" s="20">
         <v>0.1</v>
@@ -3089,12 +3083,12 @@
         <v>17</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D129" s="15"/>
       <c r="E129" s="21"/>
       <c r="F129" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G129" s="20">
         <v>0.32</v>
@@ -3106,12 +3100,12 @@
         <v>17</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D130" s="15"/>
       <c r="E130" s="21"/>
       <c r="F130" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G130" s="20">
         <v>0.4</v>
@@ -3123,12 +3117,12 @@
         <v>17</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D131" s="15"/>
       <c r="E131" s="21"/>
       <c r="F131" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G131" s="20">
         <v>0.45</v>
@@ -3140,12 +3134,12 @@
         <v>17</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D132" s="15"/>
       <c r="E132" s="21"/>
       <c r="F132" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G132" s="20">
         <v>0.48</v>
@@ -3157,12 +3151,12 @@
         <v>17</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D133" s="15"/>
       <c r="E133" s="21"/>
       <c r="F133" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G133" s="20">
         <v>0.5</v>
@@ -3174,12 +3168,12 @@
         <v>17</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D134" s="15"/>
       <c r="E134" s="21"/>
       <c r="F134" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G134" s="20">
         <v>0.55000000000000004</v>
@@ -3191,12 +3185,12 @@
         <v>17</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D135" s="15"/>
       <c r="E135" s="21"/>
       <c r="F135" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G135" s="20">
         <v>0.6</v>
@@ -3208,12 +3202,12 @@
         <v>17</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="21"/>
       <c r="F136" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G136" s="20">
         <v>0.75</v>
@@ -3225,12 +3219,12 @@
         <v>17</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D137" s="15"/>
       <c r="E137" s="21"/>
       <c r="F137" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G137" s="20">
         <v>0.8</v>
@@ -3242,12 +3236,12 @@
         <v>17</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D138" s="15"/>
       <c r="E138" s="21"/>
       <c r="F138" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G138" s="20">
         <v>0.99</v>
@@ -3259,12 +3253,12 @@
         <v>17</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D139" s="15"/>
       <c r="E139" s="21"/>
       <c r="F139" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G139" s="20">
         <v>1</v>
@@ -3276,12 +3270,12 @@
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="21"/>
       <c r="F140" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G140" s="20">
         <v>0.5</v>
@@ -3293,12 +3287,12 @@
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="21"/>
       <c r="F141" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G141" s="20">
         <v>1</v>
@@ -3310,12 +3304,12 @@
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D142" s="15"/>
       <c r="E142" s="21"/>
       <c r="F142" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G142" s="20">
         <v>1.3</v>
@@ -3327,12 +3321,12 @@
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D143" s="15"/>
       <c r="E143" s="21"/>
       <c r="F143" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G143" s="20">
         <v>2</v>
@@ -3344,12 +3338,12 @@
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="21"/>
       <c r="F144" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G144" s="20">
         <v>2.1</v>
@@ -3361,12 +3355,12 @@
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D145" s="15"/>
       <c r="E145" s="21"/>
       <c r="F145" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G145" s="20">
         <v>3</v>
@@ -3378,12 +3372,12 @@
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="21"/>
       <c r="F146" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G146" s="20">
         <v>3</v>
@@ -3395,12 +3389,12 @@
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D147" s="15"/>
       <c r="E147" s="21"/>
       <c r="F147" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G147" s="20">
         <v>4</v>
@@ -3412,12 +3406,12 @@
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D148" s="15"/>
       <c r="E148" s="21"/>
       <c r="F148" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G148" s="20">
         <v>6</v>
@@ -3429,12 +3423,12 @@
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="21"/>
       <c r="F149" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G149" s="20">
         <v>10</v>
@@ -3446,12 +3440,12 @@
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D150" s="15"/>
       <c r="E150" s="21"/>
       <c r="F150" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G150" s="20">
         <v>15</v>
@@ -3463,12 +3457,12 @@
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D151" s="15"/>
       <c r="E151" s="21"/>
       <c r="F151" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G151" s="20">
         <v>21</v>
@@ -3480,12 +3474,12 @@
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="21"/>
       <c r="F152" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G152" s="20">
         <v>0.4</v>
@@ -3497,12 +3491,12 @@
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="21"/>
       <c r="F153" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G153" s="20">
         <v>0.8</v>
@@ -3514,12 +3508,12 @@
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="21"/>
       <c r="F154" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G154" s="20">
         <v>0.82</v>
@@ -3531,12 +3525,12 @@
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="21"/>
       <c r="F155" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G155" s="20">
         <v>0.85</v>
@@ -3548,12 +3542,12 @@
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="21"/>
       <c r="F156" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G156" s="20">
         <v>0.87</v>
@@ -3565,12 +3559,12 @@
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="21"/>
       <c r="F157" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G157" s="20">
         <v>0.88</v>
@@ -3582,12 +3576,12 @@
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="21"/>
       <c r="F158" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G158" s="20">
         <v>0.9</v>
@@ -3599,12 +3593,12 @@
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="21"/>
       <c r="F159" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G159" s="20">
         <v>0.91</v>
@@ -3616,12 +3610,12 @@
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="21"/>
       <c r="F160" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G160" s="20">
         <v>0.93</v>
@@ -3633,12 +3627,12 @@
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="21"/>
       <c r="F161" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G161" s="20">
         <v>0.95</v>
@@ -3650,12 +3644,12 @@
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="21"/>
       <c r="F162" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G162" s="20">
         <v>0.99</v>
@@ -3667,12 +3661,12 @@
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="21"/>
       <c r="F163" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G163" s="20">
         <v>1</v>
@@ -3684,12 +3678,12 @@
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D164" s="19"/>
       <c r="E164" s="19"/>
       <c r="F164" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G164" s="20">
         <v>0.4</v>
@@ -3701,12 +3695,12 @@
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D165" s="19"/>
       <c r="E165" s="19"/>
       <c r="F165" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G165" s="20">
         <v>0.55000000000000004</v>
@@ -3718,12 +3712,12 @@
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D166" s="19"/>
       <c r="E166" s="19"/>
       <c r="F166" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G166" s="20">
         <v>0.63</v>
@@ -3735,12 +3729,12 @@
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D167" s="19"/>
       <c r="E167" s="19"/>
       <c r="F167" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G167" s="20">
         <v>0.74</v>
@@ -3752,12 +3746,12 @@
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D168" s="19"/>
       <c r="E168" s="19"/>
       <c r="F168" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G168" s="20">
         <v>0.85</v>
@@ -3769,12 +3763,12 @@
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D169" s="19"/>
       <c r="E169" s="19"/>
       <c r="F169" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G169" s="20">
         <v>0.98</v>
@@ -3786,12 +3780,12 @@
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D170" s="19"/>
       <c r="E170" s="19"/>
       <c r="F170" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G170" s="20">
         <v>1</v>
@@ -3803,14 +3797,14 @@
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D171" s="15"/>
       <c r="E171" s="21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F171" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G171" s="20">
         <v>1</v>
@@ -3822,14 +3816,14 @@
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D172" s="15"/>
       <c r="E172" s="21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F172" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G172" s="20">
         <v>2</v>
@@ -3841,14 +3835,14 @@
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D173" s="15"/>
       <c r="E173" s="21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F173" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G173" s="20">
         <v>3</v>
@@ -3860,14 +3854,14 @@
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D174" s="15"/>
       <c r="E174" s="21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F174" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G174" s="20">
         <v>4</v>
@@ -3879,14 +3873,14 @@
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D175" s="15"/>
       <c r="E175" s="21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F175" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G175" s="20">
         <v>5</v>
@@ -3898,14 +3892,14 @@
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D176" s="15"/>
       <c r="E176" s="21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F176" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G176" s="20">
         <v>6</v>
@@ -3917,14 +3911,14 @@
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F177" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G177" s="20">
         <v>7</v>
@@ -3936,14 +3930,14 @@
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F178" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G178" s="20">
         <v>0.4</v>
@@ -3955,14 +3949,14 @@
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F179" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G179" s="20">
         <v>0.55000000000000004</v>
@@ -3974,14 +3968,14 @@
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F180" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G180" s="20">
         <v>0.63</v>
@@ -3993,14 +3987,14 @@
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F181" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G181" s="20">
         <v>0.74</v>
@@ -4012,14 +4006,14 @@
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F182" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G182" s="20">
         <v>0.85</v>
@@ -4031,14 +4025,14 @@
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F183" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G183" s="20">
         <v>0.98</v>
@@ -4050,14 +4044,14 @@
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D184" s="15"/>
       <c r="E184" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F184" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G184" s="20">
         <v>1</v>
@@ -4069,12 +4063,12 @@
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D185" s="22"/>
       <c r="E185" s="15"/>
       <c r="F185" s="22" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G185" s="23">
         <v>1</v>
@@ -4086,12 +4080,12 @@
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D186" s="22"/>
       <c r="E186" s="15"/>
       <c r="F186" s="22" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G186" s="23">
         <v>2</v>
@@ -4103,12 +4097,12 @@
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D187" s="22"/>
       <c r="E187" s="15"/>
       <c r="F187" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G187" s="23">
         <v>2.5</v>
@@ -4120,14 +4114,14 @@
         <v>17</v>
       </c>
       <c r="C188" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D188" s="15"/>
       <c r="E188" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F188" s="22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G188" s="23">
         <v>1</v>
@@ -4139,14 +4133,14 @@
         <v>17</v>
       </c>
       <c r="C189" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D189" s="15"/>
       <c r="E189" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F189" s="22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G189" s="23">
         <v>1.5</v>
@@ -4158,14 +4152,14 @@
         <v>17</v>
       </c>
       <c r="C190" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D190" s="15"/>
       <c r="E190" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F190" s="22" t="s">
         <v>90</v>
-      </c>
-      <c r="F190" s="22" t="s">
-        <v>93</v>
       </c>
       <c r="G190" s="23">
         <v>2</v>

</xml_diff>

<commit_message>
Uploaded 04-May-2021 16:15:27 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -186,6 +186,9 @@
     <t>100 Days</t>
   </si>
   <si>
+    <t>getBenefit_group().getCoveredDays().equals("$param")</t>
+  </si>
+  <si>
     <t>12 Hours</t>
   </si>
   <si>
@@ -319,9 +322,6 @@
       </rPr>
       <t>AssumptionUsedByGroupName</t>
     </r>
-  </si>
-  <si>
-    <t>$benefit.getBenefit_group().getCoveredDays().equals("$param")</t>
   </si>
   <si>
     <t>AssumptionUsedByGroupName1</t>
@@ -1433,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A192" sqref="A192"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1526,10 +1526,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>12</v>
@@ -1549,10 +1549,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>10</v>
@@ -3645,7 +3645,7 @@
       <c r="D116" s="15"/>
       <c r="E116" s="21"/>
       <c r="F116" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G116" s="20">
         <v>0.5</v>
@@ -3664,7 +3664,7 @@
       <c r="D117" s="15"/>
       <c r="E117" s="21"/>
       <c r="F117" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G117" s="20">
         <v>1</v>
@@ -3683,7 +3683,7 @@
       <c r="D118" s="15"/>
       <c r="E118" s="21"/>
       <c r="F118" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G118" s="20">
         <v>1.3</v>
@@ -3702,7 +3702,7 @@
       <c r="D119" s="15"/>
       <c r="E119" s="21"/>
       <c r="F119" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G119" s="20">
         <v>2</v>
@@ -3721,7 +3721,7 @@
       <c r="D120" s="15"/>
       <c r="E120" s="21"/>
       <c r="F120" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G120" s="20">
         <v>2.1</v>
@@ -3740,7 +3740,7 @@
       <c r="D121" s="15"/>
       <c r="E121" s="21"/>
       <c r="F121" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G121" s="20">
         <v>3</v>
@@ -3759,7 +3759,7 @@
       <c r="D122" s="15"/>
       <c r="E122" s="21"/>
       <c r="F122" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G122" s="20">
         <v>3</v>
@@ -3835,7 +3835,7 @@
       <c r="D126" s="15"/>
       <c r="E126" s="21"/>
       <c r="F126" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G126" s="20">
         <v>15</v>
@@ -3868,12 +3868,12 @@
         <v>17</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D128" s="15"/>
       <c r="E128" s="21"/>
       <c r="F128" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G128" s="20">
         <v>0.1</v>
@@ -3887,12 +3887,12 @@
         <v>17</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D129" s="15"/>
       <c r="E129" s="21"/>
       <c r="F129" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G129" s="20">
         <v>0.32</v>
@@ -3906,12 +3906,12 @@
         <v>17</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D130" s="15"/>
       <c r="E130" s="21"/>
       <c r="F130" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G130" s="20">
         <v>0.4</v>
@@ -3925,12 +3925,12 @@
         <v>17</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D131" s="15"/>
       <c r="E131" s="21"/>
       <c r="F131" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G131" s="20">
         <v>0.45</v>
@@ -3944,12 +3944,12 @@
         <v>17</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D132" s="15"/>
       <c r="E132" s="21"/>
       <c r="F132" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G132" s="20">
         <v>0.48</v>
@@ -3963,12 +3963,12 @@
         <v>17</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D133" s="15"/>
       <c r="E133" s="21"/>
       <c r="F133" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G133" s="20">
         <v>0.5</v>
@@ -3982,12 +3982,12 @@
         <v>17</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D134" s="15"/>
       <c r="E134" s="21"/>
       <c r="F134" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G134" s="20">
         <v>0.55000000000000004</v>
@@ -4001,7 +4001,7 @@
         <v>17</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D135" s="15"/>
       <c r="E135" s="21"/>
@@ -4020,7 +4020,7 @@
         <v>17</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="21"/>
@@ -4039,7 +4039,7 @@
         <v>17</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D137" s="15"/>
       <c r="E137" s="21"/>
@@ -4058,12 +4058,12 @@
         <v>17</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D138" s="15"/>
       <c r="E138" s="21"/>
       <c r="F138" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G138" s="20">
         <v>0.99</v>
@@ -4077,7 +4077,7 @@
         <v>17</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D139" s="15"/>
       <c r="E139" s="21"/>
@@ -4096,12 +4096,12 @@
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="21"/>
       <c r="F140" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G140" s="20">
         <v>0.5</v>
@@ -4115,12 +4115,12 @@
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="21"/>
       <c r="F141" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G141" s="20">
         <v>1</v>
@@ -4134,12 +4134,12 @@
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D142" s="15"/>
       <c r="E142" s="21"/>
       <c r="F142" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G142" s="20">
         <v>1.3</v>
@@ -4153,12 +4153,12 @@
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D143" s="15"/>
       <c r="E143" s="21"/>
       <c r="F143" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G143" s="20">
         <v>2</v>
@@ -4172,12 +4172,12 @@
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="21"/>
       <c r="F144" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G144" s="20">
         <v>2.1</v>
@@ -4191,12 +4191,12 @@
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D145" s="15"/>
       <c r="E145" s="21"/>
       <c r="F145" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G145" s="20">
         <v>3</v>
@@ -4210,12 +4210,12 @@
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="21"/>
       <c r="F146" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G146" s="20">
         <v>3</v>
@@ -4229,7 +4229,7 @@
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D147" s="15"/>
       <c r="E147" s="21"/>
@@ -4248,7 +4248,7 @@
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D148" s="15"/>
       <c r="E148" s="21"/>
@@ -4267,7 +4267,7 @@
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="21"/>
@@ -4286,12 +4286,12 @@
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D150" s="15"/>
       <c r="E150" s="21"/>
       <c r="F150" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G150" s="20">
         <v>15</v>
@@ -4305,7 +4305,7 @@
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D151" s="15"/>
       <c r="E151" s="21"/>
@@ -4324,12 +4324,12 @@
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="21"/>
       <c r="F152" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G152" s="20">
         <v>0.4</v>
@@ -4343,12 +4343,12 @@
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="21"/>
       <c r="F153" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G153" s="20">
         <v>0.8</v>
@@ -4362,12 +4362,12 @@
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="21"/>
       <c r="F154" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G154" s="20">
         <v>0.82</v>
@@ -4381,12 +4381,12 @@
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="21"/>
       <c r="F155" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G155" s="20">
         <v>0.85</v>
@@ -4400,12 +4400,12 @@
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="21"/>
       <c r="F156" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G156" s="20">
         <v>0.87</v>
@@ -4419,12 +4419,12 @@
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="21"/>
       <c r="F157" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G157" s="20">
         <v>0.88</v>
@@ -4438,12 +4438,12 @@
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="21"/>
       <c r="F158" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G158" s="20">
         <v>0.9</v>
@@ -4457,7 +4457,7 @@
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="21"/>
@@ -4476,7 +4476,7 @@
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="21"/>
@@ -4495,7 +4495,7 @@
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="21"/>
@@ -4514,12 +4514,12 @@
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="21"/>
       <c r="F162" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G162" s="20">
         <v>0.99</v>
@@ -4533,7 +4533,7 @@
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="21"/>
@@ -4552,12 +4552,12 @@
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D164" s="19"/>
       <c r="E164" s="19"/>
       <c r="F164" s="19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G164" s="20">
         <v>0.4</v>
@@ -4571,12 +4571,12 @@
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D165" s="19"/>
       <c r="E165" s="19"/>
       <c r="F165" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G165" s="20">
         <v>0.55000000000000004</v>
@@ -4590,12 +4590,12 @@
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D166" s="19"/>
       <c r="E166" s="19"/>
       <c r="F166" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G166" s="20">
         <v>0.63</v>
@@ -4609,12 +4609,12 @@
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D167" s="19"/>
       <c r="E167" s="19"/>
       <c r="F167" s="19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G167" s="20">
         <v>0.74</v>
@@ -4628,12 +4628,12 @@
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D168" s="19"/>
       <c r="E168" s="19"/>
       <c r="F168" s="19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G168" s="20">
         <v>0.85</v>
@@ -4647,12 +4647,12 @@
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D169" s="19"/>
       <c r="E169" s="19"/>
       <c r="F169" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G169" s="20">
         <v>0.98</v>
@@ -4666,12 +4666,12 @@
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D170" s="19"/>
       <c r="E170" s="19"/>
       <c r="F170" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G170" s="20">
         <v>1</v>
@@ -4685,14 +4685,14 @@
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D171" s="15"/>
       <c r="E171" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F171" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G171" s="20">
         <v>1</v>
@@ -4706,14 +4706,14 @@
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D172" s="15"/>
       <c r="E172" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F172" s="19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G172" s="20">
         <v>2</v>
@@ -4727,14 +4727,14 @@
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D173" s="15"/>
       <c r="E173" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F173" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G173" s="20">
         <v>3</v>
@@ -4748,14 +4748,14 @@
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D174" s="15"/>
       <c r="E174" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F174" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G174" s="20">
         <v>4</v>
@@ -4769,14 +4769,14 @@
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D175" s="15"/>
       <c r="E175" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F175" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G175" s="20">
         <v>5</v>
@@ -4790,14 +4790,14 @@
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D176" s="15"/>
       <c r="E176" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F176" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G176" s="20">
         <v>6</v>
@@ -4811,14 +4811,14 @@
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F177" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G177" s="20">
         <v>7</v>
@@ -4832,14 +4832,14 @@
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F178" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G178" s="20">
         <v>0.4</v>
@@ -4853,14 +4853,14 @@
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F179" s="19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G179" s="20">
         <v>0.55000000000000004</v>
@@ -4874,14 +4874,14 @@
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F180" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G180" s="20">
         <v>0.63</v>
@@ -4895,14 +4895,14 @@
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F181" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G181" s="20">
         <v>0.74</v>
@@ -4916,14 +4916,14 @@
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F182" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G182" s="20">
         <v>0.85</v>
@@ -4937,14 +4937,14 @@
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F183" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G183" s="20">
         <v>0.98</v>
@@ -4958,14 +4958,14 @@
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D184" s="15"/>
       <c r="E184" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F184" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G184" s="20">
         <v>1</v>
@@ -4979,12 +4979,12 @@
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D185" s="22"/>
       <c r="E185" s="15"/>
       <c r="F185" s="22" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G185" s="23">
         <v>1</v>
@@ -4998,12 +4998,12 @@
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D186" s="22"/>
       <c r="E186" s="15"/>
       <c r="F186" s="22" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G186" s="23">
         <v>2</v>
@@ -5017,12 +5017,12 @@
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D187" s="22"/>
       <c r="E187" s="15"/>
       <c r="F187" s="22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G187" s="23">
         <v>2.5</v>
@@ -5040,10 +5040,10 @@
       </c>
       <c r="D188" s="15"/>
       <c r="E188" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F188" s="22" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G188" s="23">
         <v>1</v>
@@ -5061,10 +5061,10 @@
       </c>
       <c r="D189" s="15"/>
       <c r="E189" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F189" s="22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G189" s="23">
         <v>1.5</v>
@@ -5082,10 +5082,10 @@
       </c>
       <c r="D190" s="15"/>
       <c r="E190" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F190" s="22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G190" s="23">
         <v>2</v>

</xml_diff>

<commit_message>
Uploaded 04-May-2021 16:21:19 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="266">
   <si>
     <t>RuleSet</t>
   </si>
@@ -132,58 +132,13 @@
     <t>ADMISSIONS AND ACCOMMODATION</t>
   </si>
   <si>
-    <t>1 Day</t>
-  </si>
-  <si>
-    <t>2 Days</t>
-  </si>
-  <si>
-    <t>3 Days</t>
-  </si>
-  <si>
-    <t>4 Days</t>
-  </si>
-  <si>
     <t>5 Days</t>
   </si>
   <si>
-    <t>6 Days</t>
-  </si>
-  <si>
     <t>7 Days</t>
   </si>
   <si>
-    <t>8 Days</t>
-  </si>
-  <si>
-    <t>9 Days</t>
-  </si>
-  <si>
     <t>10 Days</t>
-  </si>
-  <si>
-    <t>15 Days</t>
-  </si>
-  <si>
-    <t>20 Days</t>
-  </si>
-  <si>
-    <t>25 Days</t>
-  </si>
-  <si>
-    <t>30 Days</t>
-  </si>
-  <si>
-    <t>45 Days</t>
-  </si>
-  <si>
-    <t>50 Days</t>
-  </si>
-  <si>
-    <t>60 Days</t>
-  </si>
-  <si>
-    <t>100 Days</t>
   </si>
   <si>
     <t>getBenefit_group().getCoveredDays().equals("$param")</t>
@@ -1433,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B103" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1467,7 +1422,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1526,10 +1481,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>12</v>
@@ -1549,10 +1504,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>10</v>
@@ -1563,7 +1518,7 @@
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B7" s="15">
         <v>17</v>
@@ -1582,7 +1537,7 @@
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B8" s="15">
         <v>17</v>
@@ -1601,7 +1556,7 @@
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B9" s="15">
         <v>17</v>
@@ -1620,7 +1575,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B10" s="15">
         <v>17</v>
@@ -1639,7 +1594,7 @@
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B11" s="15">
         <v>17</v>
@@ -1658,7 +1613,7 @@
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B12" s="15">
         <v>17</v>
@@ -1677,7 +1632,7 @@
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B13" s="15">
         <v>17</v>
@@ -1696,7 +1651,7 @@
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B14" s="15">
         <v>17</v>
@@ -1715,7 +1670,7 @@
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B15" s="15">
         <v>17</v>
@@ -1734,7 +1689,7 @@
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B16" s="15">
         <v>17</v>
@@ -1753,7 +1708,7 @@
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B17" s="15">
         <v>17</v>
@@ -1772,7 +1727,7 @@
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B18" s="15">
         <v>17</v>
@@ -1791,7 +1746,7 @@
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B19" s="15">
         <v>17</v>
@@ -1810,7 +1765,7 @@
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B20" s="15">
         <v>17</v>
@@ -1829,7 +1784,7 @@
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B21" s="15">
         <v>17</v>
@@ -1848,7 +1803,7 @@
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B22" s="15">
         <v>17</v>
@@ -1867,7 +1822,7 @@
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B23" s="15">
         <v>17</v>
@@ -1886,7 +1841,7 @@
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="B24" s="15">
         <v>17</v>
@@ -1905,7 +1860,7 @@
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B25" s="15">
         <v>17</v>
@@ -1924,7 +1879,7 @@
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B26" s="15">
         <v>17</v>
@@ -1943,7 +1898,7 @@
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B27" s="15">
         <v>17</v>
@@ -1962,7 +1917,7 @@
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="B28" s="15">
         <v>17</v>
@@ -1981,7 +1936,7 @@
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B29" s="15">
         <v>17</v>
@@ -2000,7 +1955,7 @@
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B30" s="15">
         <v>17</v>
@@ -2019,7 +1974,7 @@
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B31" s="15">
         <v>17</v>
@@ -2038,7 +1993,7 @@
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B32" s="15">
         <v>17</v>
@@ -2057,7 +2012,7 @@
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B33" s="15">
         <v>17</v>
@@ -2076,7 +2031,7 @@
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B34" s="15">
         <v>17</v>
@@ -2095,7 +2050,7 @@
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B35" s="15">
         <v>17</v>
@@ -2114,7 +2069,7 @@
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B36" s="15">
         <v>17</v>
@@ -2133,7 +2088,7 @@
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="B37" s="15">
         <v>17</v>
@@ -2152,7 +2107,7 @@
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B38" s="15">
         <v>17</v>
@@ -2171,7 +2126,7 @@
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B39" s="15">
         <v>17</v>
@@ -2190,7 +2145,7 @@
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B40" s="15">
         <v>17</v>
@@ -2209,7 +2164,7 @@
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="B41" s="15">
         <v>17</v>
@@ -2228,7 +2183,7 @@
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="B42" s="15">
         <v>17</v>
@@ -2247,7 +2202,7 @@
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B43" s="15">
         <v>17</v>
@@ -2266,7 +2221,7 @@
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B44" s="15">
         <v>17</v>
@@ -2285,7 +2240,7 @@
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B45" s="15">
         <v>17</v>
@@ -2304,7 +2259,7 @@
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B46" s="15">
         <v>17</v>
@@ -2323,7 +2278,7 @@
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B47" s="15">
         <v>17</v>
@@ -2342,7 +2297,7 @@
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="B48" s="15">
         <v>17</v>
@@ -2361,7 +2316,7 @@
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="B49" s="15">
         <v>17</v>
@@ -2380,7 +2335,7 @@
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B50" s="15">
         <v>17</v>
@@ -2399,7 +2354,7 @@
     </row>
     <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B51" s="15">
         <v>17</v>
@@ -2418,7 +2373,7 @@
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B52" s="15">
         <v>17</v>
@@ -2437,7 +2392,7 @@
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="B53" s="15">
         <v>17</v>
@@ -2456,7 +2411,7 @@
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B54" s="15">
         <v>17</v>
@@ -2475,7 +2430,7 @@
     </row>
     <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B55" s="15">
         <v>17</v>
@@ -2494,7 +2449,7 @@
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B56" s="15">
         <v>17</v>
@@ -2513,7 +2468,7 @@
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B57" s="15">
         <v>17</v>
@@ -2532,7 +2487,7 @@
     </row>
     <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B58" s="15">
         <v>17</v>
@@ -2551,7 +2506,7 @@
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B59" s="15">
         <v>17</v>
@@ -2570,7 +2525,7 @@
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B60" s="15">
         <v>17</v>
@@ -2589,7 +2544,7 @@
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B61" s="15">
         <v>17</v>
@@ -2608,7 +2563,7 @@
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B62" s="15">
         <v>17</v>
@@ -2627,7 +2582,7 @@
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B63" s="15">
         <v>17</v>
@@ -2646,7 +2601,7 @@
     </row>
     <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B64" s="15">
         <v>17</v>
@@ -2665,7 +2620,7 @@
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B65" s="15">
         <v>17</v>
@@ -2684,7 +2639,7 @@
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B66" s="15">
         <v>17</v>
@@ -2703,7 +2658,7 @@
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="B67" s="15">
         <v>17</v>
@@ -2722,7 +2677,7 @@
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B68" s="15">
         <v>17</v>
@@ -2741,7 +2696,7 @@
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B69" s="15">
         <v>17</v>
@@ -2760,7 +2715,7 @@
     </row>
     <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="B70" s="15">
         <v>17</v>
@@ -2779,7 +2734,7 @@
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="B71" s="15">
         <v>17</v>
@@ -2798,7 +2753,7 @@
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B72" s="15">
         <v>17</v>
@@ -2817,7 +2772,7 @@
     </row>
     <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="B73" s="15">
         <v>17</v>
@@ -2836,7 +2791,7 @@
     </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="B74" s="15">
         <v>17</v>
@@ -2855,7 +2810,7 @@
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B75" s="15">
         <v>17</v>
@@ -2874,7 +2829,7 @@
     </row>
     <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B76" s="15">
         <v>17</v>
@@ -2893,7 +2848,7 @@
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B77" s="15">
         <v>17</v>
@@ -2912,7 +2867,7 @@
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="B78" s="15">
         <v>17</v>
@@ -2931,7 +2886,7 @@
     </row>
     <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="B79" s="15">
         <v>17</v>
@@ -2950,7 +2905,7 @@
     </row>
     <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="B80" s="15">
         <v>17</v>
@@ -2969,7 +2924,7 @@
     </row>
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B81" s="15">
         <v>17</v>
@@ -2988,7 +2943,7 @@
     </row>
     <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B82" s="15">
         <v>17</v>
@@ -3007,7 +2962,7 @@
     </row>
     <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="B83" s="15">
         <v>17</v>
@@ -3026,7 +2981,7 @@
     </row>
     <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B84" s="15">
         <v>17</v>
@@ -3045,7 +3000,7 @@
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B85" s="15">
         <v>17</v>
@@ -3064,7 +3019,7 @@
     </row>
     <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="B86" s="15">
         <v>17</v>
@@ -3083,7 +3038,7 @@
     </row>
     <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B87" s="15">
         <v>17</v>
@@ -3102,7 +3057,7 @@
     </row>
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="B88" s="15">
         <v>17</v>
@@ -3121,7 +3076,7 @@
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="B89" s="15">
         <v>17</v>
@@ -3140,7 +3095,7 @@
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="B90" s="15">
         <v>17</v>
@@ -3159,7 +3114,7 @@
     </row>
     <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B91" s="15">
         <v>17</v>
@@ -3178,7 +3133,7 @@
     </row>
     <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B92" s="15">
         <v>17</v>
@@ -3197,7 +3152,7 @@
     </row>
     <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B93" s="15">
         <v>17</v>
@@ -3216,7 +3171,7 @@
     </row>
     <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B94" s="15">
         <v>17</v>
@@ -3235,7 +3190,7 @@
     </row>
     <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B95" s="15">
         <v>17</v>
@@ -3254,7 +3209,7 @@
     </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="B96" s="15">
         <v>17</v>
@@ -3273,7 +3228,7 @@
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="B97" s="15">
         <v>17</v>
@@ -3281,8 +3236,8 @@
       <c r="C97" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D97" s="19" t="s">
-        <v>37</v>
+      <c r="D97" s="19">
+        <v>1</v>
       </c>
       <c r="E97" s="19"/>
       <c r="F97" s="19"/>
@@ -3292,7 +3247,7 @@
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="B98" s="15">
         <v>17</v>
@@ -3300,8 +3255,8 @@
       <c r="C98" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D98" s="19" t="s">
-        <v>38</v>
+      <c r="D98" s="19">
+        <v>2</v>
       </c>
       <c r="E98" s="19"/>
       <c r="F98" s="19"/>
@@ -3311,7 +3266,7 @@
     </row>
     <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="B99" s="15">
         <v>17</v>
@@ -3319,8 +3274,8 @@
       <c r="C99" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D99" s="19" t="s">
-        <v>39</v>
+      <c r="D99" s="19">
+        <v>3</v>
       </c>
       <c r="E99" s="19"/>
       <c r="F99" s="19"/>
@@ -3330,7 +3285,7 @@
     </row>
     <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="B100" s="15">
         <v>17</v>
@@ -3338,8 +3293,8 @@
       <c r="C100" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D100" s="19" t="s">
-        <v>40</v>
+      <c r="D100" s="19">
+        <v>4</v>
       </c>
       <c r="E100" s="19"/>
       <c r="F100" s="19"/>
@@ -3349,7 +3304,7 @@
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="B101" s="15">
         <v>17</v>
@@ -3357,8 +3312,8 @@
       <c r="C101" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D101" s="19" t="s">
-        <v>41</v>
+      <c r="D101" s="19">
+        <v>5</v>
       </c>
       <c r="E101" s="19"/>
       <c r="F101" s="19"/>
@@ -3368,7 +3323,7 @@
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B102" s="15">
         <v>17</v>
@@ -3376,8 +3331,8 @@
       <c r="C102" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D102" s="19" t="s">
-        <v>42</v>
+      <c r="D102" s="19">
+        <v>6</v>
       </c>
       <c r="E102" s="19"/>
       <c r="F102" s="19"/>
@@ -3387,7 +3342,7 @@
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="B103" s="15">
         <v>17</v>
@@ -3395,8 +3350,8 @@
       <c r="C103" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D103" s="19" t="s">
-        <v>43</v>
+      <c r="D103" s="19">
+        <v>7</v>
       </c>
       <c r="E103" s="19"/>
       <c r="F103" s="19"/>
@@ -3406,7 +3361,7 @@
     </row>
     <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="B104" s="15">
         <v>17</v>
@@ -3414,8 +3369,8 @@
       <c r="C104" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D104" s="19" t="s">
-        <v>44</v>
+      <c r="D104" s="19">
+        <v>8</v>
       </c>
       <c r="E104" s="19"/>
       <c r="F104" s="19"/>
@@ -3425,7 +3380,7 @@
     </row>
     <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="B105" s="15">
         <v>17</v>
@@ -3433,8 +3388,8 @@
       <c r="C105" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D105" s="19" t="s">
-        <v>45</v>
+      <c r="D105" s="19">
+        <v>9</v>
       </c>
       <c r="E105" s="19"/>
       <c r="F105" s="19"/>
@@ -3444,7 +3399,7 @@
     </row>
     <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="B106" s="15">
         <v>17</v>
@@ -3452,8 +3407,8 @@
       <c r="C106" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D106" s="19" t="s">
-        <v>46</v>
+      <c r="D106" s="19">
+        <v>10</v>
       </c>
       <c r="E106" s="19"/>
       <c r="F106" s="19"/>
@@ -3463,7 +3418,7 @@
     </row>
     <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B107" s="15">
         <v>17</v>
@@ -3471,8 +3426,8 @@
       <c r="C107" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D107" s="19" t="s">
-        <v>47</v>
+      <c r="D107" s="19">
+        <v>15</v>
       </c>
       <c r="E107" s="19"/>
       <c r="F107" s="19"/>
@@ -3482,7 +3437,7 @@
     </row>
     <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B108" s="15">
         <v>17</v>
@@ -3490,8 +3445,8 @@
       <c r="C108" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D108" s="19" t="s">
-        <v>48</v>
+      <c r="D108" s="19">
+        <v>20</v>
       </c>
       <c r="E108" s="19"/>
       <c r="F108" s="19"/>
@@ -3501,7 +3456,7 @@
     </row>
     <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B109" s="15">
         <v>17</v>
@@ -3509,8 +3464,8 @@
       <c r="C109" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D109" s="19" t="s">
-        <v>49</v>
+      <c r="D109" s="19">
+        <v>25</v>
       </c>
       <c r="E109" s="19"/>
       <c r="F109" s="19"/>
@@ -3520,7 +3475,7 @@
     </row>
     <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B110" s="15">
         <v>17</v>
@@ -3528,8 +3483,8 @@
       <c r="C110" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D110" s="19" t="s">
-        <v>50</v>
+      <c r="D110" s="19">
+        <v>30</v>
       </c>
       <c r="E110" s="19"/>
       <c r="F110" s="19"/>
@@ -3539,7 +3494,7 @@
     </row>
     <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="B111" s="15">
         <v>17</v>
@@ -3547,8 +3502,8 @@
       <c r="C111" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D111" s="19" t="s">
-        <v>51</v>
+      <c r="D111" s="19">
+        <v>45</v>
       </c>
       <c r="E111" s="19"/>
       <c r="F111" s="19"/>
@@ -3558,7 +3513,7 @@
     </row>
     <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="B112" s="15">
         <v>17</v>
@@ -3566,8 +3521,8 @@
       <c r="C112" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D112" s="19" t="s">
-        <v>52</v>
+      <c r="D112" s="19">
+        <v>50</v>
       </c>
       <c r="E112" s="19"/>
       <c r="F112" s="19"/>
@@ -3577,7 +3532,7 @@
     </row>
     <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B113" s="15">
         <v>17</v>
@@ -3585,8 +3540,8 @@
       <c r="C113" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D113" s="19" t="s">
-        <v>53</v>
+      <c r="D113" s="19">
+        <v>60</v>
       </c>
       <c r="E113" s="19"/>
       <c r="F113" s="19"/>
@@ -3596,7 +3551,7 @@
     </row>
     <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B114" s="15">
         <v>17</v>
@@ -3604,8 +3559,8 @@
       <c r="C114" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D114" s="19" t="s">
-        <v>54</v>
+      <c r="D114" s="19">
+        <v>100</v>
       </c>
       <c r="E114" s="19"/>
       <c r="F114" s="19"/>
@@ -3615,7 +3570,7 @@
     </row>
     <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="B115" s="15">
         <v>17</v>
@@ -3623,8 +3578,8 @@
       <c r="C115" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D115" s="19" t="s">
-        <v>31</v>
+      <c r="D115" s="19">
+        <v>-1</v>
       </c>
       <c r="E115" s="19"/>
       <c r="F115" s="19"/>
@@ -3634,7 +3589,7 @@
     </row>
     <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B116" s="15">
         <v>17</v>
@@ -3645,7 +3600,7 @@
       <c r="D116" s="15"/>
       <c r="E116" s="21"/>
       <c r="F116" s="19" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="G116" s="20">
         <v>0.5</v>
@@ -3653,7 +3608,7 @@
     </row>
     <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="B117" s="15">
         <v>17</v>
@@ -3664,7 +3619,7 @@
       <c r="D117" s="15"/>
       <c r="E117" s="21"/>
       <c r="F117" s="19" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G117" s="20">
         <v>1</v>
@@ -3672,7 +3627,7 @@
     </row>
     <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="B118" s="15">
         <v>17</v>
@@ -3683,7 +3638,7 @@
       <c r="D118" s="15"/>
       <c r="E118" s="21"/>
       <c r="F118" s="19" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G118" s="20">
         <v>1.3</v>
@@ -3691,7 +3646,7 @@
     </row>
     <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="B119" s="15">
         <v>17</v>
@@ -3702,7 +3657,7 @@
       <c r="D119" s="15"/>
       <c r="E119" s="21"/>
       <c r="F119" s="19" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="G119" s="20">
         <v>2</v>
@@ -3710,7 +3665,7 @@
     </row>
     <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="B120" s="15">
         <v>17</v>
@@ -3721,7 +3676,7 @@
       <c r="D120" s="15"/>
       <c r="E120" s="21"/>
       <c r="F120" s="19" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G120" s="20">
         <v>2.1</v>
@@ -3729,7 +3684,7 @@
     </row>
     <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="B121" s="15">
         <v>17</v>
@@ -3740,7 +3695,7 @@
       <c r="D121" s="15"/>
       <c r="E121" s="21"/>
       <c r="F121" s="19" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G121" s="20">
         <v>3</v>
@@ -3748,7 +3703,7 @@
     </row>
     <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B122" s="15">
         <v>17</v>
@@ -3759,7 +3714,7 @@
       <c r="D122" s="15"/>
       <c r="E122" s="21"/>
       <c r="F122" s="19" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G122" s="20">
         <v>3</v>
@@ -3767,7 +3722,7 @@
     </row>
     <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="B123" s="15">
         <v>17</v>
@@ -3778,7 +3733,7 @@
       <c r="D123" s="15"/>
       <c r="E123" s="21"/>
       <c r="F123" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G123" s="20">
         <v>4</v>
@@ -3786,7 +3741,7 @@
     </row>
     <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="B124" s="15">
         <v>17</v>
@@ -3797,7 +3752,7 @@
       <c r="D124" s="15"/>
       <c r="E124" s="21"/>
       <c r="F124" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G124" s="20">
         <v>6</v>
@@ -3805,7 +3760,7 @@
     </row>
     <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="B125" s="15">
         <v>17</v>
@@ -3816,7 +3771,7 @@
       <c r="D125" s="15"/>
       <c r="E125" s="21"/>
       <c r="F125" s="19" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G125" s="20">
         <v>10</v>
@@ -3824,7 +3779,7 @@
     </row>
     <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="B126" s="15">
         <v>17</v>
@@ -3835,7 +3790,7 @@
       <c r="D126" s="15"/>
       <c r="E126" s="21"/>
       <c r="F126" s="19" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="G126" s="20">
         <v>15</v>
@@ -3843,7 +3798,7 @@
     </row>
     <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B127" s="15">
         <v>17</v>
@@ -3862,18 +3817,18 @@
     </row>
     <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="B128" s="15">
         <v>17</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D128" s="15"/>
       <c r="E128" s="21"/>
       <c r="F128" s="19" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="G128" s="20">
         <v>0.1</v>
@@ -3881,18 +3836,18 @@
     </row>
     <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="B129" s="15">
         <v>17</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D129" s="15"/>
       <c r="E129" s="21"/>
       <c r="F129" s="19" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G129" s="20">
         <v>0.32</v>
@@ -3900,18 +3855,18 @@
     </row>
     <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="B130" s="15">
         <v>17</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D130" s="15"/>
       <c r="E130" s="21"/>
       <c r="F130" s="19" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G130" s="20">
         <v>0.4</v>
@@ -3919,18 +3874,18 @@
     </row>
     <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="B131" s="15">
         <v>17</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D131" s="15"/>
       <c r="E131" s="21"/>
       <c r="F131" s="19" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="G131" s="20">
         <v>0.45</v>
@@ -3938,18 +3893,18 @@
     </row>
     <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="B132" s="15">
         <v>17</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D132" s="15"/>
       <c r="E132" s="21"/>
       <c r="F132" s="19" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G132" s="20">
         <v>0.48</v>
@@ -3957,18 +3912,18 @@
     </row>
     <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B133" s="15">
         <v>17</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D133" s="15"/>
       <c r="E133" s="21"/>
       <c r="F133" s="19" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G133" s="20">
         <v>0.5</v>
@@ -3976,18 +3931,18 @@
     </row>
     <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B134" s="15">
         <v>17</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D134" s="15"/>
       <c r="E134" s="21"/>
       <c r="F134" s="19" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G134" s="20">
         <v>0.55000000000000004</v>
@@ -3995,18 +3950,18 @@
     </row>
     <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="B135" s="15">
         <v>17</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D135" s="15"/>
       <c r="E135" s="21"/>
       <c r="F135" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G135" s="20">
         <v>0.6</v>
@@ -4014,18 +3969,18 @@
     </row>
     <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="B136" s="15">
         <v>17</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="21"/>
       <c r="F136" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G136" s="20">
         <v>0.75</v>
@@ -4033,18 +3988,18 @@
     </row>
     <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="B137" s="15">
         <v>17</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D137" s="15"/>
       <c r="E137" s="21"/>
       <c r="F137" s="19" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G137" s="20">
         <v>0.8</v>
@@ -4052,18 +4007,18 @@
     </row>
     <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="B138" s="15">
         <v>17</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D138" s="15"/>
       <c r="E138" s="21"/>
       <c r="F138" s="19" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="G138" s="20">
         <v>0.99</v>
@@ -4071,13 +4026,13 @@
     </row>
     <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B139" s="15">
         <v>17</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D139" s="15"/>
       <c r="E139" s="21"/>
@@ -4090,18 +4045,18 @@
     </row>
     <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B140" s="15">
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="21"/>
       <c r="F140" s="19" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="G140" s="20">
         <v>0.5</v>
@@ -4109,18 +4064,18 @@
     </row>
     <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="B141" s="15">
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="21"/>
       <c r="F141" s="19" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G141" s="20">
         <v>1</v>
@@ -4128,18 +4083,18 @@
     </row>
     <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="B142" s="15">
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D142" s="15"/>
       <c r="E142" s="21"/>
       <c r="F142" s="19" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G142" s="20">
         <v>1.3</v>
@@ -4147,18 +4102,18 @@
     </row>
     <row r="143" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="B143" s="15">
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D143" s="15"/>
       <c r="E143" s="21"/>
       <c r="F143" s="19" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="G143" s="20">
         <v>2</v>
@@ -4166,18 +4121,18 @@
     </row>
     <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B144" s="15">
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="21"/>
       <c r="F144" s="19" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G144" s="20">
         <v>2.1</v>
@@ -4185,18 +4140,18 @@
     </row>
     <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B145" s="15">
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D145" s="15"/>
       <c r="E145" s="21"/>
       <c r="F145" s="19" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G145" s="20">
         <v>3</v>
@@ -4204,18 +4159,18 @@
     </row>
     <row r="146" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="B146" s="15">
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="21"/>
       <c r="F146" s="19" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G146" s="20">
         <v>3</v>
@@ -4223,18 +4178,18 @@
     </row>
     <row r="147" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="B147" s="15">
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D147" s="15"/>
       <c r="E147" s="21"/>
       <c r="F147" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G147" s="20">
         <v>4</v>
@@ -4242,18 +4197,18 @@
     </row>
     <row r="148" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="B148" s="15">
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D148" s="15"/>
       <c r="E148" s="21"/>
       <c r="F148" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G148" s="20">
         <v>6</v>
@@ -4261,18 +4216,18 @@
     </row>
     <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B149" s="15">
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="21"/>
       <c r="F149" s="19" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G149" s="20">
         <v>10</v>
@@ -4280,18 +4235,18 @@
     </row>
     <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B150" s="15">
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D150" s="15"/>
       <c r="E150" s="21"/>
       <c r="F150" s="19" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="G150" s="20">
         <v>15</v>
@@ -4299,13 +4254,13 @@
     </row>
     <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="B151" s="15">
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D151" s="15"/>
       <c r="E151" s="21"/>
@@ -4318,18 +4273,18 @@
     </row>
     <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="B152" s="15">
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="21"/>
       <c r="F152" s="19" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="G152" s="20">
         <v>0.4</v>
@@ -4337,18 +4292,18 @@
     </row>
     <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="B153" s="15">
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="21"/>
       <c r="F153" s="19" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G153" s="20">
         <v>0.8</v>
@@ -4356,18 +4311,18 @@
     </row>
     <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="B154" s="15">
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="21"/>
       <c r="F154" s="19" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G154" s="20">
         <v>0.82</v>
@@ -4375,18 +4330,18 @@
     </row>
     <row r="155" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="B155" s="15">
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="21"/>
       <c r="F155" s="19" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="G155" s="20">
         <v>0.85</v>
@@ -4394,18 +4349,18 @@
     </row>
     <row r="156" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="B156" s="15">
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="21"/>
       <c r="F156" s="19" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G156" s="20">
         <v>0.87</v>
@@ -4413,18 +4368,18 @@
     </row>
     <row r="157" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="B157" s="15">
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="21"/>
       <c r="F157" s="19" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="G157" s="20">
         <v>0.88</v>
@@ -4432,18 +4387,18 @@
     </row>
     <row r="158" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="B158" s="15">
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="21"/>
       <c r="F158" s="19" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G158" s="20">
         <v>0.9</v>
@@ -4451,18 +4406,18 @@
     </row>
     <row r="159" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="B159" s="15">
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="21"/>
       <c r="F159" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G159" s="20">
         <v>0.91</v>
@@ -4470,18 +4425,18 @@
     </row>
     <row r="160" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="B160" s="15">
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="21"/>
       <c r="F160" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G160" s="20">
         <v>0.93</v>
@@ -4489,18 +4444,18 @@
     </row>
     <row r="161" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B161" s="15">
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="21"/>
       <c r="F161" s="19" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G161" s="20">
         <v>0.95</v>
@@ -4508,18 +4463,18 @@
     </row>
     <row r="162" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B162" s="15">
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="21"/>
       <c r="F162" s="19" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="G162" s="20">
         <v>0.99</v>
@@ -4527,13 +4482,13 @@
     </row>
     <row r="163" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="B163" s="15">
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="21"/>
@@ -4546,18 +4501,18 @@
     </row>
     <row r="164" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B164" s="15">
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D164" s="19"/>
       <c r="E164" s="19"/>
       <c r="F164" s="19" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="G164" s="20">
         <v>0.4</v>
@@ -4565,18 +4520,18 @@
     </row>
     <row r="165" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="B165" s="15">
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D165" s="19"/>
       <c r="E165" s="19"/>
       <c r="F165" s="19" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="G165" s="20">
         <v>0.55000000000000004</v>
@@ -4584,18 +4539,18 @@
     </row>
     <row r="166" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B166" s="15">
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D166" s="19"/>
       <c r="E166" s="19"/>
       <c r="F166" s="19" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="G166" s="20">
         <v>0.63</v>
@@ -4603,18 +4558,18 @@
     </row>
     <row r="167" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="B167" s="15">
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D167" s="19"/>
       <c r="E167" s="19"/>
       <c r="F167" s="19" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="G167" s="20">
         <v>0.74</v>
@@ -4622,18 +4577,18 @@
     </row>
     <row r="168" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B168" s="15">
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D168" s="19"/>
       <c r="E168" s="19"/>
       <c r="F168" s="19" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="G168" s="20">
         <v>0.85</v>
@@ -4641,18 +4596,18 @@
     </row>
     <row r="169" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="B169" s="15">
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D169" s="19"/>
       <c r="E169" s="19"/>
       <c r="F169" s="19" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="G169" s="20">
         <v>0.98</v>
@@ -4660,18 +4615,18 @@
     </row>
     <row r="170" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="B170" s="15">
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D170" s="19"/>
       <c r="E170" s="19"/>
       <c r="F170" s="19" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G170" s="20">
         <v>1</v>
@@ -4679,20 +4634,20 @@
     </row>
     <row r="171" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="B171" s="15">
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D171" s="15"/>
       <c r="E171" s="21" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F171" s="19" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="G171" s="20">
         <v>1</v>
@@ -4700,20 +4655,20 @@
     </row>
     <row r="172" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="B172" s="15">
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D172" s="15"/>
       <c r="E172" s="21" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F172" s="19" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="G172" s="20">
         <v>2</v>
@@ -4721,20 +4676,20 @@
     </row>
     <row r="173" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="B173" s="15">
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D173" s="15"/>
       <c r="E173" s="21" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F173" s="19" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="G173" s="20">
         <v>3</v>
@@ -4742,20 +4697,20 @@
     </row>
     <row r="174" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="B174" s="15">
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D174" s="15"/>
       <c r="E174" s="21" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F174" s="19" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G174" s="20">
         <v>4</v>
@@ -4763,20 +4718,20 @@
     </row>
     <row r="175" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="B175" s="15">
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D175" s="15"/>
       <c r="E175" s="21" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F175" s="19" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="G175" s="20">
         <v>5</v>
@@ -4784,20 +4739,20 @@
     </row>
     <row r="176" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="B176" s="15">
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D176" s="15"/>
       <c r="E176" s="21" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F176" s="19" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="G176" s="20">
         <v>6</v>
@@ -4805,20 +4760,20 @@
     </row>
     <row r="177" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="B177" s="15">
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="21" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F177" s="19" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="G177" s="20">
         <v>7</v>
@@ -4826,20 +4781,20 @@
     </row>
     <row r="178" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="B178" s="15">
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F178" s="19" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="G178" s="20">
         <v>0.4</v>
@@ -4847,20 +4802,20 @@
     </row>
     <row r="179" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="B179" s="15">
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F179" s="19" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="G179" s="20">
         <v>0.55000000000000004</v>
@@ -4868,20 +4823,20 @@
     </row>
     <row r="180" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B180" s="15">
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F180" s="19" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="G180" s="20">
         <v>0.63</v>
@@ -4889,20 +4844,20 @@
     </row>
     <row r="181" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B181" s="15">
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F181" s="19" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G181" s="20">
         <v>0.74</v>
@@ -4910,20 +4865,20 @@
     </row>
     <row r="182" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="B182" s="15">
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F182" s="19" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="G182" s="20">
         <v>0.85</v>
@@ -4931,20 +4886,20 @@
     </row>
     <row r="183" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B183" s="15">
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F183" s="19" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="G183" s="20">
         <v>0.98</v>
@@ -4952,20 +4907,20 @@
     </row>
     <row r="184" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B184" s="15">
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D184" s="15"/>
       <c r="E184" s="15" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F184" s="19" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="G184" s="20">
         <v>1</v>
@@ -4973,18 +4928,18 @@
     </row>
     <row r="185" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="B185" s="15">
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D185" s="22"/>
       <c r="E185" s="15"/>
       <c r="F185" s="22" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="G185" s="23">
         <v>1</v>
@@ -4992,18 +4947,18 @@
     </row>
     <row r="186" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B186" s="15">
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D186" s="22"/>
       <c r="E186" s="15"/>
       <c r="F186" s="22" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="G186" s="23">
         <v>2</v>
@@ -5011,18 +4966,18 @@
     </row>
     <row r="187" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="B187" s="15">
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D187" s="22"/>
       <c r="E187" s="15"/>
       <c r="F187" s="22" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="G187" s="23">
         <v>2.5</v>
@@ -5030,7 +4985,7 @@
     </row>
     <row r="188" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="B188" s="15">
         <v>17</v>
@@ -5040,10 +4995,10 @@
       </c>
       <c r="D188" s="15"/>
       <c r="E188" s="15" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F188" s="22" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="G188" s="23">
         <v>1</v>
@@ -5051,7 +5006,7 @@
     </row>
     <row r="189" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="B189" s="15">
         <v>17</v>
@@ -5061,10 +5016,10 @@
       </c>
       <c r="D189" s="15"/>
       <c r="E189" s="15" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F189" s="22" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="G189" s="23">
         <v>1.5</v>
@@ -5072,7 +5027,7 @@
     </row>
     <row r="190" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="B190" s="15">
         <v>17</v>
@@ -5082,10 +5037,10 @@
       </c>
       <c r="D190" s="15"/>
       <c r="E190" s="15" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F190" s="22" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="G190" s="23">
         <v>2</v>

</xml_diff>

<commit_message>
Uploaded 04-May-2021 16:22:08 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -141,9 +141,6 @@
     <t>10 Days</t>
   </si>
   <si>
-    <t>getBenefit_group().getCoveredDays().equals("$param")</t>
-  </si>
-  <si>
     <t>12 Hours</t>
   </si>
   <si>
@@ -829,6 +826,9 @@
   </si>
   <si>
     <t>AssumptionUsedByGroupName184</t>
+  </si>
+  <si>
+    <t>getBenefit_group().getCoveredDays().equals($param)</t>
   </si>
 </sst>
 </file>
@@ -1388,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B103" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1481,10 +1481,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>40</v>
+        <v>265</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>12</v>
@@ -1504,10 +1504,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>79</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>10</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="15">
         <v>17</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="15">
         <v>17</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="15">
         <v>17</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="15">
         <v>17</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="15">
         <v>17</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="15">
         <v>17</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="15">
         <v>17</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="15">
         <v>17</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="15">
         <v>17</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" s="15">
         <v>17</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B17" s="15">
         <v>17</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="15">
         <v>17</v>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B19" s="15">
         <v>17</v>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="15">
         <v>17</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="15">
         <v>17</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="15">
         <v>17</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="15">
         <v>17</v>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="15">
         <v>17</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B25" s="15">
         <v>17</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="15">
         <v>17</v>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" s="15">
         <v>17</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="15">
         <v>17</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B29" s="15">
         <v>17</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B30" s="15">
         <v>17</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B31" s="15">
         <v>17</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B32" s="15">
         <v>17</v>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B33" s="15">
         <v>17</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B34" s="15">
         <v>17</v>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="15">
         <v>17</v>
@@ -2069,7 +2069,7 @@
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B36" s="15">
         <v>17</v>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B37" s="15">
         <v>17</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38" s="15">
         <v>17</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="15">
         <v>17</v>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B40" s="15">
         <v>17</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B41" s="15">
         <v>17</v>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B42" s="15">
         <v>17</v>
@@ -2202,7 +2202,7 @@
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B43" s="15">
         <v>17</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B44" s="15">
         <v>17</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B45" s="15">
         <v>17</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B46" s="15">
         <v>17</v>
@@ -2278,7 +2278,7 @@
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B47" s="15">
         <v>17</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B48" s="15">
         <v>17</v>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B49" s="15">
         <v>17</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B50" s="15">
         <v>17</v>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B51" s="15">
         <v>17</v>
@@ -2373,7 +2373,7 @@
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B52" s="15">
         <v>17</v>
@@ -2392,7 +2392,7 @@
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B53" s="15">
         <v>17</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B54" s="15">
         <v>17</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B55" s="15">
         <v>17</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B56" s="15">
         <v>17</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B57" s="15">
         <v>17</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B58" s="15">
         <v>17</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B59" s="15">
         <v>17</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B60" s="15">
         <v>17</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B61" s="15">
         <v>17</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B62" s="15">
         <v>17</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B63" s="15">
         <v>17</v>
@@ -2601,7 +2601,7 @@
     </row>
     <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B64" s="15">
         <v>17</v>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B65" s="15">
         <v>17</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" s="15">
         <v>17</v>
@@ -2658,7 +2658,7 @@
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B67" s="15">
         <v>17</v>
@@ -2677,7 +2677,7 @@
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B68" s="15">
         <v>17</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B69" s="15">
         <v>17</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B70" s="15">
         <v>17</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B71" s="15">
         <v>17</v>
@@ -2753,7 +2753,7 @@
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B72" s="15">
         <v>17</v>
@@ -2772,7 +2772,7 @@
     </row>
     <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B73" s="15">
         <v>17</v>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B74" s="15">
         <v>17</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B75" s="15">
         <v>17</v>
@@ -2829,7 +2829,7 @@
     </row>
     <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B76" s="15">
         <v>17</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B77" s="15">
         <v>17</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B78" s="15">
         <v>17</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B79" s="15">
         <v>17</v>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B80" s="15">
         <v>17</v>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B81" s="15">
         <v>17</v>
@@ -2943,7 +2943,7 @@
     </row>
     <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B82" s="15">
         <v>17</v>
@@ -2962,7 +2962,7 @@
     </row>
     <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B83" s="15">
         <v>17</v>
@@ -2981,7 +2981,7 @@
     </row>
     <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B84" s="15">
         <v>17</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B85" s="15">
         <v>17</v>
@@ -3019,7 +3019,7 @@
     </row>
     <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B86" s="15">
         <v>17</v>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B87" s="15">
         <v>17</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B88" s="15">
         <v>17</v>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B89" s="15">
         <v>17</v>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B90" s="15">
         <v>17</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B91" s="15">
         <v>17</v>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B92" s="15">
         <v>17</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B93" s="15">
         <v>17</v>
@@ -3171,7 +3171,7 @@
     </row>
     <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B94" s="15">
         <v>17</v>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B95" s="15">
         <v>17</v>
@@ -3209,7 +3209,7 @@
     </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B96" s="15">
         <v>17</v>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B97" s="15">
         <v>17</v>
@@ -3247,7 +3247,7 @@
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B98" s="15">
         <v>17</v>
@@ -3266,7 +3266,7 @@
     </row>
     <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B99" s="15">
         <v>17</v>
@@ -3285,7 +3285,7 @@
     </row>
     <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B100" s="15">
         <v>17</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B101" s="15">
         <v>17</v>
@@ -3323,7 +3323,7 @@
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B102" s="15">
         <v>17</v>
@@ -3342,7 +3342,7 @@
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B103" s="15">
         <v>17</v>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B104" s="15">
         <v>17</v>
@@ -3380,7 +3380,7 @@
     </row>
     <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B105" s="15">
         <v>17</v>
@@ -3399,7 +3399,7 @@
     </row>
     <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B106" s="15">
         <v>17</v>
@@ -3418,7 +3418,7 @@
     </row>
     <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B107" s="15">
         <v>17</v>
@@ -3437,7 +3437,7 @@
     </row>
     <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B108" s="15">
         <v>17</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B109" s="15">
         <v>17</v>
@@ -3475,7 +3475,7 @@
     </row>
     <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B110" s="15">
         <v>17</v>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B111" s="15">
         <v>17</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B112" s="15">
         <v>17</v>
@@ -3532,7 +3532,7 @@
     </row>
     <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B113" s="15">
         <v>17</v>
@@ -3551,7 +3551,7 @@
     </row>
     <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B114" s="15">
         <v>17</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B115" s="15">
         <v>17</v>
@@ -3589,7 +3589,7 @@
     </row>
     <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B116" s="15">
         <v>17</v>
@@ -3600,7 +3600,7 @@
       <c r="D116" s="15"/>
       <c r="E116" s="21"/>
       <c r="F116" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G116" s="20">
         <v>0.5</v>
@@ -3608,7 +3608,7 @@
     </row>
     <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B117" s="15">
         <v>17</v>
@@ -3619,7 +3619,7 @@
       <c r="D117" s="15"/>
       <c r="E117" s="21"/>
       <c r="F117" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G117" s="20">
         <v>1</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B118" s="15">
         <v>17</v>
@@ -3638,7 +3638,7 @@
       <c r="D118" s="15"/>
       <c r="E118" s="21"/>
       <c r="F118" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G118" s="20">
         <v>1.3</v>
@@ -3646,7 +3646,7 @@
     </row>
     <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B119" s="15">
         <v>17</v>
@@ -3657,7 +3657,7 @@
       <c r="D119" s="15"/>
       <c r="E119" s="21"/>
       <c r="F119" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G119" s="20">
         <v>2</v>
@@ -3665,7 +3665,7 @@
     </row>
     <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B120" s="15">
         <v>17</v>
@@ -3676,7 +3676,7 @@
       <c r="D120" s="15"/>
       <c r="E120" s="21"/>
       <c r="F120" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G120" s="20">
         <v>2.1</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B121" s="15">
         <v>17</v>
@@ -3695,7 +3695,7 @@
       <c r="D121" s="15"/>
       <c r="E121" s="21"/>
       <c r="F121" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G121" s="20">
         <v>3</v>
@@ -3703,7 +3703,7 @@
     </row>
     <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B122" s="15">
         <v>17</v>
@@ -3714,7 +3714,7 @@
       <c r="D122" s="15"/>
       <c r="E122" s="21"/>
       <c r="F122" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G122" s="20">
         <v>3</v>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B123" s="15">
         <v>17</v>
@@ -3741,7 +3741,7 @@
     </row>
     <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B124" s="15">
         <v>17</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B125" s="15">
         <v>17</v>
@@ -3779,7 +3779,7 @@
     </row>
     <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B126" s="15">
         <v>17</v>
@@ -3790,7 +3790,7 @@
       <c r="D126" s="15"/>
       <c r="E126" s="21"/>
       <c r="F126" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G126" s="20">
         <v>15</v>
@@ -3798,7 +3798,7 @@
     </row>
     <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B127" s="15">
         <v>17</v>
@@ -3817,18 +3817,18 @@
     </row>
     <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B128" s="15">
         <v>17</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D128" s="15"/>
       <c r="E128" s="21"/>
       <c r="F128" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G128" s="20">
         <v>0.1</v>
@@ -3836,18 +3836,18 @@
     </row>
     <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B129" s="15">
         <v>17</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D129" s="15"/>
       <c r="E129" s="21"/>
       <c r="F129" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G129" s="20">
         <v>0.32</v>
@@ -3855,18 +3855,18 @@
     </row>
     <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B130" s="15">
         <v>17</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D130" s="15"/>
       <c r="E130" s="21"/>
       <c r="F130" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G130" s="20">
         <v>0.4</v>
@@ -3874,18 +3874,18 @@
     </row>
     <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B131" s="15">
         <v>17</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D131" s="15"/>
       <c r="E131" s="21"/>
       <c r="F131" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G131" s="20">
         <v>0.45</v>
@@ -3893,18 +3893,18 @@
     </row>
     <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B132" s="15">
         <v>17</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D132" s="15"/>
       <c r="E132" s="21"/>
       <c r="F132" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G132" s="20">
         <v>0.48</v>
@@ -3912,18 +3912,18 @@
     </row>
     <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B133" s="15">
         <v>17</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D133" s="15"/>
       <c r="E133" s="21"/>
       <c r="F133" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G133" s="20">
         <v>0.5</v>
@@ -3931,18 +3931,18 @@
     </row>
     <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B134" s="15">
         <v>17</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D134" s="15"/>
       <c r="E134" s="21"/>
       <c r="F134" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G134" s="20">
         <v>0.55000000000000004</v>
@@ -3950,13 +3950,13 @@
     </row>
     <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B135" s="15">
         <v>17</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D135" s="15"/>
       <c r="E135" s="21"/>
@@ -3969,13 +3969,13 @@
     </row>
     <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B136" s="15">
         <v>17</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="21"/>
@@ -3988,13 +3988,13 @@
     </row>
     <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B137" s="15">
         <v>17</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D137" s="15"/>
       <c r="E137" s="21"/>
@@ -4007,18 +4007,18 @@
     </row>
     <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B138" s="15">
         <v>17</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D138" s="15"/>
       <c r="E138" s="21"/>
       <c r="F138" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G138" s="20">
         <v>0.99</v>
@@ -4026,13 +4026,13 @@
     </row>
     <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B139" s="15">
         <v>17</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D139" s="15"/>
       <c r="E139" s="21"/>
@@ -4045,18 +4045,18 @@
     </row>
     <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B140" s="15">
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="21"/>
       <c r="F140" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G140" s="20">
         <v>0.5</v>
@@ -4064,18 +4064,18 @@
     </row>
     <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B141" s="15">
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="21"/>
       <c r="F141" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G141" s="20">
         <v>1</v>
@@ -4083,18 +4083,18 @@
     </row>
     <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B142" s="15">
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D142" s="15"/>
       <c r="E142" s="21"/>
       <c r="F142" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G142" s="20">
         <v>1.3</v>
@@ -4102,18 +4102,18 @@
     </row>
     <row r="143" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B143" s="15">
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D143" s="15"/>
       <c r="E143" s="21"/>
       <c r="F143" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G143" s="20">
         <v>2</v>
@@ -4121,18 +4121,18 @@
     </row>
     <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B144" s="15">
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="21"/>
       <c r="F144" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G144" s="20">
         <v>2.1</v>
@@ -4140,18 +4140,18 @@
     </row>
     <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B145" s="15">
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D145" s="15"/>
       <c r="E145" s="21"/>
       <c r="F145" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G145" s="20">
         <v>3</v>
@@ -4159,18 +4159,18 @@
     </row>
     <row r="146" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B146" s="15">
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="21"/>
       <c r="F146" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G146" s="20">
         <v>3</v>
@@ -4178,13 +4178,13 @@
     </row>
     <row r="147" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B147" s="15">
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D147" s="15"/>
       <c r="E147" s="21"/>
@@ -4197,13 +4197,13 @@
     </row>
     <row r="148" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B148" s="15">
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D148" s="15"/>
       <c r="E148" s="21"/>
@@ -4216,13 +4216,13 @@
     </row>
     <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B149" s="15">
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="21"/>
@@ -4235,18 +4235,18 @@
     </row>
     <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B150" s="15">
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D150" s="15"/>
       <c r="E150" s="21"/>
       <c r="F150" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G150" s="20">
         <v>15</v>
@@ -4254,13 +4254,13 @@
     </row>
     <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B151" s="15">
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D151" s="15"/>
       <c r="E151" s="21"/>
@@ -4273,18 +4273,18 @@
     </row>
     <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B152" s="15">
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="21"/>
       <c r="F152" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G152" s="20">
         <v>0.4</v>
@@ -4292,18 +4292,18 @@
     </row>
     <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B153" s="15">
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="21"/>
       <c r="F153" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G153" s="20">
         <v>0.8</v>
@@ -4311,18 +4311,18 @@
     </row>
     <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B154" s="15">
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="21"/>
       <c r="F154" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G154" s="20">
         <v>0.82</v>
@@ -4330,18 +4330,18 @@
     </row>
     <row r="155" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B155" s="15">
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="21"/>
       <c r="F155" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G155" s="20">
         <v>0.85</v>
@@ -4349,18 +4349,18 @@
     </row>
     <row r="156" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B156" s="15">
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="21"/>
       <c r="F156" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G156" s="20">
         <v>0.87</v>
@@ -4368,18 +4368,18 @@
     </row>
     <row r="157" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B157" s="15">
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="21"/>
       <c r="F157" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G157" s="20">
         <v>0.88</v>
@@ -4387,18 +4387,18 @@
     </row>
     <row r="158" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B158" s="15">
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="21"/>
       <c r="F158" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G158" s="20">
         <v>0.9</v>
@@ -4406,13 +4406,13 @@
     </row>
     <row r="159" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B159" s="15">
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="21"/>
@@ -4425,13 +4425,13 @@
     </row>
     <row r="160" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B160" s="15">
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="21"/>
@@ -4444,13 +4444,13 @@
     </row>
     <row r="161" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B161" s="15">
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="21"/>
@@ -4463,18 +4463,18 @@
     </row>
     <row r="162" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B162" s="15">
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="21"/>
       <c r="F162" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G162" s="20">
         <v>0.99</v>
@@ -4482,13 +4482,13 @@
     </row>
     <row r="163" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B163" s="15">
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="21"/>
@@ -4501,18 +4501,18 @@
     </row>
     <row r="164" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B164" s="15">
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D164" s="19"/>
       <c r="E164" s="19"/>
       <c r="F164" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G164" s="20">
         <v>0.4</v>
@@ -4520,18 +4520,18 @@
     </row>
     <row r="165" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B165" s="15">
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D165" s="19"/>
       <c r="E165" s="19"/>
       <c r="F165" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G165" s="20">
         <v>0.55000000000000004</v>
@@ -4539,18 +4539,18 @@
     </row>
     <row r="166" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B166" s="15">
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D166" s="19"/>
       <c r="E166" s="19"/>
       <c r="F166" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G166" s="20">
         <v>0.63</v>
@@ -4558,18 +4558,18 @@
     </row>
     <row r="167" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B167" s="15">
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D167" s="19"/>
       <c r="E167" s="19"/>
       <c r="F167" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G167" s="20">
         <v>0.74</v>
@@ -4577,18 +4577,18 @@
     </row>
     <row r="168" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B168" s="15">
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D168" s="19"/>
       <c r="E168" s="19"/>
       <c r="F168" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G168" s="20">
         <v>0.85</v>
@@ -4596,18 +4596,18 @@
     </row>
     <row r="169" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B169" s="15">
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D169" s="19"/>
       <c r="E169" s="19"/>
       <c r="F169" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G169" s="20">
         <v>0.98</v>
@@ -4615,18 +4615,18 @@
     </row>
     <row r="170" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B170" s="15">
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D170" s="19"/>
       <c r="E170" s="19"/>
       <c r="F170" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G170" s="20">
         <v>1</v>
@@ -4634,20 +4634,20 @@
     </row>
     <row r="171" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B171" s="15">
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D171" s="15"/>
       <c r="E171" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F171" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G171" s="20">
         <v>1</v>
@@ -4655,20 +4655,20 @@
     </row>
     <row r="172" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B172" s="15">
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D172" s="15"/>
       <c r="E172" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F172" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G172" s="20">
         <v>2</v>
@@ -4676,20 +4676,20 @@
     </row>
     <row r="173" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B173" s="15">
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D173" s="15"/>
       <c r="E173" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F173" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G173" s="20">
         <v>3</v>
@@ -4697,20 +4697,20 @@
     </row>
     <row r="174" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B174" s="15">
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D174" s="15"/>
       <c r="E174" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F174" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G174" s="20">
         <v>4</v>
@@ -4718,20 +4718,20 @@
     </row>
     <row r="175" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B175" s="15">
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D175" s="15"/>
       <c r="E175" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F175" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G175" s="20">
         <v>5</v>
@@ -4739,20 +4739,20 @@
     </row>
     <row r="176" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B176" s="15">
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D176" s="15"/>
       <c r="E176" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F176" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G176" s="20">
         <v>6</v>
@@ -4760,20 +4760,20 @@
     </row>
     <row r="177" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B177" s="15">
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F177" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G177" s="20">
         <v>7</v>
@@ -4781,20 +4781,20 @@
     </row>
     <row r="178" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B178" s="15">
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F178" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G178" s="20">
         <v>0.4</v>
@@ -4802,20 +4802,20 @@
     </row>
     <row r="179" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B179" s="15">
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F179" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G179" s="20">
         <v>0.55000000000000004</v>
@@ -4823,20 +4823,20 @@
     </row>
     <row r="180" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B180" s="15">
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F180" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G180" s="20">
         <v>0.63</v>
@@ -4844,20 +4844,20 @@
     </row>
     <row r="181" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B181" s="15">
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F181" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G181" s="20">
         <v>0.74</v>
@@ -4865,20 +4865,20 @@
     </row>
     <row r="182" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B182" s="15">
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F182" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G182" s="20">
         <v>0.85</v>
@@ -4886,20 +4886,20 @@
     </row>
     <row r="183" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B183" s="15">
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F183" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G183" s="20">
         <v>0.98</v>
@@ -4907,20 +4907,20 @@
     </row>
     <row r="184" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B184" s="15">
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D184" s="15"/>
       <c r="E184" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F184" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G184" s="20">
         <v>1</v>
@@ -4928,18 +4928,18 @@
     </row>
     <row r="185" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B185" s="15">
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D185" s="22"/>
       <c r="E185" s="15"/>
       <c r="F185" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G185" s="23">
         <v>1</v>
@@ -4947,18 +4947,18 @@
     </row>
     <row r="186" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B186" s="15">
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D186" s="22"/>
       <c r="E186" s="15"/>
       <c r="F186" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G186" s="23">
         <v>2</v>
@@ -4966,18 +4966,18 @@
     </row>
     <row r="187" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B187" s="15">
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D187" s="22"/>
       <c r="E187" s="15"/>
       <c r="F187" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G187" s="23">
         <v>2.5</v>
@@ -4985,7 +4985,7 @@
     </row>
     <row r="188" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B188" s="15">
         <v>17</v>
@@ -4995,10 +4995,10 @@
       </c>
       <c r="D188" s="15"/>
       <c r="E188" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F188" s="22" t="s">
         <v>75</v>
-      </c>
-      <c r="F188" s="22" t="s">
-        <v>76</v>
       </c>
       <c r="G188" s="23">
         <v>1</v>
@@ -5006,7 +5006,7 @@
     </row>
     <row r="189" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B189" s="15">
         <v>17</v>
@@ -5016,10 +5016,10 @@
       </c>
       <c r="D189" s="15"/>
       <c r="E189" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F189" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G189" s="23">
         <v>1.5</v>
@@ -5027,7 +5027,7 @@
     </row>
     <row r="190" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B190" s="15">
         <v>17</v>
@@ -5037,10 +5037,10 @@
       </c>
       <c r="D190" s="15"/>
       <c r="E190" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F190" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G190" s="23">
         <v>2</v>

</xml_diff>

<commit_message>
Uploaded 04-May-2021 16:24:53 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -828,7 +828,7 @@
     <t>AssumptionUsedByGroupName184</t>
   </si>
   <si>
-    <t>getBenefit_group().getCoveredDays().equals($param)</t>
+    <t>getBenefit_group().getCoveredDays()==$param</t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1474,7 @@
       <c r="G4" s="8"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">

</xml_diff>

<commit_message>
Uploaded 04-May-2021 16:35:27 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -126,9 +126,6 @@
     <t>INFERTILITY CARE</t>
   </si>
   <si>
-    <t>RENAL CARE</t>
-  </si>
-  <si>
     <t>ADMISSIONS AND ACCOMMODATION</t>
   </si>
   <si>
@@ -829,6 +826,9 @@
   </si>
   <si>
     <t>getBenefit_group().getCoveredDays()==$param</t>
+  </si>
+  <si>
+    <t>RENAL CARE (DIALYSIS)</t>
   </si>
 </sst>
 </file>
@@ -1388,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B75" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1481,10 +1481,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>12</v>
@@ -1504,10 +1504,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>79</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>10</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="15">
         <v>17</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="15">
         <v>17</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="15">
         <v>17</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="15">
         <v>17</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="15">
         <v>17</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="15">
         <v>17</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="15">
         <v>17</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="15">
         <v>17</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="15">
         <v>17</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="15">
         <v>17</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="15">
         <v>17</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="15">
         <v>17</v>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="15">
         <v>17</v>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="15">
         <v>17</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="15">
         <v>17</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="15">
         <v>17</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="15">
         <v>17</v>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="15">
         <v>17</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25" s="15">
         <v>17</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" s="15">
         <v>17</v>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="15">
         <v>17</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" s="15">
         <v>17</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" s="15">
         <v>17</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="15">
         <v>17</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B31" s="15">
         <v>17</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B32" s="15">
         <v>17</v>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B33" s="15">
         <v>17</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B34" s="15">
         <v>17</v>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" s="15">
         <v>17</v>
@@ -2069,7 +2069,7 @@
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" s="15">
         <v>17</v>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B37" s="15">
         <v>17</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" s="15">
         <v>17</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39" s="15">
         <v>17</v>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B40" s="15">
         <v>17</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B41" s="15">
         <v>17</v>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B42" s="15">
         <v>17</v>
@@ -2202,7 +2202,7 @@
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B43" s="15">
         <v>17</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B44" s="15">
         <v>17</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B45" s="15">
         <v>17</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B46" s="15">
         <v>17</v>
@@ -2278,7 +2278,7 @@
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B47" s="15">
         <v>17</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B48" s="15">
         <v>17</v>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B49" s="15">
         <v>17</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B50" s="15">
         <v>17</v>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B51" s="15">
         <v>17</v>
@@ -2373,7 +2373,7 @@
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B52" s="15">
         <v>17</v>
@@ -2392,7 +2392,7 @@
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B53" s="15">
         <v>17</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B54" s="15">
         <v>17</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B55" s="15">
         <v>17</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B56" s="15">
         <v>17</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B57" s="15">
         <v>17</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B58" s="15">
         <v>17</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B59" s="15">
         <v>17</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B60" s="15">
         <v>17</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B61" s="15">
         <v>17</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B62" s="15">
         <v>17</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B63" s="15">
         <v>17</v>
@@ -2601,7 +2601,7 @@
     </row>
     <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B64" s="15">
         <v>17</v>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B65" s="15">
         <v>17</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B66" s="15">
         <v>17</v>
@@ -2658,7 +2658,7 @@
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B67" s="15">
         <v>17</v>
@@ -2677,7 +2677,7 @@
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B68" s="15">
         <v>17</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B69" s="15">
         <v>17</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B70" s="15">
         <v>17</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B71" s="15">
         <v>17</v>
@@ -2753,7 +2753,7 @@
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B72" s="15">
         <v>17</v>
@@ -2772,7 +2772,7 @@
     </row>
     <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B73" s="15">
         <v>17</v>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B74" s="15">
         <v>17</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B75" s="15">
         <v>17</v>
@@ -2829,7 +2829,7 @@
     </row>
     <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B76" s="15">
         <v>17</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B77" s="15">
         <v>17</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B78" s="15">
         <v>17</v>
@@ -2886,13 +2886,13 @@
     </row>
     <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B79" s="15">
         <v>17</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="21"/>
@@ -2905,13 +2905,13 @@
     </row>
     <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B80" s="15">
         <v>17</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="21"/>
@@ -2924,13 +2924,13 @@
     </row>
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B81" s="15">
         <v>17</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="21"/>
@@ -2943,13 +2943,13 @@
     </row>
     <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B82" s="15">
         <v>17</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
@@ -2962,13 +2962,13 @@
     </row>
     <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B83" s="15">
         <v>17</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
@@ -2981,13 +2981,13 @@
     </row>
     <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B84" s="15">
         <v>17</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21"/>
@@ -3000,13 +3000,13 @@
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B85" s="15">
         <v>17</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
@@ -3019,13 +3019,13 @@
     </row>
     <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B86" s="15">
         <v>17</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21"/>
@@ -3038,13 +3038,13 @@
     </row>
     <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B87" s="15">
         <v>17</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="21"/>
@@ -3057,13 +3057,13 @@
     </row>
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B88" s="15">
         <v>17</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
@@ -3076,13 +3076,13 @@
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B89" s="15">
         <v>17</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21"/>
@@ -3095,13 +3095,13 @@
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B90" s="15">
         <v>17</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D90" s="21"/>
       <c r="E90" s="21"/>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B91" s="15">
         <v>17</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
@@ -3133,13 +3133,13 @@
     </row>
     <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B92" s="15">
         <v>17</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
@@ -3152,13 +3152,13 @@
     </row>
     <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B93" s="15">
         <v>17</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
@@ -3171,13 +3171,13 @@
     </row>
     <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B94" s="15">
         <v>17</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
@@ -3190,13 +3190,13 @@
     </row>
     <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B95" s="15">
         <v>17</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D95" s="21"/>
       <c r="E95" s="21"/>
@@ -3209,13 +3209,13 @@
     </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B96" s="15">
         <v>17</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>35</v>
+        <v>265</v>
       </c>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
@@ -3228,13 +3228,13 @@
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B97" s="15">
         <v>17</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D97" s="19">
         <v>1</v>
@@ -3247,13 +3247,13 @@
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B98" s="15">
         <v>17</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D98" s="19">
         <v>2</v>
@@ -3266,13 +3266,13 @@
     </row>
     <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B99" s="15">
         <v>17</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D99" s="19">
         <v>3</v>
@@ -3285,13 +3285,13 @@
     </row>
     <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B100" s="15">
         <v>17</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D100" s="19">
         <v>4</v>
@@ -3304,13 +3304,13 @@
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B101" s="15">
         <v>17</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D101" s="19">
         <v>5</v>
@@ -3323,13 +3323,13 @@
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B102" s="15">
         <v>17</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D102" s="19">
         <v>6</v>
@@ -3342,13 +3342,13 @@
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B103" s="15">
         <v>17</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D103" s="19">
         <v>7</v>
@@ -3361,13 +3361,13 @@
     </row>
     <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B104" s="15">
         <v>17</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D104" s="19">
         <v>8</v>
@@ -3380,13 +3380,13 @@
     </row>
     <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B105" s="15">
         <v>17</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D105" s="19">
         <v>9</v>
@@ -3399,13 +3399,13 @@
     </row>
     <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B106" s="15">
         <v>17</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D106" s="19">
         <v>10</v>
@@ -3418,13 +3418,13 @@
     </row>
     <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B107" s="15">
         <v>17</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D107" s="19">
         <v>15</v>
@@ -3437,13 +3437,13 @@
     </row>
     <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B108" s="15">
         <v>17</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D108" s="19">
         <v>20</v>
@@ -3456,13 +3456,13 @@
     </row>
     <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B109" s="15">
         <v>17</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D109" s="19">
         <v>25</v>
@@ -3475,13 +3475,13 @@
     </row>
     <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B110" s="15">
         <v>17</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D110" s="19">
         <v>30</v>
@@ -3494,13 +3494,13 @@
     </row>
     <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B111" s="15">
         <v>17</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D111" s="19">
         <v>45</v>
@@ -3513,13 +3513,13 @@
     </row>
     <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B112" s="15">
         <v>17</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D112" s="19">
         <v>50</v>
@@ -3532,13 +3532,13 @@
     </row>
     <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B113" s="15">
         <v>17</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D113" s="19">
         <v>60</v>
@@ -3551,13 +3551,13 @@
     </row>
     <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B114" s="15">
         <v>17</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D114" s="19">
         <v>100</v>
@@ -3570,13 +3570,13 @@
     </row>
     <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B115" s="15">
         <v>17</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D115" s="19">
         <v>-1</v>
@@ -3589,18 +3589,18 @@
     </row>
     <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B116" s="15">
         <v>17</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D116" s="15"/>
       <c r="E116" s="21"/>
       <c r="F116" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G116" s="20">
         <v>0.5</v>
@@ -3608,18 +3608,18 @@
     </row>
     <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B117" s="15">
         <v>17</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D117" s="15"/>
       <c r="E117" s="21"/>
       <c r="F117" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G117" s="20">
         <v>1</v>
@@ -3627,18 +3627,18 @@
     </row>
     <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B118" s="15">
         <v>17</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D118" s="15"/>
       <c r="E118" s="21"/>
       <c r="F118" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G118" s="20">
         <v>1.3</v>
@@ -3646,18 +3646,18 @@
     </row>
     <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B119" s="15">
         <v>17</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D119" s="15"/>
       <c r="E119" s="21"/>
       <c r="F119" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G119" s="20">
         <v>2</v>
@@ -3665,18 +3665,18 @@
     </row>
     <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B120" s="15">
         <v>17</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D120" s="15"/>
       <c r="E120" s="21"/>
       <c r="F120" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G120" s="20">
         <v>2.1</v>
@@ -3684,18 +3684,18 @@
     </row>
     <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B121" s="15">
         <v>17</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D121" s="15"/>
       <c r="E121" s="21"/>
       <c r="F121" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G121" s="20">
         <v>3</v>
@@ -3703,18 +3703,18 @@
     </row>
     <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B122" s="15">
         <v>17</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D122" s="15"/>
       <c r="E122" s="21"/>
       <c r="F122" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G122" s="20">
         <v>3</v>
@@ -3722,18 +3722,18 @@
     </row>
     <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B123" s="15">
         <v>17</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D123" s="15"/>
       <c r="E123" s="21"/>
       <c r="F123" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G123" s="20">
         <v>4</v>
@@ -3741,18 +3741,18 @@
     </row>
     <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B124" s="15">
         <v>17</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D124" s="15"/>
       <c r="E124" s="21"/>
       <c r="F124" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G124" s="20">
         <v>6</v>
@@ -3760,18 +3760,18 @@
     </row>
     <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B125" s="15">
         <v>17</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D125" s="15"/>
       <c r="E125" s="21"/>
       <c r="F125" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G125" s="20">
         <v>10</v>
@@ -3779,18 +3779,18 @@
     </row>
     <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B126" s="15">
         <v>17</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D126" s="15"/>
       <c r="E126" s="21"/>
       <c r="F126" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G126" s="20">
         <v>15</v>
@@ -3798,13 +3798,13 @@
     </row>
     <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B127" s="15">
         <v>17</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D127" s="15"/>
       <c r="E127" s="21"/>
@@ -3817,18 +3817,18 @@
     </row>
     <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B128" s="15">
         <v>17</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D128" s="15"/>
       <c r="E128" s="21"/>
       <c r="F128" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G128" s="20">
         <v>0.1</v>
@@ -3836,18 +3836,18 @@
     </row>
     <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B129" s="15">
         <v>17</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D129" s="15"/>
       <c r="E129" s="21"/>
       <c r="F129" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G129" s="20">
         <v>0.32</v>
@@ -3855,18 +3855,18 @@
     </row>
     <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B130" s="15">
         <v>17</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D130" s="15"/>
       <c r="E130" s="21"/>
       <c r="F130" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G130" s="20">
         <v>0.4</v>
@@ -3874,18 +3874,18 @@
     </row>
     <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B131" s="15">
         <v>17</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D131" s="15"/>
       <c r="E131" s="21"/>
       <c r="F131" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G131" s="20">
         <v>0.45</v>
@@ -3893,18 +3893,18 @@
     </row>
     <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B132" s="15">
         <v>17</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D132" s="15"/>
       <c r="E132" s="21"/>
       <c r="F132" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G132" s="20">
         <v>0.48</v>
@@ -3912,18 +3912,18 @@
     </row>
     <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B133" s="15">
         <v>17</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D133" s="15"/>
       <c r="E133" s="21"/>
       <c r="F133" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G133" s="20">
         <v>0.5</v>
@@ -3931,18 +3931,18 @@
     </row>
     <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B134" s="15">
         <v>17</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D134" s="15"/>
       <c r="E134" s="21"/>
       <c r="F134" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G134" s="20">
         <v>0.55000000000000004</v>
@@ -3950,18 +3950,18 @@
     </row>
     <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B135" s="15">
         <v>17</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D135" s="15"/>
       <c r="E135" s="21"/>
       <c r="F135" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G135" s="20">
         <v>0.6</v>
@@ -3969,18 +3969,18 @@
     </row>
     <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B136" s="15">
         <v>17</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="21"/>
       <c r="F136" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G136" s="20">
         <v>0.75</v>
@@ -3988,18 +3988,18 @@
     </row>
     <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B137" s="15">
         <v>17</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D137" s="15"/>
       <c r="E137" s="21"/>
       <c r="F137" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G137" s="20">
         <v>0.8</v>
@@ -4007,18 +4007,18 @@
     </row>
     <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B138" s="15">
         <v>17</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D138" s="15"/>
       <c r="E138" s="21"/>
       <c r="F138" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G138" s="20">
         <v>0.99</v>
@@ -4026,13 +4026,13 @@
     </row>
     <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B139" s="15">
         <v>17</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D139" s="15"/>
       <c r="E139" s="21"/>
@@ -4045,18 +4045,18 @@
     </row>
     <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B140" s="15">
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="21"/>
       <c r="F140" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G140" s="20">
         <v>0.5</v>
@@ -4064,18 +4064,18 @@
     </row>
     <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B141" s="15">
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="21"/>
       <c r="F141" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G141" s="20">
         <v>1</v>
@@ -4083,18 +4083,18 @@
     </row>
     <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B142" s="15">
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D142" s="15"/>
       <c r="E142" s="21"/>
       <c r="F142" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G142" s="20">
         <v>1.3</v>
@@ -4102,18 +4102,18 @@
     </row>
     <row r="143" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B143" s="15">
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D143" s="15"/>
       <c r="E143" s="21"/>
       <c r="F143" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G143" s="20">
         <v>2</v>
@@ -4121,18 +4121,18 @@
     </row>
     <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B144" s="15">
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="21"/>
       <c r="F144" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G144" s="20">
         <v>2.1</v>
@@ -4140,18 +4140,18 @@
     </row>
     <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B145" s="15">
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D145" s="15"/>
       <c r="E145" s="21"/>
       <c r="F145" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G145" s="20">
         <v>3</v>
@@ -4159,18 +4159,18 @@
     </row>
     <row r="146" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B146" s="15">
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="21"/>
       <c r="F146" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G146" s="20">
         <v>3</v>
@@ -4178,18 +4178,18 @@
     </row>
     <row r="147" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B147" s="15">
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D147" s="15"/>
       <c r="E147" s="21"/>
       <c r="F147" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G147" s="20">
         <v>4</v>
@@ -4197,18 +4197,18 @@
     </row>
     <row r="148" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B148" s="15">
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D148" s="15"/>
       <c r="E148" s="21"/>
       <c r="F148" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G148" s="20">
         <v>6</v>
@@ -4216,18 +4216,18 @@
     </row>
     <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B149" s="15">
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="21"/>
       <c r="F149" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G149" s="20">
         <v>10</v>
@@ -4235,18 +4235,18 @@
     </row>
     <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B150" s="15">
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D150" s="15"/>
       <c r="E150" s="21"/>
       <c r="F150" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G150" s="20">
         <v>15</v>
@@ -4254,13 +4254,13 @@
     </row>
     <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B151" s="15">
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D151" s="15"/>
       <c r="E151" s="21"/>
@@ -4273,18 +4273,18 @@
     </row>
     <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B152" s="15">
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="21"/>
       <c r="F152" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G152" s="20">
         <v>0.4</v>
@@ -4292,18 +4292,18 @@
     </row>
     <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B153" s="15">
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="21"/>
       <c r="F153" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G153" s="20">
         <v>0.8</v>
@@ -4311,18 +4311,18 @@
     </row>
     <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B154" s="15">
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="21"/>
       <c r="F154" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G154" s="20">
         <v>0.82</v>
@@ -4330,18 +4330,18 @@
     </row>
     <row r="155" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B155" s="15">
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="21"/>
       <c r="F155" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G155" s="20">
         <v>0.85</v>
@@ -4349,18 +4349,18 @@
     </row>
     <row r="156" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B156" s="15">
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="21"/>
       <c r="F156" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G156" s="20">
         <v>0.87</v>
@@ -4368,18 +4368,18 @@
     </row>
     <row r="157" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B157" s="15">
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="21"/>
       <c r="F157" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G157" s="20">
         <v>0.88</v>
@@ -4387,18 +4387,18 @@
     </row>
     <row r="158" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B158" s="15">
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="21"/>
       <c r="F158" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G158" s="20">
         <v>0.9</v>
@@ -4406,18 +4406,18 @@
     </row>
     <row r="159" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B159" s="15">
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="21"/>
       <c r="F159" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G159" s="20">
         <v>0.91</v>
@@ -4425,18 +4425,18 @@
     </row>
     <row r="160" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B160" s="15">
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="21"/>
       <c r="F160" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G160" s="20">
         <v>0.93</v>
@@ -4444,18 +4444,18 @@
     </row>
     <row r="161" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B161" s="15">
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="21"/>
       <c r="F161" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G161" s="20">
         <v>0.95</v>
@@ -4463,18 +4463,18 @@
     </row>
     <row r="162" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B162" s="15">
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="21"/>
       <c r="F162" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G162" s="20">
         <v>0.99</v>
@@ -4482,13 +4482,13 @@
     </row>
     <row r="163" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B163" s="15">
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="21"/>
@@ -4501,18 +4501,18 @@
     </row>
     <row r="164" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B164" s="15">
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D164" s="19"/>
       <c r="E164" s="19"/>
       <c r="F164" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G164" s="20">
         <v>0.4</v>
@@ -4520,18 +4520,18 @@
     </row>
     <row r="165" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B165" s="15">
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D165" s="19"/>
       <c r="E165" s="19"/>
       <c r="F165" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G165" s="20">
         <v>0.55000000000000004</v>
@@ -4539,18 +4539,18 @@
     </row>
     <row r="166" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B166" s="15">
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D166" s="19"/>
       <c r="E166" s="19"/>
       <c r="F166" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G166" s="20">
         <v>0.63</v>
@@ -4558,18 +4558,18 @@
     </row>
     <row r="167" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B167" s="15">
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D167" s="19"/>
       <c r="E167" s="19"/>
       <c r="F167" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G167" s="20">
         <v>0.74</v>
@@ -4577,18 +4577,18 @@
     </row>
     <row r="168" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B168" s="15">
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D168" s="19"/>
       <c r="E168" s="19"/>
       <c r="F168" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G168" s="20">
         <v>0.85</v>
@@ -4596,18 +4596,18 @@
     </row>
     <row r="169" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B169" s="15">
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D169" s="19"/>
       <c r="E169" s="19"/>
       <c r="F169" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G169" s="20">
         <v>0.98</v>
@@ -4615,18 +4615,18 @@
     </row>
     <row r="170" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B170" s="15">
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D170" s="19"/>
       <c r="E170" s="19"/>
       <c r="F170" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G170" s="20">
         <v>1</v>
@@ -4634,20 +4634,20 @@
     </row>
     <row r="171" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B171" s="15">
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D171" s="15"/>
       <c r="E171" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F171" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G171" s="20">
         <v>1</v>
@@ -4655,20 +4655,20 @@
     </row>
     <row r="172" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B172" s="15">
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D172" s="15"/>
       <c r="E172" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F172" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G172" s="20">
         <v>2</v>
@@ -4676,20 +4676,20 @@
     </row>
     <row r="173" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B173" s="15">
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D173" s="15"/>
       <c r="E173" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F173" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G173" s="20">
         <v>3</v>
@@ -4697,20 +4697,20 @@
     </row>
     <row r="174" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B174" s="15">
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D174" s="15"/>
       <c r="E174" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F174" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G174" s="20">
         <v>4</v>
@@ -4718,20 +4718,20 @@
     </row>
     <row r="175" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B175" s="15">
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D175" s="15"/>
       <c r="E175" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F175" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G175" s="20">
         <v>5</v>
@@ -4739,20 +4739,20 @@
     </row>
     <row r="176" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B176" s="15">
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D176" s="15"/>
       <c r="E176" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F176" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G176" s="20">
         <v>6</v>
@@ -4760,20 +4760,20 @@
     </row>
     <row r="177" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B177" s="15">
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F177" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G177" s="20">
         <v>7</v>
@@ -4781,20 +4781,20 @@
     </row>
     <row r="178" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B178" s="15">
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F178" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G178" s="20">
         <v>0.4</v>
@@ -4802,20 +4802,20 @@
     </row>
     <row r="179" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B179" s="15">
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F179" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G179" s="20">
         <v>0.55000000000000004</v>
@@ -4823,20 +4823,20 @@
     </row>
     <row r="180" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B180" s="15">
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F180" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G180" s="20">
         <v>0.63</v>
@@ -4844,20 +4844,20 @@
     </row>
     <row r="181" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B181" s="15">
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F181" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G181" s="20">
         <v>0.74</v>
@@ -4865,20 +4865,20 @@
     </row>
     <row r="182" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B182" s="15">
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F182" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G182" s="20">
         <v>0.85</v>
@@ -4886,20 +4886,20 @@
     </row>
     <row r="183" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B183" s="15">
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F183" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G183" s="20">
         <v>0.98</v>
@@ -4907,20 +4907,20 @@
     </row>
     <row r="184" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B184" s="15">
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D184" s="15"/>
       <c r="E184" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F184" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G184" s="20">
         <v>1</v>
@@ -4928,18 +4928,18 @@
     </row>
     <row r="185" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B185" s="15">
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D185" s="22"/>
       <c r="E185" s="15"/>
       <c r="F185" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G185" s="23">
         <v>1</v>
@@ -4947,18 +4947,18 @@
     </row>
     <row r="186" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B186" s="15">
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D186" s="22"/>
       <c r="E186" s="15"/>
       <c r="F186" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G186" s="23">
         <v>2</v>
@@ -4966,18 +4966,18 @@
     </row>
     <row r="187" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B187" s="15">
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D187" s="22"/>
       <c r="E187" s="15"/>
       <c r="F187" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G187" s="23">
         <v>2.5</v>
@@ -4985,20 +4985,20 @@
     </row>
     <row r="188" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B188" s="15">
         <v>17</v>
       </c>
       <c r="C188" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D188" s="15"/>
       <c r="E188" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F188" s="22" t="s">
         <v>74</v>
-      </c>
-      <c r="F188" s="22" t="s">
-        <v>75</v>
       </c>
       <c r="G188" s="23">
         <v>1</v>
@@ -5006,20 +5006,20 @@
     </row>
     <row r="189" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B189" s="15">
         <v>17</v>
       </c>
       <c r="C189" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D189" s="15"/>
       <c r="E189" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F189" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G189" s="23">
         <v>1.5</v>
@@ -5027,20 +5027,20 @@
     </row>
     <row r="190" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B190" s="15">
         <v>17</v>
       </c>
       <c r="C190" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D190" s="15"/>
       <c r="E190" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F190" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G190" s="23">
         <v>2</v>

</xml_diff>

<commit_message>
Uploaded 05-May-2021 09:27:05 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -261,12 +261,6 @@
     </r>
   </si>
   <si>
-    <t>$benefit.getName().equals("$param")</t>
-  </si>
-  <si>
-    <t>$benefit.getValue().equals("$param")</t>
-  </si>
-  <si>
     <t>AssumptionUsedByGroupName1</t>
   </si>
   <si>
@@ -822,16 +816,22 @@
     <t>RENAL CARE (DIALYSIS)</t>
   </si>
   <si>
-    <t>$benefit:Benefit()</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
-    <t>$benefit.getBenefit_group().getName().equals("$param")</t>
-  </si>
-  <si>
-    <t>$benefit.getBenefit_group().getCoveredDays()==$param</t>
+    <t>$benefit:Benefit</t>
+  </si>
+  <si>
+    <t>getBenefit_group().getName().equals("$param")</t>
+  </si>
+  <si>
+    <t>getBenefit_group().getCoveredDays()==$param</t>
+  </si>
+  <si>
+    <t>getName().equals("$param")</t>
+  </si>
+  <si>
+    <t>getValue().equals("$param")</t>
   </si>
 </sst>
 </file>
@@ -1391,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1469,7 +1469,7 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -1478,21 +1478,21 @@
       <c r="H4" s="8"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="G5" s="9" t="s">
         <v>266</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>6</v>
@@ -1524,13 +1524,13 @@
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="15">
         <v>17</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>10</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" s="15">
         <v>17</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>10</v>
@@ -1568,13 +1568,13 @@
     </row>
     <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B9" s="15">
         <v>17</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>10</v>
@@ -1590,13 +1590,13 @@
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" s="15">
         <v>17</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>10</v>
@@ -1612,13 +1612,13 @@
     </row>
     <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B11" s="15">
         <v>17</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>10</v>
@@ -1634,13 +1634,13 @@
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" s="15">
         <v>17</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>10</v>
@@ -1656,13 +1656,13 @@
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B13" s="15">
         <v>17</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>10</v>
@@ -1678,13 +1678,13 @@
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14" s="15">
         <v>17</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>10</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B15" s="15">
         <v>17</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>10</v>
@@ -1722,13 +1722,13 @@
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B16" s="15">
         <v>17</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>10</v>
@@ -1744,13 +1744,13 @@
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="15">
         <v>17</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>10</v>
@@ -1766,13 +1766,13 @@
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B18" s="15">
         <v>17</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>10</v>
@@ -1788,13 +1788,13 @@
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B19" s="15">
         <v>17</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>10</v>
@@ -1810,13 +1810,13 @@
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B20" s="15">
         <v>17</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>10</v>
@@ -1832,13 +1832,13 @@
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" s="15">
         <v>17</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>10</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B22" s="15">
         <v>17</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>10</v>
@@ -1876,13 +1876,13 @@
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" s="15">
         <v>17</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>10</v>
@@ -1898,13 +1898,13 @@
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" s="15">
         <v>17</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>10</v>
@@ -1920,13 +1920,13 @@
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B25" s="15">
         <v>17</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>29</v>
@@ -1942,13 +1942,13 @@
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B26" s="15">
         <v>17</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>29</v>
@@ -1964,13 +1964,13 @@
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" s="15">
         <v>17</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>29</v>
@@ -1986,13 +1986,13 @@
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B28" s="15">
         <v>17</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>29</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B29" s="15">
         <v>17</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>29</v>
@@ -2030,13 +2030,13 @@
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B30" s="15">
         <v>17</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>29</v>
@@ -2052,13 +2052,13 @@
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B31" s="15">
         <v>17</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>29</v>
@@ -2074,13 +2074,13 @@
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B32" s="15">
         <v>17</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>29</v>
@@ -2096,13 +2096,13 @@
     </row>
     <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B33" s="15">
         <v>17</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>29</v>
@@ -2118,13 +2118,13 @@
     </row>
     <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B34" s="15">
         <v>17</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>29</v>
@@ -2140,13 +2140,13 @@
     </row>
     <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B35" s="15">
         <v>17</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>29</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B36" s="15">
         <v>17</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>29</v>
@@ -2184,13 +2184,13 @@
     </row>
     <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B37" s="15">
         <v>17</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>29</v>
@@ -2206,13 +2206,13 @@
     </row>
     <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B38" s="15">
         <v>17</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>29</v>
@@ -2228,13 +2228,13 @@
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B39" s="15">
         <v>17</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>29</v>
@@ -2250,13 +2250,13 @@
     </row>
     <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B40" s="15">
         <v>17</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>29</v>
@@ -2272,13 +2272,13 @@
     </row>
     <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B41" s="15">
         <v>17</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>29</v>
@@ -2294,13 +2294,13 @@
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B42" s="15">
         <v>17</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>29</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B43" s="15">
         <v>17</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>30</v>
@@ -2338,13 +2338,13 @@
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B44" s="15">
         <v>17</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>30</v>
@@ -2360,13 +2360,13 @@
     </row>
     <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B45" s="15">
         <v>17</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>30</v>
@@ -2382,13 +2382,13 @@
     </row>
     <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B46" s="15">
         <v>17</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>30</v>
@@ -2404,13 +2404,13 @@
     </row>
     <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B47" s="15">
         <v>17</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D47" s="15" t="s">
         <v>30</v>
@@ -2426,13 +2426,13 @@
     </row>
     <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B48" s="15">
         <v>17</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>30</v>
@@ -2448,13 +2448,13 @@
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B49" s="15">
         <v>17</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>30</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B50" s="15">
         <v>17</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>30</v>
@@ -2492,13 +2492,13 @@
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B51" s="15">
         <v>17</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>30</v>
@@ -2514,13 +2514,13 @@
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B52" s="15">
         <v>17</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>30</v>
@@ -2536,13 +2536,13 @@
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B53" s="15">
         <v>17</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>30</v>
@@ -2558,13 +2558,13 @@
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B54" s="15">
         <v>17</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>30</v>
@@ -2580,13 +2580,13 @@
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B55" s="15">
         <v>17</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>30</v>
@@ -2602,13 +2602,13 @@
     </row>
     <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B56" s="15">
         <v>17</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>30</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B57" s="15">
         <v>17</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>30</v>
@@ -2646,13 +2646,13 @@
     </row>
     <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B58" s="15">
         <v>17</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D58" s="15" t="s">
         <v>30</v>
@@ -2668,13 +2668,13 @@
     </row>
     <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B59" s="15">
         <v>17</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>30</v>
@@ -2690,13 +2690,13 @@
     </row>
     <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B60" s="15">
         <v>17</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D60" s="15" t="s">
         <v>30</v>
@@ -2712,13 +2712,13 @@
     </row>
     <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B61" s="15">
         <v>17</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>31</v>
@@ -2734,13 +2734,13 @@
     </row>
     <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B62" s="15">
         <v>17</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D62" s="15" t="s">
         <v>31</v>
@@ -2756,13 +2756,13 @@
     </row>
     <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B63" s="15">
         <v>17</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D63" s="15" t="s">
         <v>31</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B64" s="15">
         <v>17</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>31</v>
@@ -2800,13 +2800,13 @@
     </row>
     <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B65" s="15">
         <v>17</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D65" s="15" t="s">
         <v>31</v>
@@ -2822,13 +2822,13 @@
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B66" s="15">
         <v>17</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D66" s="15" t="s">
         <v>31</v>
@@ -2844,13 +2844,13 @@
     </row>
     <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B67" s="15">
         <v>17</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D67" s="15" t="s">
         <v>31</v>
@@ -2866,13 +2866,13 @@
     </row>
     <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B68" s="15">
         <v>17</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D68" s="15" t="s">
         <v>31</v>
@@ -2888,13 +2888,13 @@
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B69" s="15">
         <v>17</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D69" s="15" t="s">
         <v>31</v>
@@ -2910,13 +2910,13 @@
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B70" s="15">
         <v>17</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D70" s="15" t="s">
         <v>31</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B71" s="15">
         <v>17</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D71" s="15" t="s">
         <v>31</v>
@@ -2954,13 +2954,13 @@
     </row>
     <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B72" s="15">
         <v>17</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D72" s="15" t="s">
         <v>31</v>
@@ -2976,13 +2976,13 @@
     </row>
     <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B73" s="15">
         <v>17</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>31</v>
@@ -2998,13 +2998,13 @@
     </row>
     <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B74" s="15">
         <v>17</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D74" s="15" t="s">
         <v>31</v>
@@ -3020,13 +3020,13 @@
     </row>
     <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B75" s="15">
         <v>17</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D75" s="15" t="s">
         <v>31</v>
@@ -3042,13 +3042,13 @@
     </row>
     <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B76" s="15">
         <v>17</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D76" s="15" t="s">
         <v>31</v>
@@ -3064,13 +3064,13 @@
     </row>
     <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B77" s="15">
         <v>17</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>31</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B78" s="15">
         <v>17</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D78" s="15" t="s">
         <v>31</v>
@@ -3108,16 +3108,16 @@
     </row>
     <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B79" s="15">
         <v>17</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E79" s="21"/>
       <c r="F79" s="21"/>
@@ -3130,16 +3130,16 @@
     </row>
     <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B80" s="15">
         <v>17</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E80" s="21"/>
       <c r="F80" s="21"/>
@@ -3152,16 +3152,16 @@
     </row>
     <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B81" s="15">
         <v>17</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D81" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E81" s="21"/>
       <c r="F81" s="21"/>
@@ -3174,16 +3174,16 @@
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B82" s="15">
         <v>17</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E82" s="21"/>
       <c r="F82" s="21"/>
@@ -3196,16 +3196,16 @@
     </row>
     <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B83" s="15">
         <v>17</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E83" s="21"/>
       <c r="F83" s="21"/>
@@ -3218,16 +3218,16 @@
     </row>
     <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B84" s="15">
         <v>17</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E84" s="21"/>
       <c r="F84" s="21"/>
@@ -3240,16 +3240,16 @@
     </row>
     <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B85" s="15">
         <v>17</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D85" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E85" s="21"/>
       <c r="F85" s="21"/>
@@ -3262,16 +3262,16 @@
     </row>
     <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B86" s="15">
         <v>17</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D86" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E86" s="21"/>
       <c r="F86" s="21"/>
@@ -3284,16 +3284,16 @@
     </row>
     <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B87" s="15">
         <v>17</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D87" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E87" s="21"/>
       <c r="F87" s="21"/>
@@ -3306,16 +3306,16 @@
     </row>
     <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B88" s="15">
         <v>17</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E88" s="21"/>
       <c r="F88" s="21"/>
@@ -3328,16 +3328,16 @@
     </row>
     <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B89" s="15">
         <v>17</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D89" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E89" s="21"/>
       <c r="F89" s="21"/>
@@ -3350,16 +3350,16 @@
     </row>
     <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B90" s="15">
         <v>17</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D90" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E90" s="21"/>
       <c r="F90" s="21"/>
@@ -3372,16 +3372,16 @@
     </row>
     <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B91" s="15">
         <v>17</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D91" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E91" s="21"/>
       <c r="F91" s="21"/>
@@ -3394,16 +3394,16 @@
     </row>
     <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B92" s="15">
         <v>17</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D92" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E92" s="21"/>
       <c r="F92" s="21"/>
@@ -3416,16 +3416,16 @@
     </row>
     <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B93" s="15">
         <v>17</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E93" s="21"/>
       <c r="F93" s="21"/>
@@ -3438,16 +3438,16 @@
     </row>
     <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B94" s="15">
         <v>17</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E94" s="21"/>
       <c r="F94" s="21"/>
@@ -3460,16 +3460,16 @@
     </row>
     <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B95" s="15">
         <v>17</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E95" s="21"/>
       <c r="F95" s="21"/>
@@ -3482,16 +3482,16 @@
     </row>
     <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B96" s="15">
         <v>17</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E96" s="21"/>
       <c r="F96" s="21"/>
@@ -3504,13 +3504,13 @@
     </row>
     <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B97" s="15">
         <v>17</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>32</v>
@@ -3526,13 +3526,13 @@
     </row>
     <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B98" s="15">
         <v>17</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>32</v>
@@ -3548,13 +3548,13 @@
     </row>
     <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B99" s="15">
         <v>17</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D99" s="15" t="s">
         <v>32</v>
@@ -3570,13 +3570,13 @@
     </row>
     <row r="100" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B100" s="15">
         <v>17</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D100" s="15" t="s">
         <v>32</v>
@@ -3592,13 +3592,13 @@
     </row>
     <row r="101" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B101" s="15">
         <v>17</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D101" s="15" t="s">
         <v>32</v>
@@ -3614,13 +3614,13 @@
     </row>
     <row r="102" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B102" s="15">
         <v>17</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D102" s="15" t="s">
         <v>32</v>
@@ -3636,13 +3636,13 @@
     </row>
     <row r="103" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B103" s="15">
         <v>17</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D103" s="15" t="s">
         <v>32</v>
@@ -3658,13 +3658,13 @@
     </row>
     <row r="104" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B104" s="15">
         <v>17</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D104" s="15" t="s">
         <v>32</v>
@@ -3680,13 +3680,13 @@
     </row>
     <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B105" s="15">
         <v>17</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D105" s="15" t="s">
         <v>32</v>
@@ -3702,13 +3702,13 @@
     </row>
     <row r="106" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B106" s="15">
         <v>17</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D106" s="15" t="s">
         <v>32</v>
@@ -3724,13 +3724,13 @@
     </row>
     <row r="107" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B107" s="15">
         <v>17</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D107" s="15" t="s">
         <v>32</v>
@@ -3746,13 +3746,13 @@
     </row>
     <row r="108" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B108" s="15">
         <v>17</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D108" s="15" t="s">
         <v>32</v>
@@ -3768,13 +3768,13 @@
     </row>
     <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B109" s="15">
         <v>17</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D109" s="15" t="s">
         <v>32</v>
@@ -3790,13 +3790,13 @@
     </row>
     <row r="110" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B110" s="15">
         <v>17</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D110" s="15" t="s">
         <v>32</v>
@@ -3812,13 +3812,13 @@
     </row>
     <row r="111" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B111" s="15">
         <v>17</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D111" s="15" t="s">
         <v>32</v>
@@ -3834,13 +3834,13 @@
     </row>
     <row r="112" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B112" s="15">
         <v>17</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D112" s="15" t="s">
         <v>32</v>
@@ -3856,13 +3856,13 @@
     </row>
     <row r="113" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B113" s="15">
         <v>17</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D113" s="15" t="s">
         <v>32</v>
@@ -3878,13 +3878,13 @@
     </row>
     <row r="114" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B114" s="15">
         <v>17</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>32</v>
@@ -3900,13 +3900,13 @@
     </row>
     <row r="115" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B115" s="15">
         <v>17</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D115" s="15" t="s">
         <v>32</v>
@@ -3922,13 +3922,13 @@
     </row>
     <row r="116" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B116" s="15">
         <v>17</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D116" s="15" t="s">
         <v>32</v>
@@ -3944,13 +3944,13 @@
     </row>
     <row r="117" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B117" s="15">
         <v>17</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D117" s="15" t="s">
         <v>32</v>
@@ -3966,13 +3966,13 @@
     </row>
     <row r="118" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B118" s="15">
         <v>17</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D118" s="15" t="s">
         <v>32</v>
@@ -3988,13 +3988,13 @@
     </row>
     <row r="119" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B119" s="15">
         <v>17</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D119" s="15" t="s">
         <v>32</v>
@@ -4010,13 +4010,13 @@
     </row>
     <row r="120" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B120" s="15">
         <v>17</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D120" s="15" t="s">
         <v>32</v>
@@ -4032,13 +4032,13 @@
     </row>
     <row r="121" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B121" s="15">
         <v>17</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D121" s="15" t="s">
         <v>32</v>
@@ -4054,13 +4054,13 @@
     </row>
     <row r="122" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B122" s="15">
         <v>17</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D122" s="15" t="s">
         <v>32</v>
@@ -4076,13 +4076,13 @@
     </row>
     <row r="123" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B123" s="15">
         <v>17</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D123" s="15" t="s">
         <v>32</v>
@@ -4098,13 +4098,13 @@
     </row>
     <row r="124" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B124" s="15">
         <v>17</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D124" s="15" t="s">
         <v>32</v>
@@ -4120,13 +4120,13 @@
     </row>
     <row r="125" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B125" s="15">
         <v>17</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D125" s="15" t="s">
         <v>32</v>
@@ -4142,13 +4142,13 @@
     </row>
     <row r="126" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B126" s="15">
         <v>17</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D126" s="15" t="s">
         <v>32</v>
@@ -4164,13 +4164,13 @@
     </row>
     <row r="127" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B127" s="15">
         <v>17</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D127" s="15" t="s">
         <v>32</v>
@@ -4186,13 +4186,13 @@
     </row>
     <row r="128" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B128" s="15">
         <v>17</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D128" s="15" t="s">
         <v>44</v>
@@ -4208,13 +4208,13 @@
     </row>
     <row r="129" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B129" s="15">
         <v>17</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D129" s="15" t="s">
         <v>44</v>
@@ -4230,13 +4230,13 @@
     </row>
     <row r="130" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B130" s="15">
         <v>17</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D130" s="15" t="s">
         <v>44</v>
@@ -4252,13 +4252,13 @@
     </row>
     <row r="131" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B131" s="15">
         <v>17</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D131" s="15" t="s">
         <v>44</v>
@@ -4274,13 +4274,13 @@
     </row>
     <row r="132" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B132" s="15">
         <v>17</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D132" s="15" t="s">
         <v>44</v>
@@ -4296,13 +4296,13 @@
     </row>
     <row r="133" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B133" s="15">
         <v>17</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D133" s="15" t="s">
         <v>44</v>
@@ -4318,13 +4318,13 @@
     </row>
     <row r="134" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B134" s="15">
         <v>17</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D134" s="15" t="s">
         <v>44</v>
@@ -4340,13 +4340,13 @@
     </row>
     <row r="135" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B135" s="15">
         <v>17</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D135" s="15" t="s">
         <v>44</v>
@@ -4362,13 +4362,13 @@
     </row>
     <row r="136" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B136" s="15">
         <v>17</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D136" s="15" t="s">
         <v>44</v>
@@ -4384,13 +4384,13 @@
     </row>
     <row r="137" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B137" s="15">
         <v>17</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D137" s="15" t="s">
         <v>44</v>
@@ -4406,13 +4406,13 @@
     </row>
     <row r="138" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B138" s="15">
         <v>17</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D138" s="15" t="s">
         <v>44</v>
@@ -4428,13 +4428,13 @@
     </row>
     <row r="139" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B139" s="15">
         <v>17</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D139" s="15" t="s">
         <v>44</v>
@@ -4450,13 +4450,13 @@
     </row>
     <row r="140" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B140" s="15">
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D140" s="15" t="s">
         <v>45</v>
@@ -4472,13 +4472,13 @@
     </row>
     <row r="141" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B141" s="15">
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D141" s="15" t="s">
         <v>45</v>
@@ -4494,13 +4494,13 @@
     </row>
     <row r="142" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B142" s="15">
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D142" s="15" t="s">
         <v>45</v>
@@ -4516,13 +4516,13 @@
     </row>
     <row r="143" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B143" s="15">
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D143" s="15" t="s">
         <v>45</v>
@@ -4538,13 +4538,13 @@
     </row>
     <row r="144" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B144" s="15">
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D144" s="15" t="s">
         <v>45</v>
@@ -4560,13 +4560,13 @@
     </row>
     <row r="145" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B145" s="15">
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D145" s="15" t="s">
         <v>45</v>
@@ -4582,13 +4582,13 @@
     </row>
     <row r="146" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B146" s="15">
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D146" s="15" t="s">
         <v>45</v>
@@ -4604,13 +4604,13 @@
     </row>
     <row r="147" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B147" s="15">
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D147" s="15" t="s">
         <v>45</v>
@@ -4626,13 +4626,13 @@
     </row>
     <row r="148" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B148" s="15">
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D148" s="15" t="s">
         <v>45</v>
@@ -4648,13 +4648,13 @@
     </row>
     <row r="149" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B149" s="15">
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D149" s="15" t="s">
         <v>45</v>
@@ -4670,13 +4670,13 @@
     </row>
     <row r="150" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B150" s="15">
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D150" s="15" t="s">
         <v>45</v>
@@ -4692,13 +4692,13 @@
     </row>
     <row r="151" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B151" s="15">
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D151" s="15" t="s">
         <v>45</v>
@@ -4714,13 +4714,13 @@
     </row>
     <row r="152" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B152" s="15">
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D152" s="15" t="s">
         <v>46</v>
@@ -4736,13 +4736,13 @@
     </row>
     <row r="153" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B153" s="15">
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D153" s="15" t="s">
         <v>46</v>
@@ -4758,13 +4758,13 @@
     </row>
     <row r="154" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B154" s="15">
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D154" s="15" t="s">
         <v>46</v>
@@ -4780,13 +4780,13 @@
     </row>
     <row r="155" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B155" s="15">
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D155" s="15" t="s">
         <v>46</v>
@@ -4802,13 +4802,13 @@
     </row>
     <row r="156" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B156" s="15">
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D156" s="15" t="s">
         <v>46</v>
@@ -4824,13 +4824,13 @@
     </row>
     <row r="157" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B157" s="15">
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D157" s="15" t="s">
         <v>46</v>
@@ -4846,13 +4846,13 @@
     </row>
     <row r="158" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B158" s="15">
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D158" s="15" t="s">
         <v>46</v>
@@ -4868,13 +4868,13 @@
     </row>
     <row r="159" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B159" s="15">
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D159" s="15" t="s">
         <v>46</v>
@@ -4890,13 +4890,13 @@
     </row>
     <row r="160" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B160" s="15">
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D160" s="15" t="s">
         <v>46</v>
@@ -4912,13 +4912,13 @@
     </row>
     <row r="161" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B161" s="15">
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D161" s="15" t="s">
         <v>46</v>
@@ -4934,13 +4934,13 @@
     </row>
     <row r="162" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B162" s="15">
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D162" s="15" t="s">
         <v>46</v>
@@ -4956,13 +4956,13 @@
     </row>
     <row r="163" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B163" s="15">
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D163" s="15" t="s">
         <v>46</v>
@@ -4978,13 +4978,13 @@
     </row>
     <row r="164" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B164" s="15">
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D164" s="15" t="s">
         <v>47</v>
@@ -5000,13 +5000,13 @@
     </row>
     <row r="165" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B165" s="15">
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D165" s="15" t="s">
         <v>47</v>
@@ -5022,13 +5022,13 @@
     </row>
     <row r="166" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B166" s="15">
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D166" s="15" t="s">
         <v>47</v>
@@ -5044,13 +5044,13 @@
     </row>
     <row r="167" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B167" s="15">
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D167" s="15" t="s">
         <v>47</v>
@@ -5066,13 +5066,13 @@
     </row>
     <row r="168" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B168" s="15">
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D168" s="15" t="s">
         <v>47</v>
@@ -5088,13 +5088,13 @@
     </row>
     <row r="169" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B169" s="15">
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D169" s="15" t="s">
         <v>47</v>
@@ -5110,13 +5110,13 @@
     </row>
     <row r="170" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B170" s="15">
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D170" s="15" t="s">
         <v>47</v>
@@ -5132,13 +5132,13 @@
     </row>
     <row r="171" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B171" s="15">
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D171" s="15" t="s">
         <v>55</v>
@@ -5156,13 +5156,13 @@
     </row>
     <row r="172" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B172" s="15">
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D172" s="15" t="s">
         <v>55</v>
@@ -5180,13 +5180,13 @@
     </row>
     <row r="173" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B173" s="15">
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D173" s="15" t="s">
         <v>55</v>
@@ -5204,13 +5204,13 @@
     </row>
     <row r="174" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B174" s="15">
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D174" s="15" t="s">
         <v>55</v>
@@ -5228,13 +5228,13 @@
     </row>
     <row r="175" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B175" s="15">
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D175" s="15" t="s">
         <v>55</v>
@@ -5252,13 +5252,13 @@
     </row>
     <row r="176" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B176" s="15">
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D176" s="15" t="s">
         <v>55</v>
@@ -5276,13 +5276,13 @@
     </row>
     <row r="177" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B177" s="15">
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D177" s="15" t="s">
         <v>55</v>
@@ -5300,13 +5300,13 @@
     </row>
     <row r="178" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B178" s="15">
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D178" s="15" t="s">
         <v>55</v>
@@ -5324,13 +5324,13 @@
     </row>
     <row r="179" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B179" s="15">
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D179" s="15" t="s">
         <v>55</v>
@@ -5348,13 +5348,13 @@
     </row>
     <row r="180" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B180" s="15">
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D180" s="15" t="s">
         <v>55</v>
@@ -5372,13 +5372,13 @@
     </row>
     <row r="181" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B181" s="15">
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D181" s="15" t="s">
         <v>55</v>
@@ -5396,13 +5396,13 @@
     </row>
     <row r="182" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B182" s="15">
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D182" s="15" t="s">
         <v>55</v>
@@ -5420,13 +5420,13 @@
     </row>
     <row r="183" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B183" s="15">
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D183" s="15" t="s">
         <v>55</v>
@@ -5444,13 +5444,13 @@
     </row>
     <row r="184" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B184" s="15">
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D184" s="15" t="s">
         <v>55</v>
@@ -5468,13 +5468,13 @@
     </row>
     <row r="185" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B185" s="15">
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D185" s="15" t="s">
         <v>65</v>
@@ -5490,13 +5490,13 @@
     </row>
     <row r="186" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B186" s="15">
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D186" s="15" t="s">
         <v>65</v>
@@ -5512,13 +5512,13 @@
     </row>
     <row r="187" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B187" s="15">
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D187" s="15" t="s">
         <v>65</v>
@@ -5534,13 +5534,13 @@
     </row>
     <row r="188" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B188" s="15">
         <v>17</v>
       </c>
       <c r="C188" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D188" s="15" t="s">
         <v>32</v>
@@ -5558,13 +5558,13 @@
     </row>
     <row r="189" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B189" s="15">
         <v>17</v>
       </c>
       <c r="C189" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D189" s="15" t="s">
         <v>32</v>
@@ -5582,13 +5582,13 @@
     </row>
     <row r="190" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B190" s="15">
         <v>17</v>
       </c>
       <c r="C190" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D190" s="15" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Uploaded 05-May-2021 09:32:00 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:L1118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1481,7 +1481,10 @@
     <row r="5" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7" t="str">
+        <f>D5&amp;E5</f>
+        <v>getBenefit_group().getName().equals("$param")getBenefit_group().getCoveredDays()==$param</v>
+      </c>
       <c r="D5" s="7" t="s">
         <v>263</v>
       </c>

</xml_diff>

<commit_message>
Uploaded 05-May-2021 10:13:40 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="267">
   <si>
     <t>RuleSet</t>
   </si>
@@ -1392,14 +1392,14 @@
   <dimension ref="A1:L1118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.42578125" style="17"/>
     <col min="2" max="2" width="10.5703125" style="17"/>
-    <col min="3" max="3" width="9.140625" style="17"/>
+    <col min="3" max="3" width="12.140625" style="17" customWidth="1"/>
     <col min="4" max="5" width="41" style="17" customWidth="1"/>
     <col min="6" max="6" width="36.140625" style="17" customWidth="1"/>
     <col min="7" max="7" width="25.140625" style="17" customWidth="1"/>
@@ -1445,7 +1445,9 @@
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Uploaded 05-May-2021 10:22:44 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -261,6 +261,12 @@
     </r>
   </si>
   <si>
+    <t>$benefit.getName().equals("$param")</t>
+  </si>
+  <si>
+    <t>$benefit.getValue().equals("$param")</t>
+  </si>
+  <si>
     <t>AssumptionUsedByGroupName1</t>
   </si>
   <si>
@@ -819,19 +825,13 @@
     <t>true</t>
   </si>
   <si>
+    <t>$benefit.getBenefit_group().getName().equals("$param")</t>
+  </si>
+  <si>
+    <t>$benefit.getBenefit_group().getCoveredDays()==$param</t>
+  </si>
+  <si>
     <t>$benefit:Benefit</t>
-  </si>
-  <si>
-    <t>getBenefit_group().getName().equals("$param")</t>
-  </si>
-  <si>
-    <t>getBenefit_group().getCoveredDays()==$param</t>
-  </si>
-  <si>
-    <t>getName().equals("$param")</t>
-  </si>
-  <si>
-    <t>getValue().equals("$param")</t>
   </si>
 </sst>
 </file>
@@ -1391,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1469,7 +1469,7 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -1478,21 +1478,21 @@
       <c r="H4" s="8"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>265</v>
+        <v>76</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>266</v>
+        <v>77</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>6</v>
@@ -1524,13 +1524,13 @@
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B7" s="15">
         <v>17</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>10</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B8" s="15">
         <v>17</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>10</v>
@@ -1568,13 +1568,13 @@
     </row>
     <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B9" s="15">
         <v>17</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>10</v>
@@ -1590,13 +1590,13 @@
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B10" s="15">
         <v>17</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>10</v>
@@ -1612,13 +1612,13 @@
     </row>
     <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B11" s="15">
         <v>17</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>10</v>
@@ -1634,13 +1634,13 @@
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B12" s="15">
         <v>17</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>10</v>
@@ -1656,13 +1656,13 @@
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B13" s="15">
         <v>17</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>10</v>
@@ -1678,13 +1678,13 @@
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B14" s="15">
         <v>17</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>10</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B15" s="15">
         <v>17</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>10</v>
@@ -1722,13 +1722,13 @@
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B16" s="15">
         <v>17</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>10</v>
@@ -1744,13 +1744,13 @@
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B17" s="15">
         <v>17</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>10</v>
@@ -1766,13 +1766,13 @@
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B18" s="15">
         <v>17</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>10</v>
@@ -1788,13 +1788,13 @@
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B19" s="15">
         <v>17</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>10</v>
@@ -1810,13 +1810,13 @@
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B20" s="15">
         <v>17</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>10</v>
@@ -1832,13 +1832,13 @@
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B21" s="15">
         <v>17</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>10</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B22" s="15">
         <v>17</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>10</v>
@@ -1876,13 +1876,13 @@
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B23" s="15">
         <v>17</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>10</v>
@@ -1898,13 +1898,13 @@
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B24" s="15">
         <v>17</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>10</v>
@@ -1920,13 +1920,13 @@
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B25" s="15">
         <v>17</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>29</v>
@@ -1942,13 +1942,13 @@
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B26" s="15">
         <v>17</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>29</v>
@@ -1964,13 +1964,13 @@
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B27" s="15">
         <v>17</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>29</v>
@@ -1986,13 +1986,13 @@
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B28" s="15">
         <v>17</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>29</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B29" s="15">
         <v>17</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>29</v>
@@ -2030,13 +2030,13 @@
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B30" s="15">
         <v>17</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>29</v>
@@ -2052,13 +2052,13 @@
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B31" s="15">
         <v>17</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>29</v>
@@ -2074,13 +2074,13 @@
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B32" s="15">
         <v>17</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>29</v>
@@ -2096,13 +2096,13 @@
     </row>
     <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B33" s="15">
         <v>17</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>29</v>
@@ -2118,13 +2118,13 @@
     </row>
     <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B34" s="15">
         <v>17</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>29</v>
@@ -2140,13 +2140,13 @@
     </row>
     <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B35" s="15">
         <v>17</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>29</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B36" s="15">
         <v>17</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>29</v>
@@ -2184,13 +2184,13 @@
     </row>
     <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B37" s="15">
         <v>17</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>29</v>
@@ -2206,13 +2206,13 @@
     </row>
     <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B38" s="15">
         <v>17</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>29</v>
@@ -2228,13 +2228,13 @@
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B39" s="15">
         <v>17</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>29</v>
@@ -2250,13 +2250,13 @@
     </row>
     <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B40" s="15">
         <v>17</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>29</v>
@@ -2272,13 +2272,13 @@
     </row>
     <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B41" s="15">
         <v>17</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>29</v>
@@ -2294,13 +2294,13 @@
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B42" s="15">
         <v>17</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>29</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B43" s="15">
         <v>17</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>30</v>
@@ -2338,13 +2338,13 @@
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B44" s="15">
         <v>17</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>30</v>
@@ -2360,13 +2360,13 @@
     </row>
     <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B45" s="15">
         <v>17</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>30</v>
@@ -2382,13 +2382,13 @@
     </row>
     <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B46" s="15">
         <v>17</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>30</v>
@@ -2404,13 +2404,13 @@
     </row>
     <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B47" s="15">
         <v>17</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D47" s="15" t="s">
         <v>30</v>
@@ -2426,13 +2426,13 @@
     </row>
     <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B48" s="15">
         <v>17</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>30</v>
@@ -2448,13 +2448,13 @@
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B49" s="15">
         <v>17</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>30</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B50" s="15">
         <v>17</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>30</v>
@@ -2492,13 +2492,13 @@
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B51" s="15">
         <v>17</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>30</v>
@@ -2514,13 +2514,13 @@
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B52" s="15">
         <v>17</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>30</v>
@@ -2536,13 +2536,13 @@
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B53" s="15">
         <v>17</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>30</v>
@@ -2558,13 +2558,13 @@
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B54" s="15">
         <v>17</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>30</v>
@@ -2580,13 +2580,13 @@
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B55" s="15">
         <v>17</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>30</v>
@@ -2602,13 +2602,13 @@
     </row>
     <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B56" s="15">
         <v>17</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>30</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B57" s="15">
         <v>17</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>30</v>
@@ -2646,13 +2646,13 @@
     </row>
     <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B58" s="15">
         <v>17</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D58" s="15" t="s">
         <v>30</v>
@@ -2668,13 +2668,13 @@
     </row>
     <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B59" s="15">
         <v>17</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>30</v>
@@ -2690,13 +2690,13 @@
     </row>
     <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B60" s="15">
         <v>17</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D60" s="15" t="s">
         <v>30</v>
@@ -2712,13 +2712,13 @@
     </row>
     <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B61" s="15">
         <v>17</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>31</v>
@@ -2734,13 +2734,13 @@
     </row>
     <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B62" s="15">
         <v>17</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D62" s="15" t="s">
         <v>31</v>
@@ -2756,13 +2756,13 @@
     </row>
     <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B63" s="15">
         <v>17</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D63" s="15" t="s">
         <v>31</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B64" s="15">
         <v>17</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>31</v>
@@ -2800,13 +2800,13 @@
     </row>
     <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B65" s="15">
         <v>17</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D65" s="15" t="s">
         <v>31</v>
@@ -2822,13 +2822,13 @@
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B66" s="15">
         <v>17</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D66" s="15" t="s">
         <v>31</v>
@@ -2844,13 +2844,13 @@
     </row>
     <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B67" s="15">
         <v>17</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D67" s="15" t="s">
         <v>31</v>
@@ -2866,13 +2866,13 @@
     </row>
     <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B68" s="15">
         <v>17</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D68" s="15" t="s">
         <v>31</v>
@@ -2888,13 +2888,13 @@
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B69" s="15">
         <v>17</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D69" s="15" t="s">
         <v>31</v>
@@ -2910,13 +2910,13 @@
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B70" s="15">
         <v>17</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D70" s="15" t="s">
         <v>31</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B71" s="15">
         <v>17</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D71" s="15" t="s">
         <v>31</v>
@@ -2954,13 +2954,13 @@
     </row>
     <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B72" s="15">
         <v>17</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D72" s="15" t="s">
         <v>31</v>
@@ -2976,13 +2976,13 @@
     </row>
     <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B73" s="15">
         <v>17</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>31</v>
@@ -2998,13 +2998,13 @@
     </row>
     <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B74" s="15">
         <v>17</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D74" s="15" t="s">
         <v>31</v>
@@ -3020,13 +3020,13 @@
     </row>
     <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B75" s="15">
         <v>17</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D75" s="15" t="s">
         <v>31</v>
@@ -3042,13 +3042,13 @@
     </row>
     <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B76" s="15">
         <v>17</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D76" s="15" t="s">
         <v>31</v>
@@ -3064,13 +3064,13 @@
     </row>
     <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B77" s="15">
         <v>17</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>31</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B78" s="15">
         <v>17</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D78" s="15" t="s">
         <v>31</v>
@@ -3108,16 +3108,16 @@
     </row>
     <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B79" s="15">
         <v>17</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E79" s="21"/>
       <c r="F79" s="21"/>
@@ -3130,16 +3130,16 @@
     </row>
     <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B80" s="15">
         <v>17</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E80" s="21"/>
       <c r="F80" s="21"/>
@@ -3152,16 +3152,16 @@
     </row>
     <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B81" s="15">
         <v>17</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D81" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E81" s="21"/>
       <c r="F81" s="21"/>
@@ -3174,16 +3174,16 @@
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B82" s="15">
         <v>17</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E82" s="21"/>
       <c r="F82" s="21"/>
@@ -3196,16 +3196,16 @@
     </row>
     <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B83" s="15">
         <v>17</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E83" s="21"/>
       <c r="F83" s="21"/>
@@ -3218,16 +3218,16 @@
     </row>
     <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B84" s="15">
         <v>17</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E84" s="21"/>
       <c r="F84" s="21"/>
@@ -3240,16 +3240,16 @@
     </row>
     <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B85" s="15">
         <v>17</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D85" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E85" s="21"/>
       <c r="F85" s="21"/>
@@ -3262,16 +3262,16 @@
     </row>
     <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B86" s="15">
         <v>17</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D86" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E86" s="21"/>
       <c r="F86" s="21"/>
@@ -3284,16 +3284,16 @@
     </row>
     <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B87" s="15">
         <v>17</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D87" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E87" s="21"/>
       <c r="F87" s="21"/>
@@ -3306,16 +3306,16 @@
     </row>
     <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B88" s="15">
         <v>17</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E88" s="21"/>
       <c r="F88" s="21"/>
@@ -3328,16 +3328,16 @@
     </row>
     <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B89" s="15">
         <v>17</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D89" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E89" s="21"/>
       <c r="F89" s="21"/>
@@ -3350,16 +3350,16 @@
     </row>
     <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B90" s="15">
         <v>17</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D90" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E90" s="21"/>
       <c r="F90" s="21"/>
@@ -3372,16 +3372,16 @@
     </row>
     <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B91" s="15">
         <v>17</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D91" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E91" s="21"/>
       <c r="F91" s="21"/>
@@ -3394,16 +3394,16 @@
     </row>
     <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B92" s="15">
         <v>17</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D92" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E92" s="21"/>
       <c r="F92" s="21"/>
@@ -3416,16 +3416,16 @@
     </row>
     <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B93" s="15">
         <v>17</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E93" s="21"/>
       <c r="F93" s="21"/>
@@ -3438,16 +3438,16 @@
     </row>
     <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B94" s="15">
         <v>17</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E94" s="21"/>
       <c r="F94" s="21"/>
@@ -3460,16 +3460,16 @@
     </row>
     <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B95" s="15">
         <v>17</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E95" s="21"/>
       <c r="F95" s="21"/>
@@ -3482,16 +3482,16 @@
     </row>
     <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B96" s="15">
         <v>17</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E96" s="21"/>
       <c r="F96" s="21"/>
@@ -3504,13 +3504,13 @@
     </row>
     <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B97" s="15">
         <v>17</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>32</v>
@@ -3526,13 +3526,13 @@
     </row>
     <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B98" s="15">
         <v>17</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>32</v>
@@ -3548,13 +3548,13 @@
     </row>
     <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B99" s="15">
         <v>17</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D99" s="15" t="s">
         <v>32</v>
@@ -3570,13 +3570,13 @@
     </row>
     <row r="100" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B100" s="15">
         <v>17</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D100" s="15" t="s">
         <v>32</v>
@@ -3592,13 +3592,13 @@
     </row>
     <row r="101" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B101" s="15">
         <v>17</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D101" s="15" t="s">
         <v>32</v>
@@ -3614,13 +3614,13 @@
     </row>
     <row r="102" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B102" s="15">
         <v>17</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D102" s="15" t="s">
         <v>32</v>
@@ -3636,13 +3636,13 @@
     </row>
     <row r="103" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B103" s="15">
         <v>17</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D103" s="15" t="s">
         <v>32</v>
@@ -3658,13 +3658,13 @@
     </row>
     <row r="104" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B104" s="15">
         <v>17</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D104" s="15" t="s">
         <v>32</v>
@@ -3680,13 +3680,13 @@
     </row>
     <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B105" s="15">
         <v>17</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D105" s="15" t="s">
         <v>32</v>
@@ -3702,13 +3702,13 @@
     </row>
     <row r="106" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B106" s="15">
         <v>17</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D106" s="15" t="s">
         <v>32</v>
@@ -3724,13 +3724,13 @@
     </row>
     <row r="107" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B107" s="15">
         <v>17</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D107" s="15" t="s">
         <v>32</v>
@@ -3746,13 +3746,13 @@
     </row>
     <row r="108" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B108" s="15">
         <v>17</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D108" s="15" t="s">
         <v>32</v>
@@ -3768,13 +3768,13 @@
     </row>
     <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B109" s="15">
         <v>17</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D109" s="15" t="s">
         <v>32</v>
@@ -3790,13 +3790,13 @@
     </row>
     <row r="110" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B110" s="15">
         <v>17</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D110" s="15" t="s">
         <v>32</v>
@@ -3812,13 +3812,13 @@
     </row>
     <row r="111" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B111" s="15">
         <v>17</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D111" s="15" t="s">
         <v>32</v>
@@ -3834,13 +3834,13 @@
     </row>
     <row r="112" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B112" s="15">
         <v>17</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D112" s="15" t="s">
         <v>32</v>
@@ -3856,13 +3856,13 @@
     </row>
     <row r="113" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B113" s="15">
         <v>17</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D113" s="15" t="s">
         <v>32</v>
@@ -3878,13 +3878,13 @@
     </row>
     <row r="114" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B114" s="15">
         <v>17</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>32</v>
@@ -3900,13 +3900,13 @@
     </row>
     <row r="115" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B115" s="15">
         <v>17</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D115" s="15" t="s">
         <v>32</v>
@@ -3922,13 +3922,13 @@
     </row>
     <row r="116" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B116" s="15">
         <v>17</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D116" s="15" t="s">
         <v>32</v>
@@ -3944,13 +3944,13 @@
     </row>
     <row r="117" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B117" s="15">
         <v>17</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D117" s="15" t="s">
         <v>32</v>
@@ -3966,13 +3966,13 @@
     </row>
     <row r="118" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B118" s="15">
         <v>17</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D118" s="15" t="s">
         <v>32</v>
@@ -3988,13 +3988,13 @@
     </row>
     <row r="119" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B119" s="15">
         <v>17</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D119" s="15" t="s">
         <v>32</v>
@@ -4010,13 +4010,13 @@
     </row>
     <row r="120" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B120" s="15">
         <v>17</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D120" s="15" t="s">
         <v>32</v>
@@ -4032,13 +4032,13 @@
     </row>
     <row r="121" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B121" s="15">
         <v>17</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D121" s="15" t="s">
         <v>32</v>
@@ -4054,13 +4054,13 @@
     </row>
     <row r="122" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B122" s="15">
         <v>17</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D122" s="15" t="s">
         <v>32</v>
@@ -4076,13 +4076,13 @@
     </row>
     <row r="123" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B123" s="15">
         <v>17</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D123" s="15" t="s">
         <v>32</v>
@@ -4098,13 +4098,13 @@
     </row>
     <row r="124" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B124" s="15">
         <v>17</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D124" s="15" t="s">
         <v>32</v>
@@ -4120,13 +4120,13 @@
     </row>
     <row r="125" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B125" s="15">
         <v>17</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D125" s="15" t="s">
         <v>32</v>
@@ -4142,13 +4142,13 @@
     </row>
     <row r="126" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B126" s="15">
         <v>17</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D126" s="15" t="s">
         <v>32</v>
@@ -4164,13 +4164,13 @@
     </row>
     <row r="127" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B127" s="15">
         <v>17</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D127" s="15" t="s">
         <v>32</v>
@@ -4186,13 +4186,13 @@
     </row>
     <row r="128" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B128" s="15">
         <v>17</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D128" s="15" t="s">
         <v>44</v>
@@ -4208,13 +4208,13 @@
     </row>
     <row r="129" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B129" s="15">
         <v>17</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D129" s="15" t="s">
         <v>44</v>
@@ -4230,13 +4230,13 @@
     </row>
     <row r="130" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B130" s="15">
         <v>17</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D130" s="15" t="s">
         <v>44</v>
@@ -4252,13 +4252,13 @@
     </row>
     <row r="131" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B131" s="15">
         <v>17</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D131" s="15" t="s">
         <v>44</v>
@@ -4274,13 +4274,13 @@
     </row>
     <row r="132" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B132" s="15">
         <v>17</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D132" s="15" t="s">
         <v>44</v>
@@ -4296,13 +4296,13 @@
     </row>
     <row r="133" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B133" s="15">
         <v>17</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D133" s="15" t="s">
         <v>44</v>
@@ -4318,13 +4318,13 @@
     </row>
     <row r="134" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B134" s="15">
         <v>17</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D134" s="15" t="s">
         <v>44</v>
@@ -4340,13 +4340,13 @@
     </row>
     <row r="135" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B135" s="15">
         <v>17</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D135" s="15" t="s">
         <v>44</v>
@@ -4362,13 +4362,13 @@
     </row>
     <row r="136" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B136" s="15">
         <v>17</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D136" s="15" t="s">
         <v>44</v>
@@ -4384,13 +4384,13 @@
     </row>
     <row r="137" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B137" s="15">
         <v>17</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D137" s="15" t="s">
         <v>44</v>
@@ -4406,13 +4406,13 @@
     </row>
     <row r="138" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B138" s="15">
         <v>17</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D138" s="15" t="s">
         <v>44</v>
@@ -4428,13 +4428,13 @@
     </row>
     <row r="139" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B139" s="15">
         <v>17</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D139" s="15" t="s">
         <v>44</v>
@@ -4450,13 +4450,13 @@
     </row>
     <row r="140" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B140" s="15">
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D140" s="15" t="s">
         <v>45</v>
@@ -4472,13 +4472,13 @@
     </row>
     <row r="141" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B141" s="15">
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D141" s="15" t="s">
         <v>45</v>
@@ -4494,13 +4494,13 @@
     </row>
     <row r="142" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B142" s="15">
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D142" s="15" t="s">
         <v>45</v>
@@ -4516,13 +4516,13 @@
     </row>
     <row r="143" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B143" s="15">
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D143" s="15" t="s">
         <v>45</v>
@@ -4538,13 +4538,13 @@
     </row>
     <row r="144" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B144" s="15">
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D144" s="15" t="s">
         <v>45</v>
@@ -4560,13 +4560,13 @@
     </row>
     <row r="145" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B145" s="15">
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D145" s="15" t="s">
         <v>45</v>
@@ -4582,13 +4582,13 @@
     </row>
     <row r="146" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B146" s="15">
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D146" s="15" t="s">
         <v>45</v>
@@ -4604,13 +4604,13 @@
     </row>
     <row r="147" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B147" s="15">
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D147" s="15" t="s">
         <v>45</v>
@@ -4626,13 +4626,13 @@
     </row>
     <row r="148" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B148" s="15">
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D148" s="15" t="s">
         <v>45</v>
@@ -4648,13 +4648,13 @@
     </row>
     <row r="149" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B149" s="15">
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D149" s="15" t="s">
         <v>45</v>
@@ -4670,13 +4670,13 @@
     </row>
     <row r="150" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B150" s="15">
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D150" s="15" t="s">
         <v>45</v>
@@ -4692,13 +4692,13 @@
     </row>
     <row r="151" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B151" s="15">
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D151" s="15" t="s">
         <v>45</v>
@@ -4714,13 +4714,13 @@
     </row>
     <row r="152" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B152" s="15">
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D152" s="15" t="s">
         <v>46</v>
@@ -4736,13 +4736,13 @@
     </row>
     <row r="153" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B153" s="15">
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D153" s="15" t="s">
         <v>46</v>
@@ -4758,13 +4758,13 @@
     </row>
     <row r="154" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B154" s="15">
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D154" s="15" t="s">
         <v>46</v>
@@ -4780,13 +4780,13 @@
     </row>
     <row r="155" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B155" s="15">
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D155" s="15" t="s">
         <v>46</v>
@@ -4802,13 +4802,13 @@
     </row>
     <row r="156" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B156" s="15">
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D156" s="15" t="s">
         <v>46</v>
@@ -4824,13 +4824,13 @@
     </row>
     <row r="157" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B157" s="15">
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D157" s="15" t="s">
         <v>46</v>
@@ -4846,13 +4846,13 @@
     </row>
     <row r="158" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B158" s="15">
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D158" s="15" t="s">
         <v>46</v>
@@ -4868,13 +4868,13 @@
     </row>
     <row r="159" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B159" s="15">
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D159" s="15" t="s">
         <v>46</v>
@@ -4890,13 +4890,13 @@
     </row>
     <row r="160" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B160" s="15">
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D160" s="15" t="s">
         <v>46</v>
@@ -4912,13 +4912,13 @@
     </row>
     <row r="161" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B161" s="15">
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D161" s="15" t="s">
         <v>46</v>
@@ -4934,13 +4934,13 @@
     </row>
     <row r="162" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B162" s="15">
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D162" s="15" t="s">
         <v>46</v>
@@ -4956,13 +4956,13 @@
     </row>
     <row r="163" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B163" s="15">
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D163" s="15" t="s">
         <v>46</v>
@@ -4978,13 +4978,13 @@
     </row>
     <row r="164" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B164" s="15">
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D164" s="15" t="s">
         <v>47</v>
@@ -5000,13 +5000,13 @@
     </row>
     <row r="165" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B165" s="15">
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D165" s="15" t="s">
         <v>47</v>
@@ -5022,13 +5022,13 @@
     </row>
     <row r="166" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B166" s="15">
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D166" s="15" t="s">
         <v>47</v>
@@ -5044,13 +5044,13 @@
     </row>
     <row r="167" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B167" s="15">
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D167" s="15" t="s">
         <v>47</v>
@@ -5066,13 +5066,13 @@
     </row>
     <row r="168" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B168" s="15">
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D168" s="15" t="s">
         <v>47</v>
@@ -5088,13 +5088,13 @@
     </row>
     <row r="169" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B169" s="15">
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D169" s="15" t="s">
         <v>47</v>
@@ -5110,13 +5110,13 @@
     </row>
     <row r="170" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B170" s="15">
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D170" s="15" t="s">
         <v>47</v>
@@ -5132,13 +5132,13 @@
     </row>
     <row r="171" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B171" s="15">
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D171" s="15" t="s">
         <v>55</v>
@@ -5156,13 +5156,13 @@
     </row>
     <row r="172" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B172" s="15">
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D172" s="15" t="s">
         <v>55</v>
@@ -5180,13 +5180,13 @@
     </row>
     <row r="173" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B173" s="15">
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D173" s="15" t="s">
         <v>55</v>
@@ -5204,13 +5204,13 @@
     </row>
     <row r="174" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B174" s="15">
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D174" s="15" t="s">
         <v>55</v>
@@ -5228,13 +5228,13 @@
     </row>
     <row r="175" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B175" s="15">
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D175" s="15" t="s">
         <v>55</v>
@@ -5252,13 +5252,13 @@
     </row>
     <row r="176" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B176" s="15">
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D176" s="15" t="s">
         <v>55</v>
@@ -5276,13 +5276,13 @@
     </row>
     <row r="177" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B177" s="15">
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D177" s="15" t="s">
         <v>55</v>
@@ -5300,13 +5300,13 @@
     </row>
     <row r="178" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B178" s="15">
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D178" s="15" t="s">
         <v>55</v>
@@ -5324,13 +5324,13 @@
     </row>
     <row r="179" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B179" s="15">
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D179" s="15" t="s">
         <v>55</v>
@@ -5348,13 +5348,13 @@
     </row>
     <row r="180" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B180" s="15">
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D180" s="15" t="s">
         <v>55</v>
@@ -5372,13 +5372,13 @@
     </row>
     <row r="181" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B181" s="15">
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D181" s="15" t="s">
         <v>55</v>
@@ -5396,13 +5396,13 @@
     </row>
     <row r="182" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B182" s="15">
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D182" s="15" t="s">
         <v>55</v>
@@ -5420,13 +5420,13 @@
     </row>
     <row r="183" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B183" s="15">
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D183" s="15" t="s">
         <v>55</v>
@@ -5444,13 +5444,13 @@
     </row>
     <row r="184" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B184" s="15">
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D184" s="15" t="s">
         <v>55</v>
@@ -5468,13 +5468,13 @@
     </row>
     <row r="185" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B185" s="15">
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D185" s="15" t="s">
         <v>65</v>
@@ -5490,13 +5490,13 @@
     </row>
     <row r="186" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B186" s="15">
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D186" s="15" t="s">
         <v>65</v>
@@ -5512,13 +5512,13 @@
     </row>
     <row r="187" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B187" s="15">
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D187" s="15" t="s">
         <v>65</v>
@@ -5534,13 +5534,13 @@
     </row>
     <row r="188" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B188" s="15">
         <v>17</v>
       </c>
       <c r="C188" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D188" s="15" t="s">
         <v>32</v>
@@ -5558,13 +5558,13 @@
     </row>
     <row r="189" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B189" s="15">
         <v>17</v>
       </c>
       <c r="C189" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D189" s="15" t="s">
         <v>32</v>
@@ -5582,13 +5582,13 @@
     </row>
     <row r="190" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B190" s="15">
         <v>17</v>
       </c>
       <c r="C190" s="15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D190" s="15" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Uploaded 05-May-2021 12:12:07 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -816,6 +816,9 @@
     <t>RENAL CARE (DIALYSIS)</t>
   </si>
   <si>
+    <t>getBenefit_group().getName().equals("$param")</t>
+  </si>
+  <si>
     <t>getName().equals("$param")</t>
   </si>
   <si>
@@ -823,9 +826,6 @@
   </si>
   <si>
     <t>$benefit: Benefit</t>
-  </si>
-  <si>
-    <t>getBenefit_group().getName().equals("$param"),getBenefit_group().getCoveredDays()==$param</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
@@ -1489,7 +1489,7 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -1501,14 +1501,14 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="25" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Uploaded 05-May-2021 12:18:27 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="266">
   <si>
     <t>RuleSet</t>
   </si>
@@ -817,6 +817,9 @@
   </si>
   <si>
     <t>getBenefit_group().getName().equals("$param")</t>
+  </si>
+  <si>
+    <t>getBenefit_group().getCoveredDays()==$param</t>
   </si>
   <si>
     <t>getName().equals("$param")</t>
@@ -968,7 +971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1039,6 +1042,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1417,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1488,10 +1497,10 @@
     <row r="4" spans="1:11" ht="25.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="D4" s="7"/>
+      <c r="C4" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" s="26"/>
       <c r="E4" s="7"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -1500,15 +1509,17 @@
     <row r="5" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="28" t="s">
+        <v>262</v>
+      </c>
       <c r="E5" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>6</v>
@@ -13423,7 +13434,7 @@
   <mergeCells count="3">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploaded 05-May-2021 12:20:48 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -918,7 +918,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -956,6 +956,17 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -971,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1046,14 +1057,20 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1426,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1497,22 +1514,22 @@
     <row r="4" spans="1:11" ht="25.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="28" t="s">
         <v>265</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="8"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>262</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -13434,7 +13451,7 @@
   <mergeCells count="3">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploaded 05-May-2021 12:24:26 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -982,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1057,20 +1057,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1443,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1514,11 +1505,11 @@
     <row r="4" spans="1:11" ht="25.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="29"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="27"/>
       <c r="G4" s="8"/>
       <c r="K4" s="3"/>
@@ -1526,10 +1517,10 @@
     <row r="5" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="7" t="s">
         <v>262</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -13451,7 +13442,7 @@
   <mergeCells count="3">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C4:F4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploaded 05-May-2021 12:37:35 {/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
+++ b/src/main/resources/com/wakandaspace/drools_price_model/AssumptionUsedByGroupName.xlsx
@@ -39,9 +39,6 @@
     <t>ACTION</t>
   </si>
   <si>
-    <t>$benefit.setCalculationResult($param);</t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
@@ -829,6 +826,9 @@
   </si>
   <si>
     <t>$benefit: Benefit</t>
+  </si>
+  <si>
+    <t>$benefit.setCalculationResult($benefit.getCalculationResult*$param);</t>
   </si>
 </sst>
 </file>
@@ -1434,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1506,7 +1506,7 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -1514,23 +1514,23 @@
       <c r="G4" s="8"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>264</v>
-      </c>
       <c r="G5" s="10" t="s">
-        <v>6</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1541,35 +1541,35 @@
         <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="15">
         <v>17</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
       <c r="F7" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="20">
         <v>0.5</v>
@@ -1577,18 +1577,18 @@
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="15">
         <v>17</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="20">
         <v>0.6</v>
@@ -1596,18 +1596,18 @@
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="15">
         <v>17</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="20">
         <v>0.65</v>
@@ -1615,18 +1615,18 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="15">
         <v>17</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
       <c r="F10" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="20">
         <v>0.7</v>
@@ -1634,18 +1634,18 @@
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="15">
         <v>17</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="20">
         <v>0.72</v>
@@ -1653,18 +1653,18 @@
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="15">
         <v>17</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
       <c r="F12" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="20">
         <v>0.75</v>
@@ -1672,18 +1672,18 @@
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="15">
         <v>17</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" s="20">
         <v>0.86</v>
@@ -1691,18 +1691,18 @@
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" s="15">
         <v>17</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
       <c r="F14" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="20">
         <v>0.89</v>
@@ -1710,18 +1710,18 @@
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="15">
         <v>17</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="20">
         <v>0.89900000000000002</v>
@@ -1729,18 +1729,18 @@
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="15">
         <v>17</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" s="20">
         <v>0.9</v>
@@ -1748,18 +1748,18 @@
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="15">
         <v>17</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
       <c r="F17" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17" s="20">
         <v>0.91</v>
@@ -1767,18 +1767,18 @@
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="15">
         <v>17</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="20">
         <v>0.99099999999999999</v>
@@ -1786,18 +1786,18 @@
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="15">
         <v>17</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
       <c r="F19" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G19" s="20">
         <v>0.995</v>
@@ -1805,18 +1805,18 @@
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B20" s="15">
         <v>17</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20" s="20">
         <v>0.996</v>
@@ -1824,18 +1824,18 @@
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" s="15">
         <v>17</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
       <c r="F21" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G21" s="20">
         <v>0.997</v>
@@ -1843,18 +1843,18 @@
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="15">
         <v>17</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
       <c r="F22" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" s="20">
         <v>0.998</v>
@@ -1862,18 +1862,18 @@
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" s="15">
         <v>17</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G23" s="20">
         <v>0.999</v>
@@ -1881,18 +1881,18 @@
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24" s="15">
         <v>17</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G24" s="20">
         <v>1</v>
@@ -1900,18 +1900,18 @@
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="15">
         <v>17</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" s="20">
         <v>0.4</v>
@@ -1919,18 +1919,18 @@
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="15">
         <v>17</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
       <c r="F26" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G26" s="20">
         <v>0.5</v>
@@ -1938,18 +1938,18 @@
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="15">
         <v>17</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
       <c r="F27" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G27" s="20">
         <v>0.55000000000000004</v>
@@ -1957,18 +1957,18 @@
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B28" s="15">
         <v>17</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
       <c r="F28" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G28" s="20">
         <v>0.6</v>
@@ -1976,18 +1976,18 @@
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="15">
         <v>17</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G29" s="20">
         <v>0.62</v>
@@ -1995,18 +1995,18 @@
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B30" s="15">
         <v>17</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
       <c r="F30" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G30" s="20">
         <v>0.65</v>
@@ -2014,18 +2014,18 @@
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" s="15">
         <v>17</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="21"/>
       <c r="F31" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G31" s="20">
         <v>0.7</v>
@@ -2033,18 +2033,18 @@
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="15">
         <v>17</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
       <c r="F32" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G32" s="20">
         <v>0.88</v>
@@ -2052,18 +2052,18 @@
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" s="15">
         <v>17</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
       <c r="F33" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G33" s="20">
         <v>0.9</v>
@@ -2071,18 +2071,18 @@
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" s="15">
         <v>17</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
       <c r="F34" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G34" s="20">
         <v>0.995</v>
@@ -2090,18 +2090,18 @@
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B35" s="15">
         <v>17</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="21"/>
       <c r="F35" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G35" s="20">
         <v>0.99550000000000005</v>
@@ -2109,18 +2109,18 @@
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" s="15">
         <v>17</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="21"/>
       <c r="F36" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G36" s="20">
         <v>0.996</v>
@@ -2128,18 +2128,18 @@
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="15">
         <v>17</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
       <c r="F37" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G37" s="20">
         <v>0.99650000000000005</v>
@@ -2147,18 +2147,18 @@
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B38" s="15">
         <v>17</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="21"/>
       <c r="F38" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G38" s="20">
         <v>0.997</v>
@@ -2166,18 +2166,18 @@
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="15">
         <v>17</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="21"/>
       <c r="F39" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G39" s="20">
         <v>0.99750000000000005</v>
@@ -2185,18 +2185,18 @@
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B40" s="15">
         <v>17</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
       <c r="F40" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G40" s="20">
         <v>0.998</v>
@@ -2204,18 +2204,18 @@
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B41" s="15">
         <v>17</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="21"/>
       <c r="F41" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G41" s="20">
         <v>0.999</v>
@@ -2223,18 +2223,18 @@
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B42" s="15">
         <v>17</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="21"/>
       <c r="F42" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G42" s="20">
         <v>1</v>
@@ -2242,18 +2242,18 @@
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B43" s="15">
         <v>17</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="21"/>
       <c r="F43" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G43" s="20">
         <v>0.1</v>
@@ -2261,18 +2261,18 @@
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B44" s="15">
         <v>17</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="21"/>
       <c r="F44" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G44" s="20">
         <v>0.25</v>
@@ -2280,18 +2280,18 @@
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45" s="15">
         <v>17</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D45" s="21"/>
       <c r="E45" s="21"/>
       <c r="F45" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G45" s="20">
         <v>0.3</v>
@@ -2299,18 +2299,18 @@
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" s="15">
         <v>17</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D46" s="21"/>
       <c r="E46" s="21"/>
       <c r="F46" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G46" s="20">
         <v>0.4</v>
@@ -2318,18 +2318,18 @@
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B47" s="15">
         <v>17</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D47" s="21"/>
       <c r="E47" s="21"/>
       <c r="F47" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G47" s="20">
         <v>0.45</v>
@@ -2337,18 +2337,18 @@
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B48" s="15">
         <v>17</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="21"/>
       <c r="F48" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G48" s="20">
         <v>0.5</v>
@@ -2356,18 +2356,18 @@
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B49" s="15">
         <v>17</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D49" s="21"/>
       <c r="E49" s="21"/>
       <c r="F49" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G49" s="20">
         <v>0.61</v>
@@ -2375,18 +2375,18 @@
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B50" s="15">
         <v>17</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21"/>
       <c r="F50" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G50" s="20">
         <v>0.65</v>
@@ -2394,18 +2394,18 @@
     </row>
     <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B51" s="15">
         <v>17</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D51" s="21"/>
       <c r="E51" s="21"/>
       <c r="F51" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G51" s="20">
         <v>0.7</v>
@@ -2413,18 +2413,18 @@
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B52" s="15">
         <v>17</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D52" s="21"/>
       <c r="E52" s="21"/>
       <c r="F52" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G52" s="20">
         <v>0.8</v>
@@ -2432,18 +2432,18 @@
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B53" s="15">
         <v>17</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="21"/>
       <c r="F53" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G53" s="20">
         <v>0.87</v>
@@ -2451,18 +2451,18 @@
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B54" s="15">
         <v>17</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="21"/>
       <c r="F54" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G54" s="20">
         <v>0.88</v>
@@ -2470,18 +2470,18 @@
     </row>
     <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B55" s="15">
         <v>17</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="21"/>
       <c r="F55" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G55" s="20">
         <v>0.9</v>
@@ -2489,18 +2489,18 @@
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B56" s="15">
         <v>17</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="21"/>
       <c r="F56" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G56" s="20">
         <v>0.996</v>
@@ -2508,18 +2508,18 @@
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" s="15">
         <v>17</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="21"/>
       <c r="F57" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G57" s="20">
         <v>0.997</v>
@@ -2527,18 +2527,18 @@
     </row>
     <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B58" s="15">
         <v>17</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="21"/>
       <c r="F58" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G58" s="20">
         <v>0.998</v>
@@ -2546,18 +2546,18 @@
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B59" s="15">
         <v>17</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="21"/>
       <c r="F59" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G59" s="20">
         <v>0.999</v>
@@ -2565,18 +2565,18 @@
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B60" s="15">
         <v>17</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="21"/>
       <c r="F60" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G60" s="20">
         <v>1</v>
@@ -2584,18 +2584,18 @@
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B61" s="15">
         <v>17</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G61" s="20">
         <v>0.48</v>
@@ -2603,18 +2603,18 @@
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B62" s="15">
         <v>17</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="21"/>
       <c r="F62" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G62" s="20">
         <v>0.55000000000000004</v>
@@ -2622,18 +2622,18 @@
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B63" s="15">
         <v>17</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D63" s="21"/>
       <c r="E63" s="21"/>
       <c r="F63" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G63" s="20">
         <v>0.65</v>
@@ -2641,18 +2641,18 @@
     </row>
     <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B64" s="15">
         <v>17</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="21"/>
       <c r="F64" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G64" s="20">
         <v>0.77</v>
@@ -2660,18 +2660,18 @@
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B65" s="15">
         <v>17</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D65" s="21"/>
       <c r="E65" s="21"/>
       <c r="F65" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G65" s="20">
         <v>0.79</v>
@@ -2679,18 +2679,18 @@
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B66" s="15">
         <v>17</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="21"/>
       <c r="F66" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G66" s="20">
         <v>0.8</v>
@@ -2698,18 +2698,18 @@
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B67" s="15">
         <v>17</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="21"/>
       <c r="F67" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G67" s="20">
         <v>0.88</v>
@@ -2717,18 +2717,18 @@
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B68" s="15">
         <v>17</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D68" s="21"/>
       <c r="E68" s="21"/>
       <c r="F68" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G68" s="20">
         <v>0.99</v>
@@ -2736,18 +2736,18 @@
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B69" s="15">
         <v>17</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D69" s="21"/>
       <c r="E69" s="21"/>
       <c r="F69" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G69" s="20">
         <v>0.99099999999999999</v>
@@ -2755,18 +2755,18 @@
     </row>
     <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B70" s="15">
         <v>17</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="21"/>
       <c r="F70" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G70" s="20">
         <v>0.99199999999999999</v>
@@ -2774,18 +2774,18 @@
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B71" s="15">
         <v>17</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D71" s="21"/>
       <c r="E71" s="21"/>
       <c r="F71" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G71" s="20">
         <v>0.99299999999999999</v>
@@ -2793,18 +2793,18 @@
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B72" s="15">
         <v>17</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="21"/>
       <c r="F72" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G72" s="20">
         <v>0.99399999999999999</v>
@@ -2812,18 +2812,18 @@
     </row>
     <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B73" s="15">
         <v>17</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D73" s="21"/>
       <c r="E73" s="21"/>
       <c r="F73" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G73" s="20">
         <v>0.995</v>
@@ -2831,18 +2831,18 @@
     </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B74" s="15">
         <v>17</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D74" s="21"/>
       <c r="E74" s="21"/>
       <c r="F74" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G74" s="20">
         <v>0.996</v>
@@ -2850,18 +2850,18 @@
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B75" s="15">
         <v>17</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D75" s="21"/>
       <c r="E75" s="21"/>
       <c r="F75" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G75" s="20">
         <v>0.997</v>
@@ -2869,18 +2869,18 @@
     </row>
     <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B76" s="15">
         <v>17</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D76" s="21"/>
       <c r="E76" s="21"/>
       <c r="F76" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G76" s="20">
         <v>0.998</v>
@@ -2888,18 +2888,18 @@
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B77" s="15">
         <v>17</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="21"/>
       <c r="F77" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G77" s="20">
         <v>0.999</v>
@@ -2907,18 +2907,18 @@
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B78" s="15">
         <v>17</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="21"/>
       <c r="F78" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G78" s="20">
         <v>1</v>
@@ -2926,18 +2926,18 @@
     </row>
     <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B79" s="15">
         <v>17</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D79" s="21"/>
       <c r="E79" s="21"/>
       <c r="F79" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G79" s="20">
         <v>0.79</v>
@@ -2945,18 +2945,18 @@
     </row>
     <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B80" s="15">
         <v>17</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D80" s="21"/>
       <c r="E80" s="21"/>
       <c r="F80" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G80" s="20">
         <v>0.82</v>
@@ -2964,18 +2964,18 @@
     </row>
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B81" s="15">
         <v>17</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="21"/>
       <c r="F81" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G81" s="20">
         <v>0.85</v>
@@ -2983,18 +2983,18 @@
     </row>
     <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B82" s="15">
         <v>17</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
       <c r="F82" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G82" s="20">
         <v>0.9</v>
@@ -3002,18 +3002,18 @@
     </row>
     <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B83" s="15">
         <v>17</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
       <c r="F83" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G83" s="20">
         <v>0.98499999999999999</v>
@@ -3021,18 +3021,18 @@
     </row>
     <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B84" s="15">
         <v>17</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21"/>
       <c r="F84" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G84" s="20">
         <v>0.98799999999999999</v>
@@ -3040,18 +3040,18 @@
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B85" s="15">
         <v>17</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
       <c r="F85" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G85" s="20">
         <v>0.98899999999999999</v>
@@ -3059,18 +3059,18 @@
     </row>
     <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B86" s="15">
         <v>17</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21"/>
       <c r="F86" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G86" s="20">
         <v>0.99</v>
@@ -3078,18 +3078,18 @@
     </row>
     <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B87" s="15">
         <v>17</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="21"/>
       <c r="F87" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G87" s="20">
         <v>0.99099999999999999</v>
@@ -3097,18 +3097,18 @@
     </row>
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B88" s="15">
         <v>17</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
       <c r="F88" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G88" s="20">
         <v>0.99199999999999999</v>
@@ -3116,18 +3116,18 @@
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B89" s="15">
         <v>17</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D89" s="21"/>
       <c r="E89" s="21"/>
       <c r="F89" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G89" s="20">
         <v>0.99299999999999999</v>
@@ -3135,18 +3135,18 @@
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B90" s="15">
         <v>17</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D90" s="21"/>
       <c r="E90" s="21"/>
       <c r="F90" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G90" s="20">
         <v>0.99399999999999999</v>
@@ -3154,18 +3154,18 @@
     </row>
     <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B91" s="15">
         <v>17</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
       <c r="F91" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G91" s="20">
         <v>0.995</v>
@@ -3173,18 +3173,18 @@
     </row>
     <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B92" s="15">
         <v>17</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
       <c r="F92" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G92" s="20">
         <v>0.996</v>
@@ -3192,18 +3192,18 @@
     </row>
     <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B93" s="15">
         <v>17</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
       <c r="F93" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G93" s="20">
         <v>0.997</v>
@@ -3211,18 +3211,18 @@
     </row>
     <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B94" s="15">
         <v>17</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
       <c r="F94" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G94" s="20">
         <v>0.998</v>
@@ -3230,18 +3230,18 @@
     </row>
     <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B95" s="15">
         <v>17</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D95" s="21"/>
       <c r="E95" s="21"/>
       <c r="F95" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G95" s="20">
         <v>0.999</v>
@@ -3249,18 +3249,18 @@
     </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B96" s="15">
         <v>17</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
       <c r="F96" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G96" s="20">
         <v>1</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B97" s="15">
         <v>17</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D97" s="19">
         <v>1</v>
@@ -3287,13 +3287,13 @@
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B98" s="15">
         <v>17</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D98" s="19">
         <v>2</v>
@@ -3306,13 +3306,13 @@
     </row>
     <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B99" s="15">
         <v>17</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D99" s="19">
         <v>3</v>
@@ -3325,13 +3325,13 @@
     </row>
     <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B100" s="15">
         <v>17</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D100" s="19">
         <v>4</v>
@@ -3344,13 +3344,13 @@
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B101" s="15">
         <v>17</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D101" s="19">
         <v>5</v>
@@ -3363,13 +3363,13 @@
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B102" s="15">
         <v>17</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D102" s="19">
         <v>6</v>
@@ -3382,13 +3382,13 @@
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B103" s="15">
         <v>17</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D103" s="19">
         <v>7</v>
@@ -3401,13 +3401,13 @@
     </row>
     <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B104" s="15">
         <v>17</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D104" s="19">
         <v>8</v>
@@ -3420,13 +3420,13 @@
     </row>
     <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B105" s="15">
         <v>17</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D105" s="19">
         <v>9</v>
@@ -3439,13 +3439,13 @@
     </row>
     <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B106" s="15">
         <v>17</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D106" s="19">
         <v>10</v>
@@ -3458,13 +3458,13 @@
     </row>
     <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B107" s="15">
         <v>17</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D107" s="19">
         <v>15</v>
@@ -3477,13 +3477,13 @@
     </row>
     <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B108" s="15">
         <v>17</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D108" s="19">
         <v>20</v>
@@ -3496,13 +3496,13 @@
     </row>
     <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B109" s="15">
         <v>17</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D109" s="19">
         <v>25</v>
@@ -3515,13 +3515,13 @@
     </row>
     <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B110" s="15">
         <v>17</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D110" s="19">
         <v>30</v>
@@ -3534,13 +3534,13 @@
     </row>
     <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B111" s="15">
         <v>17</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D111" s="19">
         <v>45</v>
@@ -3553,13 +3553,13 @@
     </row>
     <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B112" s="15">
         <v>17</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D112" s="19">
         <v>50</v>
@@ -3572,13 +3572,13 @@
     </row>
     <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B113" s="15">
         <v>17</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D113" s="19">
         <v>60</v>
@@ -3591,13 +3591,13 @@
     </row>
     <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B114" s="15">
         <v>17</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D114" s="19">
         <v>100</v>
@@ -3610,13 +3610,13 @@
     </row>
     <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B115" s="15">
         <v>17</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D115" s="19">
         <v>-1</v>
@@ -3629,18 +3629,18 @@
     </row>
     <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B116" s="15">
         <v>17</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D116" s="15"/>
       <c r="E116" s="21"/>
       <c r="F116" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G116" s="20">
         <v>0.5</v>
@@ -3648,18 +3648,18 @@
     </row>
     <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B117" s="15">
         <v>17</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D117" s="15"/>
       <c r="E117" s="21"/>
       <c r="F117" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G117" s="20">
         <v>1</v>
@@ -3667,18 +3667,18 @@
     </row>
     <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B118" s="15">
         <v>17</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D118" s="15"/>
       <c r="E118" s="21"/>
       <c r="F118" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G118" s="20">
         <v>1.3</v>
@@ -3686,18 +3686,18 @@
     </row>
     <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B119" s="15">
         <v>17</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D119" s="15"/>
       <c r="E119" s="21"/>
       <c r="F119" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G119" s="20">
         <v>2</v>
@@ -3705,18 +3705,18 @@
     </row>
     <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B120" s="15">
         <v>17</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D120" s="15"/>
       <c r="E120" s="21"/>
       <c r="F120" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G120" s="20">
         <v>2.1</v>
@@ -3724,18 +3724,18 @@
     </row>
     <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B121" s="15">
         <v>17</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D121" s="15"/>
       <c r="E121" s="21"/>
       <c r="F121" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G121" s="20">
         <v>3</v>
@@ -3743,18 +3743,18 @@
     </row>
     <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B122" s="15">
         <v>17</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D122" s="15"/>
       <c r="E122" s="21"/>
       <c r="F122" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G122" s="20">
         <v>3</v>
@@ -3762,18 +3762,18 @@
     </row>
     <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B123" s="15">
         <v>17</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D123" s="15"/>
       <c r="E123" s="21"/>
       <c r="F123" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G123" s="20">
         <v>4</v>
@@ -3781,18 +3781,18 @@
     </row>
     <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B124" s="15">
         <v>17</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D124" s="15"/>
       <c r="E124" s="21"/>
       <c r="F124" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G124" s="20">
         <v>6</v>
@@ -3800,18 +3800,18 @@
     </row>
     <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B125" s="15">
         <v>17</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D125" s="15"/>
       <c r="E125" s="21"/>
       <c r="F125" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G125" s="20">
         <v>10</v>
@@ -3819,18 +3819,18 @@
     </row>
     <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B126" s="15">
         <v>17</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D126" s="15"/>
       <c r="E126" s="21"/>
       <c r="F126" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G126" s="20">
         <v>15</v>
@@ -3838,18 +3838,18 @@
     </row>
     <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B127" s="15">
         <v>17</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D127" s="15"/>
       <c r="E127" s="21"/>
       <c r="F127" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G127" s="20">
         <v>21</v>
@@ -3857,18 +3857,18 @@
     </row>
     <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B128" s="15">
         <v>17</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D128" s="15"/>
       <c r="E128" s="21"/>
       <c r="F128" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G128" s="20">
         <v>0.1</v>
@@ -3876,18 +3876,18 @@
     </row>
     <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B129" s="15">
         <v>17</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D129" s="15"/>
       <c r="E129" s="21"/>
       <c r="F129" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G129" s="20">
         <v>0.32</v>
@@ -3895,18 +3895,18 @@
     </row>
     <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B130" s="15">
         <v>17</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D130" s="15"/>
       <c r="E130" s="21"/>
       <c r="F130" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G130" s="20">
         <v>0.4</v>
@@ -3914,18 +3914,18 @@
     </row>
     <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B131" s="15">
         <v>17</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D131" s="15"/>
       <c r="E131" s="21"/>
       <c r="F131" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G131" s="20">
         <v>0.45</v>
@@ -3933,18 +3933,18 @@
     </row>
     <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B132" s="15">
         <v>17</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D132" s="15"/>
       <c r="E132" s="21"/>
       <c r="F132" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G132" s="20">
         <v>0.48</v>
@@ -3952,18 +3952,18 @@
     </row>
     <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B133" s="15">
         <v>17</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D133" s="15"/>
       <c r="E133" s="21"/>
       <c r="F133" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G133" s="20">
         <v>0.5</v>
@@ -3971,18 +3971,18 @@
     </row>
     <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B134" s="15">
         <v>17</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D134" s="15"/>
       <c r="E134" s="21"/>
       <c r="F134" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G134" s="20">
         <v>0.55000000000000004</v>
@@ -3990,18 +3990,18 @@
     </row>
     <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B135" s="15">
         <v>17</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D135" s="15"/>
       <c r="E135" s="21"/>
       <c r="F135" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G135" s="20">
         <v>0.6</v>
@@ -4009,18 +4009,18 @@
     </row>
     <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B136" s="15">
         <v>17</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="21"/>
       <c r="F136" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G136" s="20">
         <v>0.75</v>
@@ -4028,18 +4028,18 @@
     </row>
     <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B137" s="15">
         <v>17</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D137" s="15"/>
       <c r="E137" s="21"/>
       <c r="F137" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G137" s="20">
         <v>0.8</v>
@@ -4047,18 +4047,18 @@
     </row>
     <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B138" s="15">
         <v>17</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D138" s="15"/>
       <c r="E138" s="21"/>
       <c r="F138" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G138" s="20">
         <v>0.99</v>
@@ -4066,18 +4066,18 @@
     </row>
     <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B139" s="15">
         <v>17</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D139" s="15"/>
       <c r="E139" s="21"/>
       <c r="F139" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G139" s="20">
         <v>1</v>
@@ -4085,18 +4085,18 @@
     </row>
     <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B140" s="15">
         <v>17</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="21"/>
       <c r="F140" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G140" s="20">
         <v>0.5</v>
@@ -4104,18 +4104,18 @@
     </row>
     <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B141" s="15">
         <v>17</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="21"/>
       <c r="F141" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G141" s="20">
         <v>1</v>
@@ -4123,18 +4123,18 @@
     </row>
     <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B142" s="15">
         <v>17</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D142" s="15"/>
       <c r="E142" s="21"/>
       <c r="F142" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G142" s="20">
         <v>1.3</v>
@@ -4142,18 +4142,18 @@
     </row>
     <row r="143" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B143" s="15">
         <v>17</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D143" s="15"/>
       <c r="E143" s="21"/>
       <c r="F143" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G143" s="20">
         <v>2</v>
@@ -4161,18 +4161,18 @@
     </row>
     <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B144" s="15">
         <v>17</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="21"/>
       <c r="F144" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G144" s="20">
         <v>2.1</v>
@@ -4180,18 +4180,18 @@
     </row>
     <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B145" s="15">
         <v>17</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D145" s="15"/>
       <c r="E145" s="21"/>
       <c r="F145" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G145" s="20">
         <v>3</v>
@@ -4199,18 +4199,18 @@
     </row>
     <row r="146" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B146" s="15">
         <v>17</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="21"/>
       <c r="F146" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G146" s="20">
         <v>3</v>
@@ -4218,18 +4218,18 @@
     </row>
     <row r="147" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B147" s="15">
         <v>17</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D147" s="15"/>
       <c r="E147" s="21"/>
       <c r="F147" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G147" s="20">
         <v>4</v>
@@ -4237,18 +4237,18 @@
     </row>
     <row r="148" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B148" s="15">
         <v>17</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D148" s="15"/>
       <c r="E148" s="21"/>
       <c r="F148" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G148" s="20">
         <v>6</v>
@@ -4256,18 +4256,18 @@
     </row>
     <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B149" s="15">
         <v>17</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="21"/>
       <c r="F149" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G149" s="20">
         <v>10</v>
@@ -4275,18 +4275,18 @@
     </row>
     <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B150" s="15">
         <v>17</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D150" s="15"/>
       <c r="E150" s="21"/>
       <c r="F150" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G150" s="20">
         <v>15</v>
@@ -4294,18 +4294,18 @@
     </row>
     <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B151" s="15">
         <v>17</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D151" s="15"/>
       <c r="E151" s="21"/>
       <c r="F151" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G151" s="20">
         <v>21</v>
@@ -4313,18 +4313,18 @@
     </row>
     <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B152" s="15">
         <v>17</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="21"/>
       <c r="F152" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G152" s="20">
         <v>0.4</v>
@@ -4332,18 +4332,18 @@
     </row>
     <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B153" s="15">
         <v>17</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="21"/>
       <c r="F153" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G153" s="20">
         <v>0.8</v>
@@ -4351,18 +4351,18 @@
     </row>
     <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B154" s="15">
         <v>17</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="21"/>
       <c r="F154" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G154" s="20">
         <v>0.82</v>
@@ -4370,18 +4370,18 @@
     </row>
     <row r="155" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B155" s="15">
         <v>17</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="21"/>
       <c r="F155" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G155" s="20">
         <v>0.85</v>
@@ -4389,18 +4389,18 @@
     </row>
     <row r="156" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B156" s="15">
         <v>17</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="21"/>
       <c r="F156" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G156" s="20">
         <v>0.87</v>
@@ -4408,18 +4408,18 @@
     </row>
     <row r="157" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B157" s="15">
         <v>17</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="21"/>
       <c r="F157" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G157" s="20">
         <v>0.88</v>
@@ -4427,18 +4427,18 @@
     </row>
     <row r="158" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B158" s="15">
         <v>17</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="21"/>
       <c r="F158" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G158" s="20">
         <v>0.9</v>
@@ -4446,18 +4446,18 @@
     </row>
     <row r="159" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B159" s="15">
         <v>17</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="21"/>
       <c r="F159" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G159" s="20">
         <v>0.91</v>
@@ -4465,18 +4465,18 @@
     </row>
     <row r="160" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B160" s="15">
         <v>17</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="21"/>
       <c r="F160" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G160" s="20">
         <v>0.93</v>
@@ -4484,18 +4484,18 @@
     </row>
     <row r="161" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B161" s="15">
         <v>17</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="21"/>
       <c r="F161" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G161" s="20">
         <v>0.95</v>
@@ -4503,18 +4503,18 @@
     </row>
     <row r="162" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B162" s="15">
         <v>17</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="21"/>
       <c r="F162" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G162" s="20">
         <v>0.99</v>
@@ -4522,18 +4522,18 @@
     </row>
     <row r="163" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B163" s="15">
         <v>17</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="21"/>
       <c r="F163" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G163" s="20">
         <v>1</v>
@@ -4541,18 +4541,18 @@
     </row>
     <row r="164" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B164" s="15">
         <v>17</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D164" s="19"/>
       <c r="E164" s="19"/>
       <c r="F164" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G164" s="20">
         <v>0.4</v>
@@ -4560,18 +4560,18 @@
     </row>
     <row r="165" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B165" s="15">
         <v>17</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D165" s="19"/>
       <c r="E165" s="19"/>
       <c r="F165" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G165" s="20">
         <v>0.55000000000000004</v>
@@ -4579,18 +4579,18 @@
     </row>
     <row r="166" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B166" s="15">
         <v>17</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D166" s="19"/>
       <c r="E166" s="19"/>
       <c r="F166" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G166" s="20">
         <v>0.63</v>
@@ -4598,18 +4598,18 @@
     </row>
     <row r="167" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B167" s="15">
         <v>17</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D167" s="19"/>
       <c r="E167" s="19"/>
       <c r="F167" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G167" s="20">
         <v>0.74</v>
@@ -4617,18 +4617,18 @@
     </row>
     <row r="168" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B168" s="15">
         <v>17</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D168" s="19"/>
       <c r="E168" s="19"/>
       <c r="F168" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G168" s="20">
         <v>0.85</v>
@@ -4636,18 +4636,18 @@
     </row>
     <row r="169" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B169" s="15">
         <v>17</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D169" s="19"/>
       <c r="E169" s="19"/>
       <c r="F169" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G169" s="20">
         <v>0.98</v>
@@ -4655,18 +4655,18 @@
     </row>
     <row r="170" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B170" s="15">
         <v>17</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D170" s="19"/>
       <c r="E170" s="19"/>
       <c r="F170" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G170" s="20">
         <v>1</v>
@@ -4674,20 +4674,20 @@
     </row>
     <row r="171" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B171" s="15">
         <v>17</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D171" s="15"/>
       <c r="E171" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F171" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G171" s="20">
         <v>1</v>
@@ -4695,20 +4695,20 @@
     </row>
     <row r="172" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B172" s="15">
         <v>17</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D172" s="15"/>
       <c r="E172" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F172" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G172" s="20">
         <v>2</v>
@@ -4716,20 +4716,20 @@
     </row>
     <row r="173" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B173" s="15">
         <v>17</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D173" s="15"/>
       <c r="E173" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F173" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G173" s="20">
         <v>3</v>
@@ -4737,20 +4737,20 @@
     </row>
     <row r="174" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B174" s="15">
         <v>17</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D174" s="15"/>
       <c r="E174" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F174" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G174" s="20">
         <v>4</v>
@@ -4758,20 +4758,20 @@
     </row>
     <row r="175" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B175" s="15">
         <v>17</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D175" s="15"/>
       <c r="E175" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F175" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G175" s="20">
         <v>5</v>
@@ -4779,20 +4779,20 @@
     </row>
     <row r="176" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B176" s="15">
         <v>17</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D176" s="15"/>
       <c r="E176" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F176" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G176" s="20">
         <v>6</v>
@@ -4800,20 +4800,20 @@
     </row>
     <row r="177" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B177" s="15">
         <v>17</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F177" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G177" s="20">
         <v>7</v>
@@ -4821,20 +4821,20 @@
     </row>
     <row r="178" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B178" s="15">
         <v>17</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F178" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G178" s="20">
         <v>0.4</v>
@@ -4842,20 +4842,20 @@
     </row>
     <row r="179" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B179" s="15">
         <v>17</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F179" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G179" s="20">
         <v>0.55000000000000004</v>
@@ -4863,20 +4863,20 @@
     </row>
     <row r="180" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B180" s="15">
         <v>17</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F180" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G180" s="20">
         <v>0.63</v>
@@ -4884,20 +4884,20 @@
     </row>
     <row r="181" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B181" s="15">
         <v>17</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F181" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G181" s="20">
         <v>0.74</v>
@@ -4905,20 +4905,20 @@
     </row>
     <row r="182" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B182" s="15">
         <v>17</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F182" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G182" s="20">
         <v>0.85</v>
@@ -4926,20 +4926,20 @@
     </row>
     <row r="183" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B183" s="15">
         <v>17</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F183" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G183" s="20">
         <v>0.98</v>
@@ -4947,20 +4947,20 @@
     </row>
     <row r="184" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B184" s="15">
         <v>17</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D184" s="15"/>
       <c r="E184" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F184" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G184" s="20">
         <v>1</v>
@@ -4968,18 +4968,18 @@
     </row>
     <row r="185" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B185" s="15">
         <v>17</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D185" s="22"/>
       <c r="E185" s="15"/>
       <c r="F185" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G185" s="23">
         <v>1</v>
@@ -4987,18 +4987,18 @@
     </row>
     <row r="186" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B186" s="15">
         <v>17</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D186" s="22"/>
       <c r="E186" s="15"/>
       <c r="F186" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G186" s="23">
         <v>2</v>
@@ -5006,18 +5006,18 @@
     </row>
     <row r="187" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B187" s="15">
         <v>17</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D187" s="22"/>
       <c r="E187" s="15"/>
       <c r="F187" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G187" s="23">
         <v>2.5</v>
@@ -5025,20 +5025,20 @@
     </row>
     <row r="188" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B188" s="15">
         <v>17</v>
       </c>
       <c r="C188" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D188" s="15"/>
       <c r="E188" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F188" s="22" t="s">
         <v>69</v>
-      </c>
-      <c r="F188" s="22" t="s">
-        <v>70</v>
       </c>
       <c r="G188" s="23">
         <v>1</v>
@@ -5046,20 +5046,20 @@
     </row>
     <row r="189" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B189" s="15">
         <v>17</v>
       </c>
       <c r="C189" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D189" s="15"/>
       <c r="E189" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F189" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G189" s="23">
         <v>1.5</v>
@@ -5067,20 +5067,20 @@
     </row>
     <row r="190" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B190" s="15">
         <v>17</v>
       </c>
       <c r="C190" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D190" s="15"/>
       <c r="E190" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F190" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G190" s="23">
         <v>2</v>

</xml_diff>